<commit_message>
Generación de formato ewo descargable al 95%
</commit_message>
<xml_diff>
--- a/DigiTools/Content/formats/FORMATO_EWO.XLSX
+++ b/DigiTools/Content/formats/FORMATO_EWO.XLSX
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unilever\Web\Mtto\DigiTools\DigiTools\Content\formats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UNILEVER_MTTO\Dropbox\HPC\MttoApp\DigiTools\DigiTools\Content\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2434BF55-7944-4F6F-8B37-C24B16126A0D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5910945-BA99-49A9-8870-41D5A0F937D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25155" yWindow="1260" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWO" sheetId="7" r:id="rId1"/>
@@ -81,51 +81,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
   <si>
-    <t>EWO (Emergency Work Order)</t>
+    <t>NOK</t>
   </si>
   <si>
-    <t>EWO #</t>
+    <t>OK</t>
   </si>
   <si>
-    <t>Area/Linea</t>
+    <t>No PM</t>
   </si>
   <si>
-    <t>Equipo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha </t>
-  </si>
-  <si>
-    <t>Aviso #</t>
-  </si>
-  <si>
-    <t>Diligenciada por</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo de Avería                                                                                                                                                                                                                                        </t>
-  </si>
-  <si>
-    <t>Turno</t>
-  </si>
-  <si>
-    <t>MesPack</t>
-  </si>
-  <si>
-    <t>Mespack H-360 FED 363.008</t>
-  </si>
-  <si>
-    <t>20/03/2019</t>
-  </si>
-  <si>
-    <t>1231</t>
-  </si>
-  <si>
-    <t>Jeison Perlaza</t>
-  </si>
-  <si>
-    <t>Mecánica</t>
+    <t>No AM</t>
   </si>
   <si>
     <t>Notificación Avería (Hora)</t>
@@ -166,15 +133,6 @@
     <t>Descripción gráfica de la falla [dibujos y/o planos]</t>
   </si>
   <si>
-    <t>Descripción de la avería. Si la reparación no se ha terminado en su totalidad, indique que necesita que se realice para terminarla:</t>
-  </si>
-  <si>
-    <t>una avería</t>
-  </si>
-  <si>
-    <t>( X  ) Cambio de Componente                    (    ) Ajuste</t>
-  </si>
-  <si>
     <t>Repuestos Utilizados</t>
   </si>
   <si>
@@ -190,115 +148,107 @@
     <t>Costo [COP]</t>
   </si>
   <si>
-    <t>uno mas</t>
+    <t>1 - Por qué?</t>
   </si>
   <si>
-    <t>$12333</t>
+    <t>2 - Por qué?</t>
   </si>
   <si>
-    <t>prueba 2 de mttr</t>
+    <t>3 - Por qué?</t>
+  </si>
+  <si>
+    <t>4 - Por qué?</t>
+  </si>
+  <si>
+    <t>5 - Por qué?</t>
+  </si>
+  <si>
+    <t>Dibujo / Diagrama / Foto del 5 Por qué</t>
+  </si>
+  <si>
+    <t>Ciclo de la causa raíz</t>
+  </si>
+  <si>
+    <t>¿Qué tipo de falla es? Diligencie las fechas de los mantenimiento planeados y selecciones la causa raiz basada en el gráfico de la bañera</t>
+  </si>
+  <si>
+    <t>Error Humano (instalación)</t>
+  </si>
+  <si>
+    <t>Falla de Diseño</t>
+  </si>
+  <si>
+    <t>Error Humano 
+(en operación)</t>
+  </si>
+  <si>
+    <t>Condiciones Básicas</t>
+  </si>
+  <si>
+    <t>Condiciones de Operación</t>
+  </si>
+  <si>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Lista de Acciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Descripción de la avería. Si la reparación no se ha terminado en su totalidad, indique que necesita que se realice para terminarla:</t>
+  </si>
+  <si>
+    <t>(  ) Cambio de Componente                    (  ) Ajuste</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>8.</t>
+  </si>
+  <si>
+    <t>9.</t>
+  </si>
+  <si>
+    <t>10.</t>
+  </si>
+  <si>
+    <t>11.</t>
+  </si>
+  <si>
+    <t>12.</t>
+  </si>
+  <si>
+    <t>13.</t>
   </si>
   <si>
     <t>IDENTIFICACIÓN DE CAUSAS RAICES</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">IDENTIFICACION DE CAUSAS RAICES - 5G </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(llene esta seccion teniendo en cuenta el principio de los 5G)</t>
-    </r>
-  </si>
-  <si>
-    <t>NOK</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">GEMBA </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Ir al lugar donde se produce el problema)</t>
-    </r>
-  </si>
-  <si>
-    <t>df</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">GEMBUTSU </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Ver los objetos, piezas y materiales reales que participan en el problema)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">GENJITSU </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Confirmar una descripcion precisa y cuantificada del problema)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">GENRI </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Se refiere a la teoria. Principios mecanicos y fisicos que rigen la operación)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">GENSOKU </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Siguen el estandar de operación.Las condiciones requeridas para operar sin causar problemas)</t>
-    </r>
-  </si>
-  <si>
-    <t>5W + 1H</t>
+    <t>EWO (Emergency Work Order)</t>
   </si>
   <si>
     <r>
@@ -388,6 +338,90 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">COMO (HOW) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>¿Cómo difiere con respecto al optimo? ¿Cuál es el costo ($), que cantidad, en que tiempo?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GENSOKU </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Siguen el estandar de operación.Las condiciones requeridas para operar sin causar problemas)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GENRI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Se refiere a la teoria. Principios mecanicos y fisicos que rigen la operación)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GENJITSU </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Confirmar una descripcion precisa y cuantificada del problema)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GEMBUTSU </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Ver los objetos, piezas y materiales reales que participan en el problema)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GEMBA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Ir al lugar donde se produce el problema)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Cual (WHICH)? </t>
     </r>
     <r>
@@ -401,86 +435,55 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">COMO (HOW) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>¿Cómo difiere con respecto al optimo? ¿Cuál es el costo ($), que cantidad, en que tiempo?</t>
-    </r>
-  </si>
-  <si>
     <t>HOW + WHAT + WHERE + WHEN + WHICH + WHO = FENOMENO</t>
   </si>
   <si>
-    <t>df df df df df df</t>
+    <t xml:space="preserve">Tipo de Avería                                                                                                                                                                                                                                        </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">5 ANÁLISIS POR QUÉ - POR QUÉ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(diligencie este campo si todas las causas reaices se encuentran OK)</t>
-    </r>
+    <t>Diligenciada por</t>
   </si>
   <si>
-    <t>1 - Por qué?</t>
+    <t xml:space="preserve">Fecha </t>
   </si>
   <si>
-    <t>2 - Por qué?</t>
+    <t>Aviso #</t>
   </si>
   <si>
-    <t>3 - Por qué?</t>
+    <t>Equipo</t>
   </si>
   <si>
-    <t>4 - Por qué?</t>
+    <t>Area/Linea</t>
   </si>
   <si>
-    <t>5 - Por qué?</t>
+    <t>Turno</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>EWO #</t>
   </si>
   <si>
-    <t>Dibujo / Diagrama / Foto del 5 Por qué</t>
+    <t>5W + 1H</t>
   </si>
   <si>
-    <t>otra prueba</t>
+    <t xml:space="preserve">Técnico(s) de Mantenimiento Involucrado(s)                                                                                                                                                                                                                    </t>
   </si>
   <si>
-    <t>¿Qué tipo de falla es? Diligencie las fechas de los mantenimiento planeados y selecciones la causa raiz basada en el gráfico de la bañera</t>
+    <t>Operario(s) Involucrado(s)</t>
   </si>
   <si>
-    <t>Fecha Ultimo Mtto</t>
+    <t xml:space="preserve">Fecha                                                                                                                                                                                                                                                                                                </t>
   </si>
   <si>
-    <t>Fecha Proximo Mtto</t>
+    <t>Ejecución Validada Por</t>
   </si>
   <si>
-    <t>Error Humano (instalación)</t>
+    <t>Análisis Elaborado Por</t>
   </si>
   <si>
-    <t>Condiciones de Operación</t>
+    <t>Contramedidas Definidas Por</t>
   </si>
   <si>
-    <t>Falla de Diseño</t>
-  </si>
-  <si>
-    <t>Condiciones Básicas</t>
-  </si>
-  <si>
-    <t>No PM</t>
+    <t>Tipo de Accion</t>
   </si>
   <si>
     <r>
@@ -498,74 +501,10 @@
     </r>
   </si>
   <si>
-    <t>Error Humano 
-(en operación)</t>
+    <t>Fecha Ultimo Mtto</t>
   </si>
   <si>
-    <t>No AM</t>
-  </si>
-  <si>
-    <t>Ciclo de la causa raíz</t>
-  </si>
-  <si>
-    <t>Lista de Acciones</t>
-  </si>
-  <si>
-    <t>Tipo de Accion</t>
-  </si>
-  <si>
-    <t>Responsable</t>
-  </si>
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>prueba</t>
-  </si>
-  <si>
-    <t>CM</t>
-  </si>
-  <si>
-    <t>Angel Morales</t>
-  </si>
-  <si>
-    <t>2.</t>
-  </si>
-  <si>
-    <t>3.</t>
-  </si>
-  <si>
-    <t>4.</t>
-  </si>
-  <si>
-    <t>5.</t>
-  </si>
-  <si>
-    <t>6.</t>
-  </si>
-  <si>
-    <t>7.</t>
-  </si>
-  <si>
-    <t>8.</t>
-  </si>
-  <si>
-    <t>9.</t>
-  </si>
-  <si>
-    <t>10.</t>
-  </si>
-  <si>
-    <t>11.</t>
-  </si>
-  <si>
-    <t>12.</t>
-  </si>
-  <si>
-    <t>13.</t>
+    <t>Fecha Proximo Mtto</t>
   </si>
   <si>
     <r>
@@ -630,37 +569,32 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Técnico(s) de Mantenimiento Involucrado(s)                                                                                                                                                                                                                    </t>
+    <r>
+      <t xml:space="preserve">5 ANÁLISIS POR QUÉ - POR QUÉ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(diligencie este campo si todas las causas reaices se encuentran OK)</t>
+    </r>
   </si>
   <si>
-    <t>Operario(s) Involucrado(s)</t>
-  </si>
-  <si>
-    <t>Édinson Rodríguez Urrea</t>
-  </si>
-  <si>
-    <t>Deisy Ipus</t>
-  </si>
-  <si>
-    <t>Análisis Elaborado Por</t>
-  </si>
-  <si>
-    <t>Contramedidas Definidas Por</t>
-  </si>
-  <si>
-    <t>Ejecución Validada Por</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha                                                                                                                                                                                                                                                                                                </t>
-  </si>
-  <si>
-    <t>Fabian Morante Olmos</t>
-  </si>
-  <si>
-    <t>Diego Fernando Murillo Arboleda</t>
-  </si>
-  <si>
-    <t>Carlos Andres Varela</t>
+    <r>
+      <t xml:space="preserve">IDENTIFICACION DE CAUSAS RAICES - 5G </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(llene esta seccion teniendo en cuenta el principio de los 5G)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -788,8 +722,21 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF0000FF"/>
+      <name val="Unilever DIN Offc Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
       <i/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Unilever DIN Offc Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
       <color theme="1"/>
       <name val="Unilever DIN Offc Pro"/>
       <family val="2"/>
@@ -802,23 +749,9 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
-      <color theme="1"/>
-      <name val="Unilever DIN Offc Pro"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Unilever DIN Offc Pro"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="7"/>
-      <color rgb="FF0000FF"/>
-      <name val="Unilever DIN Offc Pro"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -829,9 +762,10 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <color theme="1"/>
+      <name val="Unilever DIN Offc Pro"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1507,6 +1441,333 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1564,13 +1825,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1587,333 +1848,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1947,7 +1881,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1963,7 +1897,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2033,9 +1967,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
+      <xdr:colOff>631050</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>447676</xdr:rowOff>
+      <xdr:rowOff>447675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7460,159 +7394,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>571500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="image1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>285750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="image3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Elipse 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{371A65B0-A949-47B4-8F7D-3B8D1DCB20D9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3556000" y="21590000"/>
-          <a:ext cx="1016000" cy="2540000"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:alpha val="11000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-CO" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7956,46 +7737,46 @@
     <col min="9" max="10" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="144" t="s">
-        <v>0</v>
+    <row r="1" spans="1:16" ht="39.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="81" t="s">
+        <v>53</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="147"/>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="84"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
-      <c r="C2" s="96" t="s">
-        <v>3</v>
+      <c r="C2" s="85" t="s">
+        <v>70</v>
       </c>
-      <c r="D2" s="148"/>
+      <c r="D2" s="86"/>
       <c r="E2" s="31" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
-      <c r="H2" s="149" t="s">
-        <v>7</v>
+      <c r="H2" s="87" t="s">
+        <v>66</v>
       </c>
-      <c r="I2" s="150"/>
+      <c r="I2" s="88"/>
       <c r="J2" s="2" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -8004,33 +7785,17 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25">
-        <v>2</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="162" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="163"/>
-      <c r="E3" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="162" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="163"/>
-      <c r="J3" s="30">
-        <v>3</v>
-      </c>
+    <row r="3" spans="1:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="30"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -8038,27 +7803,27 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="151" t="s">
-        <v>15</v>
+    <row r="4" spans="1:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="89" t="s">
+        <v>4</v>
       </c>
-      <c r="B4" s="151" t="s">
-        <v>16</v>
+      <c r="B4" s="89" t="s">
+        <v>5</v>
       </c>
-      <c r="C4" s="153" t="s">
-        <v>17</v>
+      <c r="C4" s="91" t="s">
+        <v>6</v>
       </c>
-      <c r="D4" s="153"/>
-      <c r="E4" s="153"/>
-      <c r="F4" s="154"/>
-      <c r="G4" s="154"/>
-      <c r="H4" s="151" t="s">
-        <v>18</v>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="89" t="s">
+        <v>7</v>
       </c>
-      <c r="I4" s="155" t="s">
-        <v>19</v>
+      <c r="I4" s="93" t="s">
+        <v>8</v>
       </c>
-      <c r="J4" s="156"/>
+      <c r="J4" s="94"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -8066,27 +7831,27 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="152"/>
-      <c r="B5" s="152"/>
+    <row r="5" spans="1:16" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="90"/>
+      <c r="B5" s="90"/>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
-      <c r="H5" s="152"/>
-      <c r="I5" s="157"/>
-      <c r="J5" s="158"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="96"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -8094,35 +7859,17 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
-        <v>43544.515972222202</v>
-      </c>
-      <c r="B6" s="15">
-        <v>43544.524305555598</v>
-      </c>
-      <c r="C6" s="16">
-        <v>12</v>
-      </c>
-      <c r="D6" s="16">
-        <v>9</v>
-      </c>
-      <c r="E6" s="16">
-        <v>2</v>
-      </c>
-      <c r="F6" s="16">
-        <v>1</v>
-      </c>
-      <c r="G6" s="16">
-        <v>3</v>
-      </c>
-      <c r="H6" s="15">
-        <v>43544.534722222197</v>
-      </c>
-      <c r="I6" s="168">
-        <v>27</v>
-      </c>
-      <c r="J6" s="169"/>
+    <row r="6" spans="1:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="110"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -8130,21 +7877,21 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="164" t="s">
-        <v>25</v>
+    <row r="7" spans="1:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="105" t="s">
+        <v>14</v>
       </c>
-      <c r="B7" s="165"/>
-      <c r="C7" s="165"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="119" t="s">
-        <v>26</v>
+      <c r="B7" s="106"/>
+      <c r="C7" s="106"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="97" t="s">
+        <v>37</v>
       </c>
-      <c r="G7" s="167"/>
-      <c r="H7" s="167"/>
-      <c r="I7" s="167"/>
-      <c r="J7" s="120"/>
+      <c r="G7" s="108"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="98"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -8153,214 +7900,204 @@
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="140"/>
-      <c r="B8" s="141"/>
-      <c r="C8" s="141"/>
-      <c r="D8" s="141"/>
-      <c r="E8" s="142"/>
-      <c r="F8" s="170" t="s">
-        <v>27</v>
+      <c r="A8" s="131"/>
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="112"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="113"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="99"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="115"/>
+      <c r="H9" s="115"/>
+      <c r="I9" s="115"/>
+      <c r="J9" s="116"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="99"/>
+      <c r="B10" s="100"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="129"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="115"/>
+      <c r="H10" s="115"/>
+      <c r="I10" s="115"/>
+      <c r="J10" s="116"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="99"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="100"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="129"/>
+      <c r="F11" s="114"/>
+      <c r="G11" s="115"/>
+      <c r="H11" s="115"/>
+      <c r="I11" s="115"/>
+      <c r="J11" s="116"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="99"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="117" t="s">
+        <v>38</v>
       </c>
-      <c r="G8" s="171"/>
-      <c r="H8" s="171"/>
-      <c r="I8" s="171"/>
-      <c r="J8" s="172"/>
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="143"/>
-      <c r="B9" s="136"/>
-      <c r="C9" s="136"/>
-      <c r="D9" s="136"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="174"/>
-      <c r="H9" s="174"/>
-      <c r="I9" s="174"/>
-      <c r="J9" s="175"/>
-      <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="143"/>
-      <c r="B10" s="136"/>
-      <c r="C10" s="136"/>
-      <c r="D10" s="136"/>
-      <c r="E10" s="137"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="174"/>
-      <c r="H10" s="174"/>
-      <c r="I10" s="174"/>
-      <c r="J10" s="175"/>
-      <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="143"/>
-      <c r="B11" s="136"/>
-      <c r="C11" s="136"/>
-      <c r="D11" s="136"/>
-      <c r="E11" s="137"/>
-      <c r="F11" s="173"/>
-      <c r="G11" s="174"/>
-      <c r="H11" s="174"/>
-      <c r="I11" s="174"/>
-      <c r="J11" s="175"/>
-      <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="143"/>
-      <c r="B12" s="136"/>
-      <c r="C12" s="136"/>
-      <c r="D12" s="136"/>
-      <c r="E12" s="137"/>
-      <c r="F12" s="121" t="s">
-        <v>28</v>
+      <c r="G12" s="118"/>
+      <c r="H12" s="118"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="119"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="99"/>
+      <c r="B13" s="100"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="120" t="s">
+        <v>15</v>
       </c>
-      <c r="G12" s="122"/>
-      <c r="H12" s="122"/>
-      <c r="I12" s="122"/>
-      <c r="J12" s="123"/>
-      <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="143"/>
-      <c r="B13" s="136"/>
-      <c r="C13" s="136"/>
-      <c r="D13" s="136"/>
-      <c r="E13" s="137"/>
-      <c r="F13" s="124" t="s">
-        <v>29</v>
+      <c r="G13" s="121"/>
+      <c r="H13" s="121"/>
+      <c r="I13" s="121"/>
+      <c r="J13" s="122"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="99"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="100"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="129"/>
+      <c r="F14" s="33" t="s">
+        <v>16</v>
       </c>
-      <c r="G13" s="125"/>
-      <c r="H13" s="125"/>
-      <c r="I13" s="125"/>
-      <c r="J13" s="126"/>
-      <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="143"/>
-      <c r="B14" s="136"/>
-      <c r="C14" s="136"/>
-      <c r="D14" s="136"/>
-      <c r="E14" s="137"/>
-      <c r="F14" s="33" t="s">
-        <v>30</v>
+      <c r="G14" s="123" t="s">
+        <v>17</v>
       </c>
-      <c r="G14" s="130" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="130"/>
+      <c r="H14" s="123"/>
       <c r="I14" s="34" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="J14" s="35" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="143"/>
-      <c r="B15" s="136"/>
-      <c r="C15" s="136"/>
-      <c r="D15" s="136"/>
-      <c r="E15" s="137"/>
-      <c r="F15" s="17">
-        <v>233</v>
-      </c>
-      <c r="G15" s="131" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="131"/>
+      <c r="A15" s="99"/>
+      <c r="B15" s="100"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="129"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
       <c r="I15" s="11"/>
-      <c r="J15" s="11" t="s">
-        <v>35</v>
-      </c>
+      <c r="J15" s="11"/>
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="143" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="136"/>
-      <c r="C16" s="136"/>
-      <c r="D16" s="136"/>
-      <c r="E16" s="137"/>
+      <c r="A16" s="99"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="100"/>
+      <c r="E16" s="129"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="131"/>
-      <c r="H16" s="131"/>
+      <c r="G16" s="124"/>
+      <c r="H16" s="124"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="143"/>
-      <c r="B17" s="136"/>
-      <c r="C17" s="136"/>
-      <c r="D17" s="136"/>
-      <c r="E17" s="137"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="129"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="131"/>
-      <c r="H17" s="131"/>
+      <c r="G17" s="124"/>
+      <c r="H17" s="124"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="143"/>
-      <c r="B18" s="136"/>
-      <c r="C18" s="136"/>
-      <c r="D18" s="136"/>
-      <c r="E18" s="137"/>
+      <c r="A18" s="99"/>
+      <c r="B18" s="100"/>
+      <c r="C18" s="100"/>
+      <c r="D18" s="100"/>
+      <c r="E18" s="129"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="131"/>
-      <c r="H18" s="131"/>
+      <c r="G18" s="124"/>
+      <c r="H18" s="124"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="161"/>
-      <c r="B19" s="138"/>
-      <c r="C19" s="138"/>
-      <c r="D19" s="138"/>
-      <c r="E19" s="139"/>
+    <row r="19" spans="1:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="101"/>
+      <c r="B19" s="102"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="102"/>
+      <c r="E19" s="130"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="132"/>
-      <c r="H19" s="132"/>
+      <c r="G19" s="125"/>
+      <c r="H19" s="125"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="127" t="s">
-        <v>37</v>
+    <row r="20" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="54" t="s">
+        <v>52</v>
       </c>
-      <c r="B20" s="128"/>
-      <c r="C20" s="128"/>
-      <c r="D20" s="128"/>
-      <c r="E20" s="128"/>
-      <c r="F20" s="128"/>
-      <c r="G20" s="128"/>
-      <c r="H20" s="128"/>
-      <c r="I20" s="128"/>
-      <c r="J20" s="129"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="56"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="185" t="s">
-        <v>38</v>
+    <row r="21" spans="1:16" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="76" t="s">
+        <v>87</v>
       </c>
-      <c r="B21" s="186"/>
-      <c r="C21" s="186"/>
-      <c r="D21" s="186"/>
-      <c r="E21" s="186"/>
-      <c r="F21" s="186"/>
-      <c r="G21" s="186"/>
-      <c r="H21" s="186"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
       <c r="I21" s="5" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -8369,22 +8106,18 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="119" t="s">
-        <v>41</v>
+    <row r="22" spans="1:16" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="97" t="s">
+        <v>63</v>
       </c>
-      <c r="B22" s="120"/>
-      <c r="C22" s="133" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="134"/>
-      <c r="E22" s="134"/>
-      <c r="F22" s="134"/>
-      <c r="G22" s="134"/>
-      <c r="H22" s="135"/>
-      <c r="I22" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="B22" s="98"/>
+      <c r="C22" s="126"/>
+      <c r="D22" s="127"/>
+      <c r="E22" s="127"/>
+      <c r="F22" s="127"/>
+      <c r="G22" s="127"/>
+      <c r="H22" s="128"/>
+      <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -8393,22 +8126,18 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="119" t="s">
-        <v>44</v>
+    <row r="23" spans="1:16" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="97" t="s">
+        <v>62</v>
       </c>
-      <c r="B23" s="120"/>
-      <c r="C23" s="133" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="134"/>
-      <c r="E23" s="134"/>
-      <c r="F23" s="134"/>
-      <c r="G23" s="134"/>
-      <c r="H23" s="135"/>
-      <c r="I23" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="B23" s="98"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="127"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="128"/>
+      <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -8417,22 +8146,18 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="119" t="s">
-        <v>45</v>
+    <row r="24" spans="1:16" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="97" t="s">
+        <v>61</v>
       </c>
-      <c r="B24" s="120"/>
-      <c r="C24" s="133" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="134"/>
-      <c r="E24" s="134"/>
-      <c r="F24" s="134"/>
-      <c r="G24" s="134"/>
-      <c r="H24" s="135"/>
-      <c r="I24" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="B24" s="98"/>
+      <c r="C24" s="126"/>
+      <c r="D24" s="127"/>
+      <c r="E24" s="127"/>
+      <c r="F24" s="127"/>
+      <c r="G24" s="127"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -8441,20 +8166,18 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="119" t="s">
-        <v>46</v>
+    <row r="25" spans="1:16" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="97" t="s">
+        <v>60</v>
       </c>
-      <c r="B25" s="120"/>
-      <c r="C25" s="133"/>
-      <c r="D25" s="134"/>
-      <c r="E25" s="134"/>
-      <c r="F25" s="134"/>
-      <c r="G25" s="134"/>
-      <c r="H25" s="135"/>
-      <c r="I25" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="B25" s="98"/>
+      <c r="C25" s="126"/>
+      <c r="D25" s="127"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="127"/>
+      <c r="G25" s="127"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -8463,20 +8186,18 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="119" t="s">
-        <v>47</v>
+    <row r="26" spans="1:16" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="97" t="s">
+        <v>59</v>
       </c>
-      <c r="B26" s="120"/>
-      <c r="C26" s="133"/>
-      <c r="D26" s="134"/>
-      <c r="E26" s="134"/>
-      <c r="F26" s="134"/>
-      <c r="G26" s="134"/>
-      <c r="H26" s="135"/>
-      <c r="I26" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="B26" s="98"/>
+      <c r="C26" s="126"/>
+      <c r="D26" s="127"/>
+      <c r="E26" s="127"/>
+      <c r="F26" s="127"/>
+      <c r="G26" s="127"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="9"/>
       <c r="J26" s="9"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -8485,19 +8206,19 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="127" t="s">
-        <v>48</v>
+    <row r="27" spans="1:16" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="54" t="s">
+        <v>74</v>
       </c>
-      <c r="B27" s="128"/>
-      <c r="C27" s="128"/>
-      <c r="D27" s="128"/>
-      <c r="E27" s="128"/>
-      <c r="F27" s="128"/>
-      <c r="G27" s="128"/>
-      <c r="H27" s="128"/>
-      <c r="I27" s="128"/>
-      <c r="J27" s="129"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="56"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -8505,21 +8226,19 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="119" t="s">
-        <v>49</v>
+    <row r="28" spans="1:16" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="97" t="s">
+        <v>54</v>
       </c>
-      <c r="B28" s="120"/>
-      <c r="C28" s="159" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="159"/>
-      <c r="E28" s="159"/>
-      <c r="F28" s="159"/>
-      <c r="G28" s="159"/>
-      <c r="H28" s="159"/>
-      <c r="I28" s="159"/>
-      <c r="J28" s="160"/>
+      <c r="B28" s="98"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="72"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -8527,21 +8246,19 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="119" t="s">
-        <v>50</v>
+    <row r="29" spans="1:16" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="97" t="s">
+        <v>55</v>
       </c>
-      <c r="B29" s="120"/>
-      <c r="C29" s="159" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="159"/>
-      <c r="E29" s="159"/>
-      <c r="F29" s="159"/>
-      <c r="G29" s="159"/>
-      <c r="H29" s="159"/>
-      <c r="I29" s="159"/>
-      <c r="J29" s="160"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="72"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -8549,21 +8266,19 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="119" t="s">
-        <v>51</v>
+    <row r="30" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="97" t="s">
+        <v>56</v>
       </c>
-      <c r="B30" s="120"/>
-      <c r="C30" s="159" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="159"/>
-      <c r="E30" s="159"/>
-      <c r="F30" s="159"/>
-      <c r="G30" s="159"/>
-      <c r="H30" s="159"/>
-      <c r="I30" s="159"/>
-      <c r="J30" s="160"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="72"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -8571,21 +8286,19 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="119" t="s">
-        <v>52</v>
+    <row r="31" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="97" t="s">
+        <v>57</v>
       </c>
-      <c r="B31" s="120"/>
-      <c r="C31" s="159" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="159"/>
-      <c r="E31" s="159"/>
-      <c r="F31" s="159"/>
-      <c r="G31" s="159"/>
-      <c r="H31" s="159"/>
-      <c r="I31" s="159"/>
-      <c r="J31" s="160"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="72"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -8593,21 +8306,19 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="119" t="s">
-        <v>53</v>
+    <row r="32" spans="1:16" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="97" t="s">
+        <v>64</v>
       </c>
-      <c r="B32" s="120"/>
-      <c r="C32" s="159" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="159"/>
-      <c r="E32" s="159"/>
-      <c r="F32" s="159"/>
-      <c r="G32" s="159"/>
-      <c r="H32" s="159"/>
-      <c r="I32" s="159"/>
-      <c r="J32" s="160"/>
+      <c r="B32" s="98"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="72"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -8615,21 +8326,19 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="119" t="s">
-        <v>54</v>
+    <row r="33" spans="1:16" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="97" t="s">
+        <v>58</v>
       </c>
-      <c r="B33" s="120"/>
-      <c r="C33" s="159" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" s="159"/>
-      <c r="E33" s="159"/>
-      <c r="F33" s="159"/>
-      <c r="G33" s="159"/>
-      <c r="H33" s="159"/>
-      <c r="I33" s="159"/>
-      <c r="J33" s="160"/>
+      <c r="B33" s="98"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="72"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -8637,19 +8346,19 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="187" t="s">
-        <v>55</v>
+    <row r="34" spans="1:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="78" t="s">
+        <v>65</v>
       </c>
-      <c r="B34" s="188"/>
-      <c r="C34" s="188"/>
-      <c r="D34" s="188"/>
-      <c r="E34" s="188"/>
-      <c r="F34" s="188"/>
-      <c r="G34" s="188"/>
-      <c r="H34" s="188"/>
-      <c r="I34" s="188"/>
-      <c r="J34" s="189"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="79"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="79"/>
+      <c r="G34" s="79"/>
+      <c r="H34" s="79"/>
+      <c r="I34" s="79"/>
+      <c r="J34" s="80"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -8657,19 +8366,17 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="181" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" s="159"/>
-      <c r="C35" s="159"/>
-      <c r="D35" s="159"/>
-      <c r="E35" s="159"/>
-      <c r="F35" s="159"/>
-      <c r="G35" s="159"/>
-      <c r="H35" s="159"/>
-      <c r="I35" s="159"/>
-      <c r="J35" s="160"/>
+    <row r="35" spans="1:16" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="70"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="72"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -8677,285 +8384,283 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="182" t="s">
-        <v>57</v>
+    <row r="36" spans="1:16" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="73" t="s">
+        <v>86</v>
       </c>
-      <c r="B36" s="183"/>
-      <c r="C36" s="183"/>
-      <c r="D36" s="183"/>
-      <c r="E36" s="183"/>
-      <c r="F36" s="183"/>
-      <c r="G36" s="183"/>
-      <c r="H36" s="183"/>
-      <c r="I36" s="183"/>
-      <c r="J36" s="184"/>
+      <c r="B36" s="74"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="74"/>
+      <c r="I36" s="74"/>
+      <c r="J36" s="75"/>
     </row>
     <row r="37" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="114" t="s">
-        <v>58</v>
+      <c r="A37" s="134" t="s">
+        <v>20</v>
       </c>
-      <c r="B37" s="115"/>
-      <c r="C37" s="116" t="s">
-        <v>59</v>
+      <c r="B37" s="135"/>
+      <c r="C37" s="136" t="s">
+        <v>21</v>
       </c>
-      <c r="D37" s="115"/>
-      <c r="E37" s="116" t="s">
-        <v>60</v>
+      <c r="D37" s="135"/>
+      <c r="E37" s="136" t="s">
+        <v>22</v>
       </c>
-      <c r="F37" s="115"/>
-      <c r="G37" s="116" t="s">
-        <v>61</v>
+      <c r="F37" s="135"/>
+      <c r="G37" s="136" t="s">
+        <v>23</v>
       </c>
-      <c r="H37" s="115"/>
-      <c r="I37" s="116" t="s">
-        <v>62</v>
+      <c r="H37" s="135"/>
+      <c r="I37" s="136" t="s">
+        <v>24</v>
       </c>
-      <c r="J37" s="117"/>
+      <c r="J37" s="137"/>
     </row>
     <row r="38" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="118"/>
-      <c r="B38" s="106"/>
-      <c r="C38" s="106"/>
-      <c r="D38" s="106"/>
-      <c r="E38" s="106"/>
-      <c r="F38" s="106"/>
-      <c r="G38" s="106"/>
-      <c r="H38" s="106"/>
-      <c r="I38" s="106"/>
-      <c r="J38" s="108"/>
+      <c r="A38" s="138"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="144"/>
     </row>
     <row r="39" spans="1:16" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="118" t="s">
-        <v>63</v>
+      <c r="A39" s="138" t="s">
+        <v>36</v>
       </c>
-      <c r="B39" s="106"/>
-      <c r="C39" s="106"/>
-      <c r="D39" s="106"/>
-      <c r="E39" s="106"/>
-      <c r="F39" s="106"/>
-      <c r="G39" s="106"/>
-      <c r="H39" s="106"/>
-      <c r="I39" s="106"/>
-      <c r="J39" s="109"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="62"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="62"/>
+      <c r="I39" s="62"/>
+      <c r="J39" s="145"/>
     </row>
     <row r="40" spans="1:16" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="102" t="s">
-        <v>63</v>
+      <c r="A40" s="139" t="s">
+        <v>36</v>
       </c>
-      <c r="B40" s="103"/>
-      <c r="C40" s="106"/>
-      <c r="D40" s="107"/>
-      <c r="E40" s="106" t="s">
-        <v>63</v>
+      <c r="B40" s="140"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="143"/>
+      <c r="E40" s="62" t="s">
+        <v>36</v>
       </c>
-      <c r="F40" s="106"/>
-      <c r="G40" s="106" t="s">
-        <v>63</v>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62" t="s">
+        <v>36</v>
       </c>
-      <c r="H40" s="106"/>
-      <c r="I40" s="110" t="s">
-        <v>63</v>
+      <c r="H40" s="62"/>
+      <c r="I40" s="146" t="s">
+        <v>36</v>
       </c>
-      <c r="J40" s="109"/>
-    </row>
-    <row r="41" spans="1:16" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="104"/>
-      <c r="B41" s="105"/>
-      <c r="C41" s="105"/>
-      <c r="D41" s="105"/>
-      <c r="E41" s="113"/>
-      <c r="F41" s="113"/>
-      <c r="G41" s="113"/>
-      <c r="H41" s="113"/>
-      <c r="I41" s="111"/>
-      <c r="J41" s="112"/>
+      <c r="J40" s="145"/>
+    </row>
+    <row r="41" spans="1:16" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="141"/>
+      <c r="B41" s="142"/>
+      <c r="C41" s="142"/>
+      <c r="D41" s="142"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="63"/>
+      <c r="I41" s="147"/>
+      <c r="J41" s="148"/>
     </row>
     <row r="42" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="54" t="s">
-        <v>64</v>
+      <c r="A42" s="163" t="s">
+        <v>25</v>
       </c>
-      <c r="B42" s="55"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="55"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="56"/>
+      <c r="B42" s="164"/>
+      <c r="C42" s="164"/>
+      <c r="D42" s="164"/>
+      <c r="E42" s="164"/>
+      <c r="F42" s="164"/>
+      <c r="G42" s="164"/>
+      <c r="H42" s="164"/>
+      <c r="I42" s="164"/>
+      <c r="J42" s="165"/>
     </row>
     <row r="43" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="57"/>
-      <c r="B43" s="58"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="59"/>
+      <c r="A43" s="166"/>
+      <c r="B43" s="167"/>
+      <c r="C43" s="167"/>
+      <c r="D43" s="167"/>
+      <c r="E43" s="167"/>
+      <c r="F43" s="167"/>
+      <c r="G43" s="167"/>
+      <c r="H43" s="167"/>
+      <c r="I43" s="167"/>
+      <c r="J43" s="168"/>
     </row>
     <row r="44" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="57"/>
-      <c r="B44" s="58"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="59"/>
+      <c r="A44" s="166"/>
+      <c r="B44" s="167"/>
+      <c r="C44" s="167"/>
+      <c r="D44" s="167"/>
+      <c r="E44" s="167"/>
+      <c r="F44" s="167"/>
+      <c r="G44" s="167"/>
+      <c r="H44" s="167"/>
+      <c r="I44" s="167"/>
+      <c r="J44" s="168"/>
     </row>
     <row r="45" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="57"/>
-      <c r="B45" s="58"/>
-      <c r="C45" s="58"/>
-      <c r="D45" s="58"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="58"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="58"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="59"/>
+      <c r="A45" s="166"/>
+      <c r="B45" s="167"/>
+      <c r="C45" s="167"/>
+      <c r="D45" s="167"/>
+      <c r="E45" s="167"/>
+      <c r="F45" s="167"/>
+      <c r="G45" s="167"/>
+      <c r="H45" s="167"/>
+      <c r="I45" s="167"/>
+      <c r="J45" s="168"/>
     </row>
     <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="57"/>
-      <c r="B46" s="58"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="58"/>
-      <c r="J46" s="59"/>
+      <c r="A46" s="166"/>
+      <c r="B46" s="167"/>
+      <c r="C46" s="167"/>
+      <c r="D46" s="167"/>
+      <c r="E46" s="167"/>
+      <c r="F46" s="167"/>
+      <c r="G46" s="167"/>
+      <c r="H46" s="167"/>
+      <c r="I46" s="167"/>
+      <c r="J46" s="168"/>
     </row>
     <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="57"/>
-      <c r="B47" s="58"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="58"/>
-      <c r="J47" s="59"/>
+      <c r="A47" s="166"/>
+      <c r="B47" s="167"/>
+      <c r="C47" s="167"/>
+      <c r="D47" s="167"/>
+      <c r="E47" s="167"/>
+      <c r="F47" s="167"/>
+      <c r="G47" s="167"/>
+      <c r="H47" s="167"/>
+      <c r="I47" s="167"/>
+      <c r="J47" s="168"/>
     </row>
     <row r="48" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="57"/>
-      <c r="B48" s="58"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="58"/>
-      <c r="J48" s="59"/>
+      <c r="A48" s="166"/>
+      <c r="B48" s="167"/>
+      <c r="C48" s="167"/>
+      <c r="D48" s="167"/>
+      <c r="E48" s="167"/>
+      <c r="F48" s="167"/>
+      <c r="G48" s="167"/>
+      <c r="H48" s="167"/>
+      <c r="I48" s="167"/>
+      <c r="J48" s="168"/>
     </row>
     <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="57"/>
-      <c r="B49" s="58"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
-      <c r="J49" s="59"/>
+      <c r="A49" s="166"/>
+      <c r="B49" s="167"/>
+      <c r="C49" s="167"/>
+      <c r="D49" s="167"/>
+      <c r="E49" s="167"/>
+      <c r="F49" s="167"/>
+      <c r="G49" s="167"/>
+      <c r="H49" s="167"/>
+      <c r="I49" s="167"/>
+      <c r="J49" s="168"/>
     </row>
     <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="57"/>
-      <c r="B50" s="58"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
-      <c r="J50" s="59"/>
+      <c r="A50" s="166"/>
+      <c r="B50" s="167"/>
+      <c r="C50" s="167"/>
+      <c r="D50" s="167"/>
+      <c r="E50" s="167"/>
+      <c r="F50" s="167"/>
+      <c r="G50" s="167"/>
+      <c r="H50" s="167"/>
+      <c r="I50" s="167"/>
+      <c r="J50" s="168"/>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="57"/>
-      <c r="B51" s="58"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="58"/>
-      <c r="I51" s="58"/>
-      <c r="J51" s="59"/>
+      <c r="A51" s="166"/>
+      <c r="B51" s="167"/>
+      <c r="C51" s="167"/>
+      <c r="D51" s="167"/>
+      <c r="E51" s="167"/>
+      <c r="F51" s="167"/>
+      <c r="G51" s="167"/>
+      <c r="H51" s="167"/>
+      <c r="I51" s="167"/>
+      <c r="J51" s="168"/>
     </row>
     <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="57"/>
-      <c r="B52" s="58"/>
-      <c r="C52" s="58"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="58"/>
-      <c r="G52" s="58"/>
-      <c r="H52" s="58"/>
-      <c r="I52" s="58"/>
-      <c r="J52" s="59"/>
+      <c r="A52" s="166"/>
+      <c r="B52" s="167"/>
+      <c r="C52" s="167"/>
+      <c r="D52" s="167"/>
+      <c r="E52" s="167"/>
+      <c r="F52" s="167"/>
+      <c r="G52" s="167"/>
+      <c r="H52" s="167"/>
+      <c r="I52" s="167"/>
+      <c r="J52" s="168"/>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="57"/>
-      <c r="B53" s="58"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="58"/>
-      <c r="J53" s="59"/>
+      <c r="A53" s="166"/>
+      <c r="B53" s="167"/>
+      <c r="C53" s="167"/>
+      <c r="D53" s="167"/>
+      <c r="E53" s="167"/>
+      <c r="F53" s="167"/>
+      <c r="G53" s="167"/>
+      <c r="H53" s="167"/>
+      <c r="I53" s="167"/>
+      <c r="J53" s="168"/>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="57"/>
-      <c r="B54" s="58"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
-      <c r="J54" s="59"/>
+      <c r="A54" s="166"/>
+      <c r="B54" s="167"/>
+      <c r="C54" s="167"/>
+      <c r="D54" s="167"/>
+      <c r="E54" s="167"/>
+      <c r="F54" s="167"/>
+      <c r="G54" s="167"/>
+      <c r="H54" s="167"/>
+      <c r="I54" s="167"/>
+      <c r="J54" s="168"/>
     </row>
     <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="60" t="s">
-        <v>65</v>
+      <c r="A55" s="169"/>
+      <c r="B55" s="169"/>
+      <c r="C55" s="169"/>
+      <c r="D55" s="169"/>
+      <c r="E55" s="169"/>
+      <c r="F55" s="169"/>
+      <c r="G55" s="169"/>
+      <c r="H55" s="169"/>
+      <c r="I55" s="169"/>
+      <c r="J55" s="169"/>
+    </row>
+    <row r="56" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="170" t="s">
+        <v>27</v>
       </c>
-      <c r="B55" s="60"/>
-      <c r="C55" s="60"/>
-      <c r="D55" s="60"/>
-      <c r="E55" s="60"/>
-      <c r="F55" s="60"/>
-      <c r="G55" s="60"/>
-      <c r="H55" s="60"/>
-      <c r="I55" s="60"/>
-      <c r="J55" s="60"/>
-    </row>
-    <row r="56" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="61" t="s">
-        <v>66</v>
-      </c>
-      <c r="B56" s="62"/>
-      <c r="C56" s="62"/>
-      <c r="D56" s="62"/>
-      <c r="E56" s="62"/>
-      <c r="F56" s="62"/>
-      <c r="G56" s="62"/>
-      <c r="H56" s="62"/>
-      <c r="I56" s="62"/>
-      <c r="J56" s="63"/>
+      <c r="B56" s="171"/>
+      <c r="C56" s="171"/>
+      <c r="D56" s="171"/>
+      <c r="E56" s="171"/>
+      <c r="F56" s="171"/>
+      <c r="G56" s="171"/>
+      <c r="H56" s="171"/>
+      <c r="I56" s="171"/>
+      <c r="J56" s="172"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="18"/>
@@ -9032,7 +8737,7 @@
     <row r="63" spans="1:10" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A63" s="18"/>
       <c r="B63" s="43" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
@@ -9040,28 +8745,24 @@
       <c r="F63" s="19"/>
       <c r="G63" s="44"/>
       <c r="H63" s="50" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="I63" s="19"/>
       <c r="J63" s="20"/>
     </row>
     <row r="64" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="47"/>
-      <c r="B64" s="48" t="s">
-        <v>11</v>
-      </c>
+      <c r="B64" s="48"/>
       <c r="C64" s="49" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="D64" s="42"/>
       <c r="E64" s="21" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="F64" s="19"/>
       <c r="G64" s="45"/>
-      <c r="H64" s="48" t="s">
-        <v>11</v>
-      </c>
+      <c r="H64" s="48"/>
       <c r="I64" s="51"/>
       <c r="J64" s="20"/>
     </row>
@@ -9069,15 +8770,15 @@
       <c r="A65" s="18"/>
       <c r="B65" s="46"/>
       <c r="C65" s="22" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
       <c r="D65" s="42"/>
       <c r="E65" s="21" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="F65" s="19"/>
       <c r="G65" s="23" t="s">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="H65" s="46"/>
       <c r="I65" s="19"/>
@@ -9087,15 +8788,15 @@
       <c r="A66" s="18"/>
       <c r="B66" s="19"/>
       <c r="C66" s="22" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D66" s="43"/>
       <c r="E66" s="21" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="F66" s="19"/>
       <c r="G66" s="23" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="H66" s="19"/>
       <c r="I66" s="19"/>
@@ -9113,542 +8814,618 @@
       <c r="I67" s="19"/>
       <c r="J67" s="20"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="73" t="s">
+    <row r="68" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="182" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="183"/>
+      <c r="C68" s="183"/>
+      <c r="D68" s="183"/>
+      <c r="E68" s="183"/>
+      <c r="F68" s="183"/>
+      <c r="G68" s="183"/>
+      <c r="H68" s="183"/>
+      <c r="I68" s="183"/>
+      <c r="J68" s="184"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="173"/>
+      <c r="B69" s="174"/>
+      <c r="C69" s="174"/>
+      <c r="D69" s="174"/>
+      <c r="E69" s="174"/>
+      <c r="F69" s="174"/>
+      <c r="G69" s="174"/>
+      <c r="H69" s="174"/>
+      <c r="I69" s="174"/>
+      <c r="J69" s="175"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="176"/>
+      <c r="B70" s="177"/>
+      <c r="C70" s="177"/>
+      <c r="D70" s="177"/>
+      <c r="E70" s="177"/>
+      <c r="F70" s="177"/>
+      <c r="G70" s="177"/>
+      <c r="H70" s="177"/>
+      <c r="I70" s="177"/>
+      <c r="J70" s="178"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="176"/>
+      <c r="B71" s="177"/>
+      <c r="C71" s="177"/>
+      <c r="D71" s="177"/>
+      <c r="E71" s="177"/>
+      <c r="F71" s="177"/>
+      <c r="G71" s="177"/>
+      <c r="H71" s="177"/>
+      <c r="I71" s="177"/>
+      <c r="J71" s="178"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="176"/>
+      <c r="B72" s="177"/>
+      <c r="C72" s="177"/>
+      <c r="D72" s="177"/>
+      <c r="E72" s="177"/>
+      <c r="F72" s="177"/>
+      <c r="G72" s="177"/>
+      <c r="H72" s="177"/>
+      <c r="I72" s="177"/>
+      <c r="J72" s="178"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="176"/>
+      <c r="B73" s="177"/>
+      <c r="C73" s="177"/>
+      <c r="D73" s="177"/>
+      <c r="E73" s="177"/>
+      <c r="F73" s="177"/>
+      <c r="G73" s="177"/>
+      <c r="H73" s="177"/>
+      <c r="I73" s="177"/>
+      <c r="J73" s="178"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="176"/>
+      <c r="B74" s="177"/>
+      <c r="C74" s="177"/>
+      <c r="D74" s="177"/>
+      <c r="E74" s="177"/>
+      <c r="F74" s="177"/>
+      <c r="G74" s="177"/>
+      <c r="H74" s="177"/>
+      <c r="I74" s="177"/>
+      <c r="J74" s="178"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="176"/>
+      <c r="B75" s="177"/>
+      <c r="C75" s="177"/>
+      <c r="D75" s="177"/>
+      <c r="E75" s="177"/>
+      <c r="F75" s="177"/>
+      <c r="G75" s="177"/>
+      <c r="H75" s="177"/>
+      <c r="I75" s="177"/>
+      <c r="J75" s="178"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="176"/>
+      <c r="B76" s="177"/>
+      <c r="C76" s="177"/>
+      <c r="D76" s="177"/>
+      <c r="E76" s="177"/>
+      <c r="F76" s="177"/>
+      <c r="G76" s="177"/>
+      <c r="H76" s="177"/>
+      <c r="I76" s="177"/>
+      <c r="J76" s="178"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="176"/>
+      <c r="B77" s="177"/>
+      <c r="C77" s="177"/>
+      <c r="D77" s="177"/>
+      <c r="E77" s="177"/>
+      <c r="F77" s="177"/>
+      <c r="G77" s="177"/>
+      <c r="H77" s="177"/>
+      <c r="I77" s="177"/>
+      <c r="J77" s="178"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="176"/>
+      <c r="B78" s="177"/>
+      <c r="C78" s="177"/>
+      <c r="D78" s="177"/>
+      <c r="E78" s="177"/>
+      <c r="F78" s="177"/>
+      <c r="G78" s="177"/>
+      <c r="H78" s="177"/>
+      <c r="I78" s="177"/>
+      <c r="J78" s="178"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="176"/>
+      <c r="B79" s="177"/>
+      <c r="C79" s="177"/>
+      <c r="D79" s="177"/>
+      <c r="E79" s="177"/>
+      <c r="F79" s="177"/>
+      <c r="G79" s="177"/>
+      <c r="H79" s="177"/>
+      <c r="I79" s="177"/>
+      <c r="J79" s="178"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="176"/>
+      <c r="B80" s="177"/>
+      <c r="C80" s="177"/>
+      <c r="D80" s="177"/>
+      <c r="E80" s="177"/>
+      <c r="F80" s="177"/>
+      <c r="G80" s="177"/>
+      <c r="H80" s="177"/>
+      <c r="I80" s="177"/>
+      <c r="J80" s="178"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="176"/>
+      <c r="B81" s="177"/>
+      <c r="C81" s="177"/>
+      <c r="D81" s="177"/>
+      <c r="E81" s="177"/>
+      <c r="F81" s="177"/>
+      <c r="G81" s="177"/>
+      <c r="H81" s="177"/>
+      <c r="I81" s="177"/>
+      <c r="J81" s="178"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="176"/>
+      <c r="B82" s="177"/>
+      <c r="C82" s="177"/>
+      <c r="D82" s="177"/>
+      <c r="E82" s="177"/>
+      <c r="F82" s="177"/>
+      <c r="G82" s="177"/>
+      <c r="H82" s="177"/>
+      <c r="I82" s="177"/>
+      <c r="J82" s="178"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="176"/>
+      <c r="B83" s="177"/>
+      <c r="C83" s="177"/>
+      <c r="D83" s="177"/>
+      <c r="E83" s="177"/>
+      <c r="F83" s="177"/>
+      <c r="G83" s="177"/>
+      <c r="H83" s="177"/>
+      <c r="I83" s="177"/>
+      <c r="J83" s="178"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="176"/>
+      <c r="B84" s="177"/>
+      <c r="C84" s="177"/>
+      <c r="D84" s="177"/>
+      <c r="E84" s="177"/>
+      <c r="F84" s="177"/>
+      <c r="G84" s="177"/>
+      <c r="H84" s="177"/>
+      <c r="I84" s="177"/>
+      <c r="J84" s="178"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="176"/>
+      <c r="B85" s="177"/>
+      <c r="C85" s="177"/>
+      <c r="D85" s="177"/>
+      <c r="E85" s="177"/>
+      <c r="F85" s="177"/>
+      <c r="G85" s="177"/>
+      <c r="H85" s="177"/>
+      <c r="I85" s="177"/>
+      <c r="J85" s="178"/>
+    </row>
+    <row r="86" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="179"/>
+      <c r="B86" s="180"/>
+      <c r="C86" s="180"/>
+      <c r="D86" s="180"/>
+      <c r="E86" s="180"/>
+      <c r="F86" s="180"/>
+      <c r="G86" s="180"/>
+      <c r="H86" s="180"/>
+      <c r="I86" s="180"/>
+      <c r="J86" s="181"/>
+    </row>
+    <row r="87" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="185" t="s">
+        <v>35</v>
+      </c>
+      <c r="B87" s="186"/>
+      <c r="C87" s="186"/>
+      <c r="D87" s="186"/>
+      <c r="E87" s="186"/>
+      <c r="F87" s="187"/>
+      <c r="G87" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="H87" s="185" t="s">
+        <v>33</v>
+      </c>
+      <c r="I87" s="187"/>
+      <c r="J87" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B88" s="188"/>
+      <c r="C88" s="188"/>
+      <c r="D88" s="188"/>
+      <c r="E88" s="188"/>
+      <c r="F88" s="189"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="68"/>
+      <c r="I88" s="69"/>
+      <c r="J88" s="10"/>
+    </row>
+    <row r="89" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B89" s="149"/>
+      <c r="C89" s="149"/>
+      <c r="D89" s="149"/>
+      <c r="E89" s="149"/>
+      <c r="F89" s="150"/>
+      <c r="G89" s="12"/>
+      <c r="H89" s="68"/>
+      <c r="I89" s="69"/>
+      <c r="J89" s="10"/>
+    </row>
+    <row r="90" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B90" s="149"/>
+      <c r="C90" s="149"/>
+      <c r="D90" s="149"/>
+      <c r="E90" s="149"/>
+      <c r="F90" s="150"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="68"/>
+      <c r="I90" s="69"/>
+      <c r="J90" s="10"/>
+    </row>
+    <row r="91" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B91" s="64"/>
+      <c r="C91" s="64"/>
+      <c r="D91" s="64"/>
+      <c r="E91" s="64"/>
+      <c r="F91" s="65"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="66"/>
+      <c r="I91" s="67"/>
+      <c r="J91" s="7"/>
+    </row>
+    <row r="92" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B92" s="64"/>
+      <c r="C92" s="64"/>
+      <c r="D92" s="64"/>
+      <c r="E92" s="64"/>
+      <c r="F92" s="65"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="66"/>
+      <c r="I92" s="67"/>
+      <c r="J92" s="7"/>
+    </row>
+    <row r="93" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B93" s="64"/>
+      <c r="C93" s="64"/>
+      <c r="D93" s="64"/>
+      <c r="E93" s="64"/>
+      <c r="F93" s="65"/>
+      <c r="G93" s="12"/>
+      <c r="H93" s="66"/>
+      <c r="I93" s="67"/>
+      <c r="J93" s="7"/>
+    </row>
+    <row r="94" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B94" s="64"/>
+      <c r="C94" s="64"/>
+      <c r="D94" s="64"/>
+      <c r="E94" s="64"/>
+      <c r="F94" s="65"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="66"/>
+      <c r="I94" s="67"/>
+      <c r="J94" s="7"/>
+    </row>
+    <row r="95" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B95" s="64"/>
+      <c r="C95" s="64"/>
+      <c r="D95" s="64"/>
+      <c r="E95" s="64"/>
+      <c r="F95" s="65"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="66"/>
+      <c r="I95" s="67"/>
+      <c r="J95" s="7"/>
+    </row>
+    <row r="96" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B96" s="64"/>
+      <c r="C96" s="64"/>
+      <c r="D96" s="64"/>
+      <c r="E96" s="64"/>
+      <c r="F96" s="65"/>
+      <c r="G96" s="12"/>
+      <c r="H96" s="66"/>
+      <c r="I96" s="67"/>
+      <c r="J96" s="7"/>
+    </row>
+    <row r="97" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B97" s="64"/>
+      <c r="C97" s="64"/>
+      <c r="D97" s="64"/>
+      <c r="E97" s="64"/>
+      <c r="F97" s="65"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="66"/>
+      <c r="I97" s="67"/>
+      <c r="J97" s="7"/>
+    </row>
+    <row r="98" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B98" s="64"/>
+      <c r="C98" s="64"/>
+      <c r="D98" s="64"/>
+      <c r="E98" s="64"/>
+      <c r="F98" s="65"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="66"/>
+      <c r="I98" s="67"/>
+      <c r="J98" s="7"/>
+    </row>
+    <row r="99" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B99" s="64"/>
+      <c r="C99" s="64"/>
+      <c r="D99" s="64"/>
+      <c r="E99" s="64"/>
+      <c r="F99" s="65"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="66"/>
+      <c r="I99" s="67"/>
+      <c r="J99" s="7"/>
+    </row>
+    <row r="100" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B100" s="64"/>
+      <c r="C100" s="64"/>
+      <c r="D100" s="64"/>
+      <c r="E100" s="64"/>
+      <c r="F100" s="65"/>
+      <c r="G100" s="12"/>
+      <c r="H100" s="66"/>
+      <c r="I100" s="67"/>
+      <c r="J100" s="7"/>
+    </row>
+    <row r="101" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="155" t="s">
+        <v>85</v>
+      </c>
+      <c r="B101" s="156"/>
+      <c r="C101" s="156"/>
+      <c r="D101" s="156"/>
+      <c r="E101" s="156"/>
+      <c r="F101" s="156"/>
+      <c r="G101" s="156"/>
+      <c r="H101" s="156"/>
+      <c r="I101" s="156"/>
+      <c r="J101" s="157"/>
+    </row>
+    <row r="102" spans="1:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="85" t="s">
+        <v>75</v>
+      </c>
+      <c r="B102" s="158"/>
+      <c r="C102" s="158"/>
+      <c r="D102" s="158"/>
+      <c r="E102" s="159"/>
+      <c r="F102" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="G102" s="158"/>
+      <c r="H102" s="158"/>
+      <c r="I102" s="158"/>
+      <c r="J102" s="159"/>
+    </row>
+    <row r="103" spans="1:10" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="160"/>
+      <c r="B103" s="161"/>
+      <c r="C103" s="161"/>
+      <c r="D103" s="161"/>
+      <c r="E103" s="162"/>
+      <c r="F103" s="161"/>
+      <c r="G103" s="161"/>
+      <c r="H103" s="161"/>
+      <c r="I103" s="161"/>
+      <c r="J103" s="162"/>
+    </row>
+    <row r="104" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="151" t="s">
+        <v>79</v>
+      </c>
+      <c r="B104" s="152"/>
+      <c r="C104" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="D104" s="153" t="s">
+        <v>80</v>
+      </c>
+      <c r="E104" s="152"/>
+      <c r="F104" s="152"/>
+      <c r="G104" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="H104" s="151" t="s">
+        <v>78</v>
+      </c>
+      <c r="I104" s="154"/>
+      <c r="J104" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="B68" s="74"/>
-      <c r="C68" s="74"/>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
-      <c r="F68" s="74"/>
-      <c r="G68" s="74"/>
-      <c r="H68" s="74"/>
-      <c r="I68" s="74"/>
-      <c r="J68" s="75"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="64"/>
-      <c r="B69" s="65"/>
-      <c r="C69" s="65"/>
-      <c r="D69" s="65"/>
-      <c r="E69" s="65"/>
-      <c r="F69" s="65"/>
-      <c r="G69" s="65"/>
-      <c r="H69" s="65"/>
-      <c r="I69" s="65"/>
-      <c r="J69" s="66"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="67"/>
-      <c r="B70" s="68"/>
-      <c r="C70" s="68"/>
-      <c r="D70" s="68"/>
-      <c r="E70" s="68"/>
-      <c r="F70" s="68"/>
-      <c r="G70" s="68"/>
-      <c r="H70" s="68"/>
-      <c r="I70" s="68"/>
-      <c r="J70" s="69"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="67"/>
-      <c r="B71" s="68"/>
-      <c r="C71" s="68"/>
-      <c r="D71" s="68"/>
-      <c r="E71" s="68"/>
-      <c r="F71" s="68"/>
-      <c r="G71" s="68"/>
-      <c r="H71" s="68"/>
-      <c r="I71" s="68"/>
-      <c r="J71" s="69"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="67"/>
-      <c r="B72" s="68"/>
-      <c r="C72" s="68"/>
-      <c r="D72" s="68"/>
-      <c r="E72" s="68"/>
-      <c r="F72" s="68"/>
-      <c r="G72" s="68"/>
-      <c r="H72" s="68"/>
-      <c r="I72" s="68"/>
-      <c r="J72" s="69"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="67"/>
-      <c r="B73" s="68"/>
-      <c r="C73" s="68"/>
-      <c r="D73" s="68"/>
-      <c r="E73" s="68"/>
-      <c r="F73" s="68"/>
-      <c r="G73" s="68"/>
-      <c r="H73" s="68"/>
-      <c r="I73" s="68"/>
-      <c r="J73" s="69"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="67"/>
-      <c r="B74" s="68"/>
-      <c r="C74" s="68"/>
-      <c r="D74" s="68"/>
-      <c r="E74" s="68"/>
-      <c r="F74" s="68"/>
-      <c r="G74" s="68"/>
-      <c r="H74" s="68"/>
-      <c r="I74" s="68"/>
-      <c r="J74" s="69"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="67"/>
-      <c r="B75" s="68"/>
-      <c r="C75" s="68"/>
-      <c r="D75" s="68"/>
-      <c r="E75" s="68"/>
-      <c r="F75" s="68"/>
-      <c r="G75" s="68"/>
-      <c r="H75" s="68"/>
-      <c r="I75" s="68"/>
-      <c r="J75" s="69"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="67"/>
-      <c r="B76" s="68"/>
-      <c r="C76" s="68"/>
-      <c r="D76" s="68"/>
-      <c r="E76" s="68"/>
-      <c r="F76" s="68"/>
-      <c r="G76" s="68"/>
-      <c r="H76" s="68"/>
-      <c r="I76" s="68"/>
-      <c r="J76" s="69"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="67"/>
-      <c r="B77" s="68"/>
-      <c r="C77" s="68"/>
-      <c r="D77" s="68"/>
-      <c r="E77" s="68"/>
-      <c r="F77" s="68"/>
-      <c r="G77" s="68"/>
-      <c r="H77" s="68"/>
-      <c r="I77" s="68"/>
-      <c r="J77" s="69"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="67"/>
-      <c r="B78" s="68"/>
-      <c r="C78" s="68"/>
-      <c r="D78" s="68"/>
-      <c r="E78" s="68"/>
-      <c r="F78" s="68"/>
-      <c r="G78" s="68"/>
-      <c r="H78" s="68"/>
-      <c r="I78" s="68"/>
-      <c r="J78" s="69"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="67"/>
-      <c r="B79" s="68"/>
-      <c r="C79" s="68"/>
-      <c r="D79" s="68"/>
-      <c r="E79" s="68"/>
-      <c r="F79" s="68"/>
-      <c r="G79" s="68"/>
-      <c r="H79" s="68"/>
-      <c r="I79" s="68"/>
-      <c r="J79" s="69"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="67"/>
-      <c r="B80" s="68"/>
-      <c r="C80" s="68"/>
-      <c r="D80" s="68"/>
-      <c r="E80" s="68"/>
-      <c r="F80" s="68"/>
-      <c r="G80" s="68"/>
-      <c r="H80" s="68"/>
-      <c r="I80" s="68"/>
-      <c r="J80" s="69"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="67"/>
-      <c r="B81" s="68"/>
-      <c r="C81" s="68"/>
-      <c r="D81" s="68"/>
-      <c r="E81" s="68"/>
-      <c r="F81" s="68"/>
-      <c r="G81" s="68"/>
-      <c r="H81" s="68"/>
-      <c r="I81" s="68"/>
-      <c r="J81" s="69"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="67"/>
-      <c r="B82" s="68"/>
-      <c r="C82" s="68"/>
-      <c r="D82" s="68"/>
-      <c r="E82" s="68"/>
-      <c r="F82" s="68"/>
-      <c r="G82" s="68"/>
-      <c r="H82" s="68"/>
-      <c r="I82" s="68"/>
-      <c r="J82" s="69"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="67"/>
-      <c r="B83" s="68"/>
-      <c r="C83" s="68"/>
-      <c r="D83" s="68"/>
-      <c r="E83" s="68"/>
-      <c r="F83" s="68"/>
-      <c r="G83" s="68"/>
-      <c r="H83" s="68"/>
-      <c r="I83" s="68"/>
-      <c r="J83" s="69"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="67"/>
-      <c r="B84" s="68"/>
-      <c r="C84" s="68"/>
-      <c r="D84" s="68"/>
-      <c r="E84" s="68"/>
-      <c r="F84" s="68"/>
-      <c r="G84" s="68"/>
-      <c r="H84" s="68"/>
-      <c r="I84" s="68"/>
-      <c r="J84" s="69"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="67"/>
-      <c r="B85" s="68"/>
-      <c r="C85" s="68"/>
-      <c r="D85" s="68"/>
-      <c r="E85" s="68"/>
-      <c r="F85" s="68"/>
-      <c r="G85" s="68"/>
-      <c r="H85" s="68"/>
-      <c r="I85" s="68"/>
-      <c r="J85" s="69"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="70"/>
-      <c r="B86" s="71"/>
-      <c r="C86" s="71"/>
-      <c r="D86" s="71"/>
-      <c r="E86" s="71"/>
-      <c r="F86" s="71"/>
-      <c r="G86" s="71"/>
-      <c r="H86" s="71"/>
-      <c r="I86" s="71"/>
-      <c r="J86" s="72"/>
-    </row>
-    <row r="87" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="B87" s="77"/>
-      <c r="C87" s="77"/>
-      <c r="D87" s="77"/>
-      <c r="E87" s="77"/>
-      <c r="F87" s="78"/>
-      <c r="G87" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H87" s="76" t="s">
-        <v>80</v>
-      </c>
-      <c r="I87" s="78"/>
-      <c r="J87" s="24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="B88" s="79" t="s">
-        <v>83</v>
-      </c>
-      <c r="C88" s="79"/>
-      <c r="D88" s="79"/>
-      <c r="E88" s="79"/>
-      <c r="F88" s="80"/>
-      <c r="G88" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="H88" s="85" t="s">
-        <v>85</v>
-      </c>
-      <c r="I88" s="86"/>
-      <c r="J88" s="10">
-        <v>43544</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A89" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="B89" s="81"/>
-      <c r="C89" s="81"/>
-      <c r="D89" s="81"/>
-      <c r="E89" s="81"/>
-      <c r="F89" s="82"/>
-      <c r="G89" s="12"/>
-      <c r="H89" s="85"/>
-      <c r="I89" s="86"/>
-      <c r="J89" s="10"/>
-    </row>
-    <row r="90" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="B90" s="81"/>
-      <c r="C90" s="81"/>
-      <c r="D90" s="81"/>
-      <c r="E90" s="81"/>
-      <c r="F90" s="82"/>
-      <c r="G90" s="12"/>
-      <c r="H90" s="85"/>
-      <c r="I90" s="86"/>
-      <c r="J90" s="10"/>
-    </row>
-    <row r="91" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="B91" s="83"/>
-      <c r="C91" s="83"/>
-      <c r="D91" s="83"/>
-      <c r="E91" s="83"/>
-      <c r="F91" s="84"/>
-      <c r="G91" s="12"/>
-      <c r="H91" s="87"/>
-      <c r="I91" s="88"/>
-      <c r="J91" s="7"/>
-    </row>
-    <row r="92" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="B92" s="83"/>
-      <c r="C92" s="83"/>
-      <c r="D92" s="83"/>
-      <c r="E92" s="83"/>
-      <c r="F92" s="84"/>
-      <c r="G92" s="12"/>
-      <c r="H92" s="87"/>
-      <c r="I92" s="88"/>
-      <c r="J92" s="7"/>
-    </row>
-    <row r="93" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="B93" s="83"/>
-      <c r="C93" s="83"/>
-      <c r="D93" s="83"/>
-      <c r="E93" s="83"/>
-      <c r="F93" s="84"/>
-      <c r="G93" s="12"/>
-      <c r="H93" s="87"/>
-      <c r="I93" s="88"/>
-      <c r="J93" s="7"/>
-    </row>
-    <row r="94" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A94" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="B94" s="83"/>
-      <c r="C94" s="83"/>
-      <c r="D94" s="83"/>
-      <c r="E94" s="83"/>
-      <c r="F94" s="84"/>
-      <c r="G94" s="12"/>
-      <c r="H94" s="87"/>
-      <c r="I94" s="88"/>
-      <c r="J94" s="7"/>
-    </row>
-    <row r="95" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A95" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="B95" s="83"/>
-      <c r="C95" s="83"/>
-      <c r="D95" s="83"/>
-      <c r="E95" s="83"/>
-      <c r="F95" s="84"/>
-      <c r="G95" s="12"/>
-      <c r="H95" s="87"/>
-      <c r="I95" s="88"/>
-      <c r="J95" s="7"/>
-    </row>
-    <row r="96" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A96" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="B96" s="83"/>
-      <c r="C96" s="83"/>
-      <c r="D96" s="83"/>
-      <c r="E96" s="83"/>
-      <c r="F96" s="84"/>
-      <c r="G96" s="12"/>
-      <c r="H96" s="87"/>
-      <c r="I96" s="88"/>
-      <c r="J96" s="7"/>
-    </row>
-    <row r="97" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A97" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="B97" s="83"/>
-      <c r="C97" s="83"/>
-      <c r="D97" s="83"/>
-      <c r="E97" s="83"/>
-      <c r="F97" s="84"/>
-      <c r="G97" s="12"/>
-      <c r="H97" s="87"/>
-      <c r="I97" s="88"/>
-      <c r="J97" s="7"/>
-    </row>
-    <row r="98" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A98" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="B98" s="83"/>
-      <c r="C98" s="83"/>
-      <c r="D98" s="83"/>
-      <c r="E98" s="83"/>
-      <c r="F98" s="84"/>
-      <c r="G98" s="12"/>
-      <c r="H98" s="87"/>
-      <c r="I98" s="88"/>
-      <c r="J98" s="7"/>
-    </row>
-    <row r="99" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A99" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="B99" s="83"/>
-      <c r="C99" s="83"/>
-      <c r="D99" s="83"/>
-      <c r="E99" s="83"/>
-      <c r="F99" s="84"/>
-      <c r="G99" s="12"/>
-      <c r="H99" s="87"/>
-      <c r="I99" s="88"/>
-      <c r="J99" s="7"/>
-    </row>
-    <row r="100" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A100" s="40" t="s">
-        <v>97</v>
-      </c>
-      <c r="B100" s="83"/>
-      <c r="C100" s="83"/>
-      <c r="D100" s="83"/>
-      <c r="E100" s="83"/>
-      <c r="F100" s="84"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="87"/>
-      <c r="I100" s="88"/>
-      <c r="J100" s="7"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="93" t="s">
-        <v>98</v>
-      </c>
-      <c r="B101" s="94"/>
-      <c r="C101" s="94"/>
-      <c r="D101" s="94"/>
-      <c r="E101" s="94"/>
-      <c r="F101" s="94"/>
-      <c r="G101" s="94"/>
-      <c r="H101" s="94"/>
-      <c r="I101" s="94"/>
-      <c r="J101" s="95"/>
-    </row>
-    <row r="102" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="96" t="s">
-        <v>99</v>
-      </c>
-      <c r="B102" s="97"/>
-      <c r="C102" s="97"/>
-      <c r="D102" s="97"/>
-      <c r="E102" s="98"/>
-      <c r="F102" s="96" t="s">
-        <v>100</v>
-      </c>
-      <c r="G102" s="97"/>
-      <c r="H102" s="97"/>
-      <c r="I102" s="97"/>
-      <c r="J102" s="98"/>
-    </row>
-    <row r="103" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="99" t="s">
-        <v>101</v>
-      </c>
-      <c r="B103" s="100"/>
-      <c r="C103" s="100"/>
-      <c r="D103" s="100"/>
-      <c r="E103" s="101"/>
-      <c r="F103" s="100" t="s">
-        <v>102</v>
-      </c>
-      <c r="G103" s="100"/>
-      <c r="H103" s="100"/>
-      <c r="I103" s="100"/>
-      <c r="J103" s="101"/>
-    </row>
-    <row r="104" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="89" t="s">
-        <v>103</v>
-      </c>
-      <c r="B104" s="90"/>
-      <c r="C104" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="D104" s="91" t="s">
-        <v>104</v>
-      </c>
-      <c r="E104" s="90"/>
-      <c r="F104" s="90"/>
-      <c r="G104" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="H104" s="89" t="s">
-        <v>105</v>
-      </c>
-      <c r="I104" s="92"/>
-      <c r="J104" s="36" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="176" t="s">
-        <v>107</v>
-      </c>
-      <c r="B105" s="177"/>
-      <c r="C105" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="D105" s="178" t="s">
-        <v>108</v>
-      </c>
-      <c r="E105" s="179"/>
-      <c r="F105" s="180"/>
-      <c r="G105" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="H105" s="178" t="s">
-        <v>109</v>
-      </c>
-      <c r="I105" s="180"/>
-      <c r="J105" s="52" t="s">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="105" spans="1:10" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="57"/>
+      <c r="B105" s="58"/>
+      <c r="C105" s="52"/>
+      <c r="D105" s="59"/>
+      <c r="E105" s="60"/>
+      <c r="F105" s="61"/>
+      <c r="G105" s="53"/>
+      <c r="H105" s="59"/>
+      <c r="I105" s="61"/>
+      <c r="J105" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="123">
+    <mergeCell ref="A42:J54"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="F55:J55"/>
+    <mergeCell ref="A56:J56"/>
+    <mergeCell ref="A69:J86"/>
+    <mergeCell ref="A68:J68"/>
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="H87:I87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="A101:J101"/>
+    <mergeCell ref="A102:E102"/>
+    <mergeCell ref="F102:J102"/>
+    <mergeCell ref="A103:E103"/>
+    <mergeCell ref="F103:J103"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="H93:I93"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C16:E19"/>
+    <mergeCell ref="A8:E15"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="C29:J29"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A16:B19"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="F8:J11"/>
+    <mergeCell ref="A20:J20"/>
     <mergeCell ref="A105:B105"/>
     <mergeCell ref="D105:F105"/>
     <mergeCell ref="H105:I105"/>
@@ -9665,119 +9442,19 @@
     <mergeCell ref="H97:I97"/>
     <mergeCell ref="B95:F95"/>
     <mergeCell ref="H98:I98"/>
-    <mergeCell ref="C33:J33"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A16:B19"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="F8:J11"/>
-    <mergeCell ref="A20:J20"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="C28:J28"/>
-    <mergeCell ref="C29:J29"/>
-    <mergeCell ref="C30:J30"/>
-    <mergeCell ref="C31:J31"/>
-    <mergeCell ref="C32:J32"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:J5"/>
-    <mergeCell ref="A8:E15"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C16:E19"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="H94:I94"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="H88:I88"/>
     <mergeCell ref="A35:J35"/>
     <mergeCell ref="A36:J36"/>
+    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A34:J34"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="H93:I93"/>
-    <mergeCell ref="H95:I95"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="H94:I94"/>
-    <mergeCell ref="H88:I88"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D104:F104"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="A101:J101"/>
-    <mergeCell ref="A102:E102"/>
-    <mergeCell ref="F102:J102"/>
-    <mergeCell ref="A103:E103"/>
-    <mergeCell ref="F103:J103"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="H91:I91"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="A87:F87"/>
-    <mergeCell ref="H87:I87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="A42:J54"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="F55:J55"/>
-    <mergeCell ref="A56:J56"/>
-    <mergeCell ref="A69:J86"/>
-    <mergeCell ref="A68:J68"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="63" fitToHeight="6" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="41" max="1048575" man="1"/>
+    <brk id="41" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
@@ -9967,6 +9644,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <Please_x0020_note xmlns="f17bae92-5fa7-4270-afeb-ed962faafa52" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B342DF5A2DEFD64586E21F8B44CF3641" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="97e464cb99569ca8a9ef17fb08900847">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns3="f17bae92-5fa7-4270-afeb-ed962faafa52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6356073c4c24c81483cf02fe07ae928c" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -10105,39 +9800,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <Please_x0020_note xmlns="f17bae92-5fa7-4270-afeb-ed962faafa52" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544619E3-E001-4BD0-A0E9-1E9FD84B48E5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A06E1120-8501-409E-8BA8-1494F83C4851}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="f17bae92-5fa7-4270-afeb-ed962faafa52"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10160,9 +9826,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A06E1120-8501-409E-8BA8-1494F83C4851}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544619E3-E001-4BD0-A0E9-1E9FD84B48E5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="f17bae92-5fa7-4270-afeb-ed962faafa52"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
generación de formato ewo completada. Inicio de edición de ewo.
</commit_message>
<xml_diff>
--- a/DigiTools/Content/formats/FORMATO_EWO.XLSX
+++ b/DigiTools/Content/formats/FORMATO_EWO.XLSX
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UNILEVER_MTTO\Dropbox\HPC\MttoApp\DigiTools\DigiTools\Content\formats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unilever\Web\Mtto\DigiTools\DigiTools\Content\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5910945-BA99-49A9-8870-41D5A0F937D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC477D80-2EF2-482A-83D0-CCF8CF24495E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWO" sheetId="7" r:id="rId1"/>
@@ -81,18 +81,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
-  <si>
-    <t>NOK</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>No PM</t>
-  </si>
-  <si>
-    <t>No AM</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="111">
+  <si>
+    <t>EWO (Emergency Work Order)</t>
+  </si>
+  <si>
+    <t>EWO #</t>
+  </si>
+  <si>
+    <t>Area/Linea</t>
+  </si>
+  <si>
+    <t>Equipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha </t>
+  </si>
+  <si>
+    <t>Aviso #</t>
+  </si>
+  <si>
+    <t>Diligenciada por</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de Avería                                                                                                                                                                                                                                        </t>
+  </si>
+  <si>
+    <t>Turno</t>
+  </si>
+  <si>
+    <t>MesPack</t>
+  </si>
+  <si>
+    <t>Mespack H-360 FED 363.008</t>
+  </si>
+  <si>
+    <t>20/03/2019</t>
+  </si>
+  <si>
+    <t>1231</t>
+  </si>
+  <si>
+    <t>Jeison Perlaza</t>
+  </si>
+  <si>
+    <t>Mecánica</t>
   </si>
   <si>
     <t>Notificación Avería (Hora)</t>
@@ -133,6 +166,15 @@
     <t>Descripción gráfica de la falla [dibujos y/o planos]</t>
   </si>
   <si>
+    <t>Descripción de la avería. Si la reparación no se ha terminado en su totalidad, indique que necesita que se realice para terminarla:</t>
+  </si>
+  <si>
+    <t>una avería</t>
+  </si>
+  <si>
+    <t>( X  ) Cambio de Componente                    (    ) Ajuste</t>
+  </si>
+  <si>
     <t>Repuestos Utilizados</t>
   </si>
   <si>
@@ -148,107 +190,118 @@
     <t>Costo [COP]</t>
   </si>
   <si>
-    <t>1 - Por qué?</t>
-  </si>
-  <si>
-    <t>2 - Por qué?</t>
-  </si>
-  <si>
-    <t>3 - Por qué?</t>
-  </si>
-  <si>
-    <t>4 - Por qué?</t>
-  </si>
-  <si>
-    <t>5 - Por qué?</t>
-  </si>
-  <si>
-    <t>Dibujo / Diagrama / Foto del 5 Por qué</t>
-  </si>
-  <si>
-    <t>Ciclo de la causa raíz</t>
-  </si>
-  <si>
-    <t>¿Qué tipo de falla es? Diligencie las fechas de los mantenimiento planeados y selecciones la causa raiz basada en el gráfico de la bañera</t>
-  </si>
-  <si>
-    <t>Error Humano (instalación)</t>
-  </si>
-  <si>
-    <t>Falla de Diseño</t>
-  </si>
-  <si>
-    <t>Error Humano 
-(en operación)</t>
-  </si>
-  <si>
-    <t>Condiciones Básicas</t>
-  </si>
-  <si>
-    <t>Condiciones de Operación</t>
-  </si>
-  <si>
-    <t>Responsable</t>
-  </si>
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>Lista de Acciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Descripción de la avería. Si la reparación no se ha terminado en su totalidad, indique que necesita que se realice para terminarla:</t>
-  </si>
-  <si>
-    <t>(  ) Cambio de Componente                    (  ) Ajuste</t>
-  </si>
-  <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>2.</t>
-  </si>
-  <si>
-    <t>3.</t>
-  </si>
-  <si>
-    <t>4.</t>
-  </si>
-  <si>
-    <t>5.</t>
-  </si>
-  <si>
-    <t>6.</t>
-  </si>
-  <si>
-    <t>7.</t>
-  </si>
-  <si>
-    <t>8.</t>
-  </si>
-  <si>
-    <t>9.</t>
-  </si>
-  <si>
-    <t>10.</t>
-  </si>
-  <si>
-    <t>11.</t>
-  </si>
-  <si>
-    <t>12.</t>
-  </si>
-  <si>
-    <t>13.</t>
+    <t>uno mas</t>
+  </si>
+  <si>
+    <t>1 metro</t>
+  </si>
+  <si>
+    <t>$12333,0000</t>
+  </si>
+  <si>
+    <t>prueba 2 de mttr</t>
   </si>
   <si>
     <t>IDENTIFICACIÓN DE CAUSAS RAICES</t>
   </si>
   <si>
-    <t>EWO (Emergency Work Order)</t>
+    <r>
+      <t xml:space="preserve">IDENTIFICACION DE CAUSAS RAICES - 5G </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(llene esta seccion teniendo en cuenta el principio de los 5G)</t>
+    </r>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GEMBA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Ir al lugar donde se produce el problema)</t>
+    </r>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GEMBUTSU </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Ver los objetos, piezas y materiales reales que participan en el problema)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GENJITSU </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Confirmar una descripcion precisa y cuantificada del problema)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GENRI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Se refiere a la teoria. Principios mecanicos y fisicos que rigen la operación)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GENSOKU </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Siguen el estandar de operación.Las condiciones requeridas para operar sin causar problemas)</t>
+    </r>
+  </si>
+  <si>
+    <t>5W + 1H</t>
   </si>
   <si>
     <r>
@@ -338,6 +391,20 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Cual (WHICH)? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>¿Existe tendencia aleatoria o hay un patron? Existe relación con otras variables?</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">COMO (HOW) </t>
     </r>
     <r>
@@ -351,139 +418,72 @@
     </r>
   </si>
   <si>
+    <t>HOW + WHAT + WHERE + WHEN + WHICH + WHO = FENOMENO</t>
+  </si>
+  <si>
+    <t>df df df df df df</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">GENSOKU </t>
+      <t xml:space="preserve">5 ANÁLISIS POR QUÉ - POR QUÉ </t>
     </r>
     <r>
       <rPr>
-        <sz val="7"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Unilever DIN Offc Pro"/>
         <family val="2"/>
       </rPr>
-      <t>(Siguen el estandar de operación.Las condiciones requeridas para operar sin causar problemas)</t>
+      <t>(diligencie este campo si todas las causas reaices se encuentran OK)</t>
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">GENRI </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Se refiere a la teoria. Principios mecanicos y fisicos que rigen la operación)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">GENJITSU </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Confirmar una descripcion precisa y cuantificada del problema)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">GEMBUTSU </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Ver los objetos, piezas y materiales reales que participan en el problema)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">GEMBA </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Ir al lugar donde se produce el problema)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Cual (WHICH)? </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>¿Existe tendencia aleatoria o hay un patron? Existe relación con otras variables?</t>
-    </r>
-  </si>
-  <si>
-    <t>HOW + WHAT + WHERE + WHEN + WHICH + WHO = FENOMENO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo de Avería                                                                                                                                                                                                                                        </t>
-  </si>
-  <si>
-    <t>Diligenciada por</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha </t>
-  </si>
-  <si>
-    <t>Aviso #</t>
-  </si>
-  <si>
-    <t>Equipo</t>
-  </si>
-  <si>
-    <t>Area/Linea</t>
-  </si>
-  <si>
-    <t>Turno</t>
-  </si>
-  <si>
-    <t>EWO #</t>
-  </si>
-  <si>
-    <t>5W + 1H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Técnico(s) de Mantenimiento Involucrado(s)                                                                                                                                                                                                                    </t>
-  </si>
-  <si>
-    <t>Operario(s) Involucrado(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha                                                                                                                                                                                                                                                                                                </t>
-  </si>
-  <si>
-    <t>Ejecución Validada Por</t>
-  </si>
-  <si>
-    <t>Análisis Elaborado Por</t>
-  </si>
-  <si>
-    <t>Contramedidas Definidas Por</t>
-  </si>
-  <si>
-    <t>Tipo de Accion</t>
+    <t>1 - Por qué?</t>
+  </si>
+  <si>
+    <t>2 - Por qué?</t>
+  </si>
+  <si>
+    <t>3 - Por qué?</t>
+  </si>
+  <si>
+    <t>4 - Por qué?</t>
+  </si>
+  <si>
+    <t>5 - Por qué?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Dibujo / Diagrama / Foto del 5 Por qué</t>
+  </si>
+  <si>
+    <t>otra prueba</t>
+  </si>
+  <si>
+    <t>¿Qué tipo de falla es? Diligencie las fechas de los mantenimiento planeados y selecciones la causa raiz basada en el gráfico de la bañera</t>
+  </si>
+  <si>
+    <t>Fecha Ultimo Mtto</t>
+  </si>
+  <si>
+    <t>Fecha Proximo Mtto</t>
+  </si>
+  <si>
+    <t>Error Humano (instalación)</t>
+  </si>
+  <si>
+    <t>Condiciones de Operación</t>
+  </si>
+  <si>
+    <t>Falla de Diseño</t>
+  </si>
+  <si>
+    <t>Condiciones Básicas</t>
+  </si>
+  <si>
+    <t>No PM</t>
   </si>
   <si>
     <r>
@@ -501,10 +501,74 @@
     </r>
   </si>
   <si>
-    <t>Fecha Ultimo Mtto</t>
-  </si>
-  <si>
-    <t>Fecha Proximo Mtto</t>
+    <t>Error Humano 
+(en operación)</t>
+  </si>
+  <si>
+    <t>No AM</t>
+  </si>
+  <si>
+    <t>Ciclo de la causa raíz</t>
+  </si>
+  <si>
+    <t>Lista de Acciones</t>
+  </si>
+  <si>
+    <t>Tipo de Accion</t>
+  </si>
+  <si>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>prueba</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Angel Morales</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>8.</t>
+  </si>
+  <si>
+    <t>9.</t>
+  </si>
+  <si>
+    <t>10.</t>
+  </si>
+  <si>
+    <t>11.</t>
+  </si>
+  <si>
+    <t>12.</t>
+  </si>
+  <si>
+    <t>13.</t>
   </si>
   <si>
     <r>
@@ -569,32 +633,37 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">5 ANÁLISIS POR QUÉ - POR QUÉ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(diligencie este campo si todas las causas reaices se encuentran OK)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">IDENTIFICACION DE CAUSAS RAICES - 5G </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(llene esta seccion teniendo en cuenta el principio de los 5G)</t>
-    </r>
+    <t xml:space="preserve">Técnico(s) de Mantenimiento Involucrado(s)                                                                                                                                                                                                                    </t>
+  </si>
+  <si>
+    <t>Operario(s) Involucrado(s)</t>
+  </si>
+  <si>
+    <t>Édinson Rodríguez Urrea</t>
+  </si>
+  <si>
+    <t>Deisy Ipus</t>
+  </si>
+  <si>
+    <t>Análisis Elaborado Por</t>
+  </si>
+  <si>
+    <t>Contramedidas Definidas Por</t>
+  </si>
+  <si>
+    <t>Ejecución Validada Por</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha                                                                                                                                                                                                                                                                                                </t>
+  </si>
+  <si>
+    <t>Fabian Morante Olmos</t>
+  </si>
+  <si>
+    <t>Diego Fernando Murillo Arboleda</t>
+  </si>
+  <si>
+    <t>Carlos Andres Varela</t>
   </si>
 </sst>
 </file>
@@ -722,15 +791,22 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="7"/>
-      <color rgb="FF0000FF"/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Unilever DIN Offc Pro"/>
       <family val="2"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Unilever DIN Offc Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Unilever DIN Offc Pro"/>
       <family val="2"/>
@@ -743,15 +819,9 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="7"/>
+      <color rgb="FF0000FF"/>
       <name val="Unilever DIN Offc Pro"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -762,10 +832,9 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
-      <color theme="1"/>
-      <name val="Unilever DIN Offc Pro"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1285,569 +1354,569 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="190">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1881,7 +1950,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1897,7 +1966,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1967,9 +2036,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>631050</xdr:colOff>
+      <xdr:colOff>628650</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>447675</xdr:rowOff>
+      <xdr:rowOff>447676</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7394,6 +7463,159 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>571500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="image1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="image3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Elipse 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{386A29A4-D55C-4AED-926C-AC5703E538A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1069975" y="21590000"/>
+          <a:ext cx="1016000" cy="2540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:alpha val="11000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-CO" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7737,46 +7959,46 @@
     <col min="9" max="10" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="84"/>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="39.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="144" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="145"/>
+      <c r="E1" s="145"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="147"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="85" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="86"/>
+        <v>2</v>
+      </c>
+      <c r="C2" s="96" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="148"/>
       <c r="E2" s="31" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" s="87" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" s="88"/>
+        <v>6</v>
+      </c>
+      <c r="H2" s="149" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="150"/>
       <c r="J2" s="2" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -7785,17 +8007,33 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="30"/>
+    <row r="3" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25">
+        <v>2</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="162" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="163"/>
+      <c r="E3" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="162" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="163"/>
+      <c r="J3" s="30">
+        <v>3</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -7803,27 +8041,27 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="89" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="89" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="91" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="89" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="93" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="94"/>
+    <row r="4" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="151" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="151" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="153" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="153"/>
+      <c r="E4" s="153"/>
+      <c r="F4" s="154"/>
+      <c r="G4" s="154"/>
+      <c r="H4" s="151" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="155" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="156"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -7831,27 +8069,27 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="90"/>
-      <c r="B5" s="90"/>
+    <row r="5" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="152"/>
+      <c r="B5" s="152"/>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="90"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="96"/>
+        <v>24</v>
+      </c>
+      <c r="H5" s="152"/>
+      <c r="I5" s="157"/>
+      <c r="J5" s="158"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -7859,17 +8097,35 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="110"/>
+    <row r="6" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>43544.515972222202</v>
+      </c>
+      <c r="B6" s="15">
+        <v>43544.524305555598</v>
+      </c>
+      <c r="C6" s="16">
+        <v>12</v>
+      </c>
+      <c r="D6" s="16">
+        <v>9</v>
+      </c>
+      <c r="E6" s="16">
+        <v>2</v>
+      </c>
+      <c r="F6" s="16">
+        <v>1</v>
+      </c>
+      <c r="G6" s="16">
+        <v>3</v>
+      </c>
+      <c r="H6" s="15">
+        <v>43544.534722222197</v>
+      </c>
+      <c r="I6" s="168">
+        <v>27</v>
+      </c>
+      <c r="J6" s="169"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -7877,21 +8133,21 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="105" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="106"/>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="97" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="108"/>
-      <c r="H7" s="108"/>
-      <c r="I7" s="108"/>
-      <c r="J7" s="98"/>
+    <row r="7" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="164" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="165"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="166"/>
+      <c r="F7" s="119" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="167"/>
+      <c r="H7" s="167"/>
+      <c r="I7" s="167"/>
+      <c r="J7" s="120"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -7900,204 +8156,216 @@
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="131"/>
-      <c r="B8" s="132"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="111"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="112"/>
-      <c r="I8" s="112"/>
-      <c r="J8" s="113"/>
+      <c r="A8" s="140"/>
+      <c r="B8" s="141"/>
+      <c r="C8" s="141"/>
+      <c r="D8" s="141"/>
+      <c r="E8" s="142"/>
+      <c r="F8" s="170" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="171"/>
+      <c r="H8" s="171"/>
+      <c r="I8" s="171"/>
+      <c r="J8" s="172"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="99"/>
-      <c r="B9" s="100"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="129"/>
-      <c r="F9" s="114"/>
-      <c r="G9" s="115"/>
-      <c r="H9" s="115"/>
-      <c r="I9" s="115"/>
-      <c r="J9" s="116"/>
+      <c r="A9" s="143"/>
+      <c r="B9" s="136"/>
+      <c r="C9" s="136"/>
+      <c r="D9" s="136"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="173"/>
+      <c r="G9" s="174"/>
+      <c r="H9" s="174"/>
+      <c r="I9" s="174"/>
+      <c r="J9" s="175"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="99"/>
-      <c r="B10" s="100"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
-      <c r="E10" s="129"/>
-      <c r="F10" s="114"/>
-      <c r="G10" s="115"/>
-      <c r="H10" s="115"/>
-      <c r="I10" s="115"/>
-      <c r="J10" s="116"/>
+      <c r="A10" s="143"/>
+      <c r="B10" s="136"/>
+      <c r="C10" s="136"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="137"/>
+      <c r="F10" s="173"/>
+      <c r="G10" s="174"/>
+      <c r="H10" s="174"/>
+      <c r="I10" s="174"/>
+      <c r="J10" s="175"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="99"/>
-      <c r="B11" s="100"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="129"/>
-      <c r="F11" s="114"/>
-      <c r="G11" s="115"/>
-      <c r="H11" s="115"/>
-      <c r="I11" s="115"/>
-      <c r="J11" s="116"/>
+    <row r="11" spans="1:16" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="143"/>
+      <c r="B11" s="136"/>
+      <c r="C11" s="136"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="137"/>
+      <c r="F11" s="173"/>
+      <c r="G11" s="174"/>
+      <c r="H11" s="174"/>
+      <c r="I11" s="174"/>
+      <c r="J11" s="175"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="99"/>
-      <c r="B12" s="100"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="129"/>
-      <c r="F12" s="117" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="118"/>
-      <c r="H12" s="118"/>
-      <c r="I12" s="118"/>
-      <c r="J12" s="119"/>
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="143"/>
+      <c r="B12" s="136"/>
+      <c r="C12" s="136"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="137"/>
+      <c r="F12" s="121" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="122"/>
+      <c r="H12" s="122"/>
+      <c r="I12" s="122"/>
+      <c r="J12" s="123"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="99"/>
-      <c r="B13" s="100"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="129"/>
-      <c r="F13" s="120" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="121"/>
-      <c r="H13" s="121"/>
-      <c r="I13" s="121"/>
-      <c r="J13" s="122"/>
+      <c r="A13" s="143"/>
+      <c r="B13" s="136"/>
+      <c r="C13" s="136"/>
+      <c r="D13" s="136"/>
+      <c r="E13" s="137"/>
+      <c r="F13" s="124" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="125"/>
+      <c r="H13" s="125"/>
+      <c r="I13" s="125"/>
+      <c r="J13" s="126"/>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="99"/>
-      <c r="B14" s="100"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="129"/>
+      <c r="A14" s="143"/>
+      <c r="B14" s="136"/>
+      <c r="C14" s="136"/>
+      <c r="D14" s="136"/>
+      <c r="E14" s="137"/>
       <c r="F14" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="123" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="123"/>
+        <v>30</v>
+      </c>
+      <c r="G14" s="130" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="130"/>
       <c r="I14" s="34" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="J14" s="35" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="99"/>
-      <c r="B15" s="100"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="129"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="124"/>
-      <c r="H15" s="124"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
+      <c r="A15" s="143"/>
+      <c r="B15" s="136"/>
+      <c r="C15" s="136"/>
+      <c r="D15" s="136"/>
+      <c r="E15" s="137"/>
+      <c r="F15" s="17">
+        <v>233</v>
+      </c>
+      <c r="G15" s="131" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="131"/>
+      <c r="I15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="99"/>
-      <c r="B16" s="100"/>
-      <c r="C16" s="100"/>
-      <c r="D16" s="100"/>
-      <c r="E16" s="129"/>
+      <c r="A16" s="143" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="136"/>
+      <c r="C16" s="136"/>
+      <c r="D16" s="136"/>
+      <c r="E16" s="137"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="124"/>
-      <c r="H16" s="124"/>
+      <c r="G16" s="131"/>
+      <c r="H16" s="131"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="99"/>
-      <c r="B17" s="100"/>
-      <c r="C17" s="100"/>
-      <c r="D17" s="100"/>
-      <c r="E17" s="129"/>
+      <c r="A17" s="143"/>
+      <c r="B17" s="136"/>
+      <c r="C17" s="136"/>
+      <c r="D17" s="136"/>
+      <c r="E17" s="137"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="124"/>
-      <c r="H17" s="124"/>
+      <c r="G17" s="131"/>
+      <c r="H17" s="131"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="99"/>
-      <c r="B18" s="100"/>
-      <c r="C18" s="100"/>
-      <c r="D18" s="100"/>
-      <c r="E18" s="129"/>
+      <c r="A18" s="143"/>
+      <c r="B18" s="136"/>
+      <c r="C18" s="136"/>
+      <c r="D18" s="136"/>
+      <c r="E18" s="137"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="124"/>
-      <c r="H18" s="124"/>
+      <c r="G18" s="131"/>
+      <c r="H18" s="131"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="101"/>
-      <c r="B19" s="102"/>
-      <c r="C19" s="102"/>
-      <c r="D19" s="102"/>
-      <c r="E19" s="130"/>
+    <row r="19" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="161"/>
+      <c r="B19" s="138"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="139"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="125"/>
-      <c r="H19" s="125"/>
+      <c r="G19" s="132"/>
+      <c r="H19" s="132"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="56"/>
+    <row r="20" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="127" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="128"/>
+      <c r="C20" s="128"/>
+      <c r="D20" s="128"/>
+      <c r="E20" s="128"/>
+      <c r="F20" s="128"/>
+      <c r="G20" s="128"/>
+      <c r="H20" s="128"/>
+      <c r="I20" s="128"/>
+      <c r="J20" s="129"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="77"/>
+    <row r="21" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="185" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="186"/>
+      <c r="C21" s="186"/>
+      <c r="D21" s="186"/>
+      <c r="E21" s="186"/>
+      <c r="F21" s="186"/>
+      <c r="G21" s="186"/>
+      <c r="H21" s="186"/>
       <c r="I21" s="5" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -8106,18 +8374,22 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="97" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="98"/>
-      <c r="C22" s="126"/>
-      <c r="D22" s="127"/>
-      <c r="E22" s="127"/>
-      <c r="F22" s="127"/>
-      <c r="G22" s="127"/>
-      <c r="H22" s="128"/>
-      <c r="I22" s="8"/>
+    <row r="22" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="119" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="120"/>
+      <c r="C22" s="133" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="134"/>
+      <c r="E22" s="134"/>
+      <c r="F22" s="134"/>
+      <c r="G22" s="134"/>
+      <c r="H22" s="135"/>
+      <c r="I22" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="J22" s="8"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -8126,18 +8398,22 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="97" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="98"/>
-      <c r="C23" s="126"/>
-      <c r="D23" s="127"/>
-      <c r="E23" s="127"/>
-      <c r="F23" s="127"/>
-      <c r="G23" s="127"/>
-      <c r="H23" s="128"/>
-      <c r="I23" s="8"/>
+    <row r="23" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="119" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="120"/>
+      <c r="C23" s="133" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="134"/>
+      <c r="E23" s="134"/>
+      <c r="F23" s="134"/>
+      <c r="G23" s="134"/>
+      <c r="H23" s="135"/>
+      <c r="I23" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="J23" s="8"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -8146,18 +8422,22 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="97" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="98"/>
-      <c r="C24" s="126"/>
-      <c r="D24" s="127"/>
-      <c r="E24" s="127"/>
-      <c r="F24" s="127"/>
-      <c r="G24" s="127"/>
-      <c r="H24" s="128"/>
-      <c r="I24" s="8"/>
+    <row r="24" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="119" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="120"/>
+      <c r="C24" s="133" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="134"/>
+      <c r="E24" s="134"/>
+      <c r="F24" s="134"/>
+      <c r="G24" s="134"/>
+      <c r="H24" s="135"/>
+      <c r="I24" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="J24" s="8"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -8166,18 +8446,20 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="97" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="98"/>
-      <c r="C25" s="126"/>
-      <c r="D25" s="127"/>
-      <c r="E25" s="127"/>
-      <c r="F25" s="127"/>
-      <c r="G25" s="127"/>
-      <c r="H25" s="128"/>
-      <c r="I25" s="8"/>
+    <row r="25" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="119" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="120"/>
+      <c r="C25" s="133"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="134"/>
+      <c r="F25" s="134"/>
+      <c r="G25" s="134"/>
+      <c r="H25" s="135"/>
+      <c r="I25" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="J25" s="8"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -8186,18 +8468,20 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="97" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="98"/>
-      <c r="C26" s="126"/>
-      <c r="D26" s="127"/>
-      <c r="E26" s="127"/>
-      <c r="F26" s="127"/>
-      <c r="G26" s="127"/>
-      <c r="H26" s="128"/>
-      <c r="I26" s="9"/>
+    <row r="26" spans="1:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="119" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="120"/>
+      <c r="C26" s="133"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="134"/>
+      <c r="F26" s="134"/>
+      <c r="G26" s="134"/>
+      <c r="H26" s="135"/>
+      <c r="I26" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="J26" s="9"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -8206,19 +8490,19 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="54" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="56"/>
+    <row r="27" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="127" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="128"/>
+      <c r="C27" s="128"/>
+      <c r="D27" s="128"/>
+      <c r="E27" s="128"/>
+      <c r="F27" s="128"/>
+      <c r="G27" s="128"/>
+      <c r="H27" s="128"/>
+      <c r="I27" s="128"/>
+      <c r="J27" s="129"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -8226,19 +8510,21 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="97" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="98"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="72"/>
+    <row r="28" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="119" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="120"/>
+      <c r="C28" s="159" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="159"/>
+      <c r="E28" s="159"/>
+      <c r="F28" s="159"/>
+      <c r="G28" s="159"/>
+      <c r="H28" s="159"/>
+      <c r="I28" s="159"/>
+      <c r="J28" s="160"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -8246,19 +8532,21 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="97" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="98"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="71"/>
-      <c r="E29" s="71"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="71"/>
-      <c r="J29" s="72"/>
+    <row r="29" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="119" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="120"/>
+      <c r="C29" s="159" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="159"/>
+      <c r="E29" s="159"/>
+      <c r="F29" s="159"/>
+      <c r="G29" s="159"/>
+      <c r="H29" s="159"/>
+      <c r="I29" s="159"/>
+      <c r="J29" s="160"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -8266,19 +8554,21 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="97" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="98"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="72"/>
+    <row r="30" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="119" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="120"/>
+      <c r="C30" s="159" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="159"/>
+      <c r="E30" s="159"/>
+      <c r="F30" s="159"/>
+      <c r="G30" s="159"/>
+      <c r="H30" s="159"/>
+      <c r="I30" s="159"/>
+      <c r="J30" s="160"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -8286,19 +8576,21 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="97" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="98"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="71"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="71"/>
-      <c r="I31" s="71"/>
-      <c r="J31" s="72"/>
+    <row r="31" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="119" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="120"/>
+      <c r="C31" s="159" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="159"/>
+      <c r="E31" s="159"/>
+      <c r="F31" s="159"/>
+      <c r="G31" s="159"/>
+      <c r="H31" s="159"/>
+      <c r="I31" s="159"/>
+      <c r="J31" s="160"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -8306,19 +8598,21 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="97" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="98"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="71"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="71"/>
-      <c r="G32" s="71"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="71"/>
-      <c r="J32" s="72"/>
+    <row r="32" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="119" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="120"/>
+      <c r="C32" s="159" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="159"/>
+      <c r="E32" s="159"/>
+      <c r="F32" s="159"/>
+      <c r="G32" s="159"/>
+      <c r="H32" s="159"/>
+      <c r="I32" s="159"/>
+      <c r="J32" s="160"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -8326,19 +8620,21 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="97" t="s">
-        <v>58</v>
-      </c>
-      <c r="B33" s="98"/>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="71"/>
-      <c r="I33" s="71"/>
-      <c r="J33" s="72"/>
+    <row r="33" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="119" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="120"/>
+      <c r="C33" s="159" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="159"/>
+      <c r="E33" s="159"/>
+      <c r="F33" s="159"/>
+      <c r="G33" s="159"/>
+      <c r="H33" s="159"/>
+      <c r="I33" s="159"/>
+      <c r="J33" s="160"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -8346,19 +8642,19 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="78" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" s="79"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="79"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="79"/>
-      <c r="G34" s="79"/>
-      <c r="H34" s="79"/>
-      <c r="I34" s="79"/>
-      <c r="J34" s="80"/>
+    <row r="34" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="187" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="188"/>
+      <c r="C34" s="188"/>
+      <c r="D34" s="188"/>
+      <c r="E34" s="188"/>
+      <c r="F34" s="188"/>
+      <c r="G34" s="188"/>
+      <c r="H34" s="188"/>
+      <c r="I34" s="188"/>
+      <c r="J34" s="189"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -8366,17 +8662,19 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="70"/>
-      <c r="B35" s="71"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="71"/>
-      <c r="J35" s="72"/>
+    <row r="35" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="181" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="159"/>
+      <c r="C35" s="159"/>
+      <c r="D35" s="159"/>
+      <c r="E35" s="159"/>
+      <c r="F35" s="159"/>
+      <c r="G35" s="159"/>
+      <c r="H35" s="159"/>
+      <c r="I35" s="159"/>
+      <c r="J35" s="160"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -8384,283 +8682,285 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="73" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" s="74"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="74"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="75"/>
+    <row r="36" spans="1:16" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="182" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="183"/>
+      <c r="C36" s="183"/>
+      <c r="D36" s="183"/>
+      <c r="E36" s="183"/>
+      <c r="F36" s="183"/>
+      <c r="G36" s="183"/>
+      <c r="H36" s="183"/>
+      <c r="I36" s="183"/>
+      <c r="J36" s="184"/>
     </row>
     <row r="37" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="134" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="135"/>
-      <c r="C37" s="136" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="135"/>
-      <c r="E37" s="136" t="s">
-        <v>22</v>
-      </c>
-      <c r="F37" s="135"/>
-      <c r="G37" s="136" t="s">
-        <v>23</v>
-      </c>
-      <c r="H37" s="135"/>
-      <c r="I37" s="136" t="s">
-        <v>24</v>
-      </c>
-      <c r="J37" s="137"/>
+      <c r="A37" s="114" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="115"/>
+      <c r="C37" s="116" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="115"/>
+      <c r="E37" s="116" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" s="115"/>
+      <c r="G37" s="116" t="s">
+        <v>62</v>
+      </c>
+      <c r="H37" s="115"/>
+      <c r="I37" s="116" t="s">
+        <v>63</v>
+      </c>
+      <c r="J37" s="117"/>
     </row>
     <row r="38" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="138"/>
-      <c r="B38" s="62"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="62"/>
-      <c r="I38" s="62"/>
-      <c r="J38" s="144"/>
+      <c r="A38" s="118"/>
+      <c r="B38" s="106"/>
+      <c r="C38" s="106"/>
+      <c r="D38" s="106"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="106"/>
+      <c r="G38" s="106"/>
+      <c r="H38" s="106"/>
+      <c r="I38" s="106"/>
+      <c r="J38" s="108"/>
     </row>
     <row r="39" spans="1:16" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="138" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="62"/>
-      <c r="C39" s="62"/>
-      <c r="D39" s="62"/>
-      <c r="E39" s="62"/>
-      <c r="F39" s="62"/>
-      <c r="G39" s="62"/>
-      <c r="H39" s="62"/>
-      <c r="I39" s="62"/>
-      <c r="J39" s="145"/>
+      <c r="A39" s="118" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="106"/>
+      <c r="C39" s="106"/>
+      <c r="D39" s="106"/>
+      <c r="E39" s="106"/>
+      <c r="F39" s="106"/>
+      <c r="G39" s="106"/>
+      <c r="H39" s="106"/>
+      <c r="I39" s="106"/>
+      <c r="J39" s="109"/>
     </row>
     <row r="40" spans="1:16" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="139" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="140"/>
-      <c r="C40" s="62"/>
-      <c r="D40" s="143"/>
-      <c r="E40" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="F40" s="62"/>
-      <c r="G40" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="H40" s="62"/>
-      <c r="I40" s="146" t="s">
-        <v>36</v>
-      </c>
-      <c r="J40" s="145"/>
-    </row>
-    <row r="41" spans="1:16" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="141"/>
-      <c r="B41" s="142"/>
-      <c r="C41" s="142"/>
-      <c r="D41" s="142"/>
-      <c r="E41" s="63"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="63"/>
-      <c r="I41" s="147"/>
-      <c r="J41" s="148"/>
+      <c r="A40" s="102" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="103"/>
+      <c r="C40" s="106"/>
+      <c r="D40" s="107"/>
+      <c r="E40" s="106" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" s="106"/>
+      <c r="G40" s="106" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" s="106"/>
+      <c r="I40" s="110" t="s">
+        <v>64</v>
+      </c>
+      <c r="J40" s="109"/>
+    </row>
+    <row r="41" spans="1:16" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="104"/>
+      <c r="B41" s="105"/>
+      <c r="C41" s="105"/>
+      <c r="D41" s="105"/>
+      <c r="E41" s="113"/>
+      <c r="F41" s="113"/>
+      <c r="G41" s="113"/>
+      <c r="H41" s="113"/>
+      <c r="I41" s="111"/>
+      <c r="J41" s="112"/>
     </row>
     <row r="42" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="163" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" s="164"/>
-      <c r="C42" s="164"/>
-      <c r="D42" s="164"/>
-      <c r="E42" s="164"/>
-      <c r="F42" s="164"/>
-      <c r="G42" s="164"/>
-      <c r="H42" s="164"/>
-      <c r="I42" s="164"/>
-      <c r="J42" s="165"/>
+      <c r="A42" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="55"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="55"/>
+      <c r="F42" s="55"/>
+      <c r="G42" s="55"/>
+      <c r="H42" s="55"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="56"/>
     </row>
     <row r="43" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="166"/>
-      <c r="B43" s="167"/>
-      <c r="C43" s="167"/>
-      <c r="D43" s="167"/>
-      <c r="E43" s="167"/>
-      <c r="F43" s="167"/>
-      <c r="G43" s="167"/>
-      <c r="H43" s="167"/>
-      <c r="I43" s="167"/>
-      <c r="J43" s="168"/>
+      <c r="A43" s="57"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="59"/>
     </row>
     <row r="44" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="166"/>
-      <c r="B44" s="167"/>
-      <c r="C44" s="167"/>
-      <c r="D44" s="167"/>
-      <c r="E44" s="167"/>
-      <c r="F44" s="167"/>
-      <c r="G44" s="167"/>
-      <c r="H44" s="167"/>
-      <c r="I44" s="167"/>
-      <c r="J44" s="168"/>
+      <c r="A44" s="57"/>
+      <c r="B44" s="58"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="58"/>
+      <c r="E44" s="58"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="58"/>
+      <c r="J44" s="59"/>
     </row>
     <row r="45" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="166"/>
-      <c r="B45" s="167"/>
-      <c r="C45" s="167"/>
-      <c r="D45" s="167"/>
-      <c r="E45" s="167"/>
-      <c r="F45" s="167"/>
-      <c r="G45" s="167"/>
-      <c r="H45" s="167"/>
-      <c r="I45" s="167"/>
-      <c r="J45" s="168"/>
+      <c r="A45" s="57"/>
+      <c r="B45" s="58"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="58"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="58"/>
+      <c r="J45" s="59"/>
     </row>
     <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="166"/>
-      <c r="B46" s="167"/>
-      <c r="C46" s="167"/>
-      <c r="D46" s="167"/>
-      <c r="E46" s="167"/>
-      <c r="F46" s="167"/>
-      <c r="G46" s="167"/>
-      <c r="H46" s="167"/>
-      <c r="I46" s="167"/>
-      <c r="J46" s="168"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="58"/>
+      <c r="J46" s="59"/>
     </row>
     <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="166"/>
-      <c r="B47" s="167"/>
-      <c r="C47" s="167"/>
-      <c r="D47" s="167"/>
-      <c r="E47" s="167"/>
-      <c r="F47" s="167"/>
-      <c r="G47" s="167"/>
-      <c r="H47" s="167"/>
-      <c r="I47" s="167"/>
-      <c r="J47" s="168"/>
+      <c r="A47" s="57"/>
+      <c r="B47" s="58"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="58"/>
+      <c r="I47" s="58"/>
+      <c r="J47" s="59"/>
     </row>
     <row r="48" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="166"/>
-      <c r="B48" s="167"/>
-      <c r="C48" s="167"/>
-      <c r="D48" s="167"/>
-      <c r="E48" s="167"/>
-      <c r="F48" s="167"/>
-      <c r="G48" s="167"/>
-      <c r="H48" s="167"/>
-      <c r="I48" s="167"/>
-      <c r="J48" s="168"/>
+      <c r="A48" s="57"/>
+      <c r="B48" s="58"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
+      <c r="I48" s="58"/>
+      <c r="J48" s="59"/>
     </row>
     <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="166"/>
-      <c r="B49" s="167"/>
-      <c r="C49" s="167"/>
-      <c r="D49" s="167"/>
-      <c r="E49" s="167"/>
-      <c r="F49" s="167"/>
-      <c r="G49" s="167"/>
-      <c r="H49" s="167"/>
-      <c r="I49" s="167"/>
-      <c r="J49" s="168"/>
+      <c r="A49" s="57"/>
+      <c r="B49" s="58"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="58"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="58"/>
+      <c r="I49" s="58"/>
+      <c r="J49" s="59"/>
     </row>
     <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="166"/>
-      <c r="B50" s="167"/>
-      <c r="C50" s="167"/>
-      <c r="D50" s="167"/>
-      <c r="E50" s="167"/>
-      <c r="F50" s="167"/>
-      <c r="G50" s="167"/>
-      <c r="H50" s="167"/>
-      <c r="I50" s="167"/>
-      <c r="J50" s="168"/>
+      <c r="A50" s="57"/>
+      <c r="B50" s="58"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
+      <c r="E50" s="58"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="58"/>
+      <c r="I50" s="58"/>
+      <c r="J50" s="59"/>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="166"/>
-      <c r="B51" s="167"/>
-      <c r="C51" s="167"/>
-      <c r="D51" s="167"/>
-      <c r="E51" s="167"/>
-      <c r="F51" s="167"/>
-      <c r="G51" s="167"/>
-      <c r="H51" s="167"/>
-      <c r="I51" s="167"/>
-      <c r="J51" s="168"/>
+      <c r="A51" s="57"/>
+      <c r="B51" s="58"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="58"/>
+      <c r="E51" s="58"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="58"/>
+      <c r="H51" s="58"/>
+      <c r="I51" s="58"/>
+      <c r="J51" s="59"/>
     </row>
     <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="166"/>
-      <c r="B52" s="167"/>
-      <c r="C52" s="167"/>
-      <c r="D52" s="167"/>
-      <c r="E52" s="167"/>
-      <c r="F52" s="167"/>
-      <c r="G52" s="167"/>
-      <c r="H52" s="167"/>
-      <c r="I52" s="167"/>
-      <c r="J52" s="168"/>
+      <c r="A52" s="57"/>
+      <c r="B52" s="58"/>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
+      <c r="E52" s="58"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="58"/>
+      <c r="I52" s="58"/>
+      <c r="J52" s="59"/>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="166"/>
-      <c r="B53" s="167"/>
-      <c r="C53" s="167"/>
-      <c r="D53" s="167"/>
-      <c r="E53" s="167"/>
-      <c r="F53" s="167"/>
-      <c r="G53" s="167"/>
-      <c r="H53" s="167"/>
-      <c r="I53" s="167"/>
-      <c r="J53" s="168"/>
+      <c r="A53" s="57"/>
+      <c r="B53" s="58"/>
+      <c r="C53" s="58"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="58"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="58"/>
+      <c r="I53" s="58"/>
+      <c r="J53" s="59"/>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="166"/>
-      <c r="B54" s="167"/>
-      <c r="C54" s="167"/>
-      <c r="D54" s="167"/>
-      <c r="E54" s="167"/>
-      <c r="F54" s="167"/>
-      <c r="G54" s="167"/>
-      <c r="H54" s="167"/>
-      <c r="I54" s="167"/>
-      <c r="J54" s="168"/>
+      <c r="A54" s="57"/>
+      <c r="B54" s="58"/>
+      <c r="C54" s="58"/>
+      <c r="D54" s="58"/>
+      <c r="E54" s="58"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="I54" s="58"/>
+      <c r="J54" s="59"/>
     </row>
     <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="169"/>
-      <c r="B55" s="169"/>
-      <c r="C55" s="169"/>
-      <c r="D55" s="169"/>
-      <c r="E55" s="169"/>
-      <c r="F55" s="169"/>
-      <c r="G55" s="169"/>
-      <c r="H55" s="169"/>
-      <c r="I55" s="169"/>
-      <c r="J55" s="169"/>
+      <c r="A55" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="60"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="60"/>
+      <c r="F55" s="60"/>
+      <c r="G55" s="60"/>
+      <c r="H55" s="60"/>
+      <c r="I55" s="60"/>
+      <c r="J55" s="60"/>
     </row>
     <row r="56" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="170" t="s">
-        <v>27</v>
-      </c>
-      <c r="B56" s="171"/>
-      <c r="C56" s="171"/>
-      <c r="D56" s="171"/>
-      <c r="E56" s="171"/>
-      <c r="F56" s="171"/>
-      <c r="G56" s="171"/>
-      <c r="H56" s="171"/>
-      <c r="I56" s="171"/>
-      <c r="J56" s="172"/>
+      <c r="A56" s="61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="62"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="62"/>
+      <c r="E56" s="62"/>
+      <c r="F56" s="62"/>
+      <c r="G56" s="62"/>
+      <c r="H56" s="62"/>
+      <c r="I56" s="62"/>
+      <c r="J56" s="63"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="18"/>
@@ -8737,7 +9037,7 @@
     <row r="63" spans="1:10" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A63" s="18"/>
       <c r="B63" s="43" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
@@ -8745,24 +9045,28 @@
       <c r="F63" s="19"/>
       <c r="G63" s="44"/>
       <c r="H63" s="50" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="I63" s="19"/>
       <c r="J63" s="20"/>
     </row>
     <row r="64" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="47"/>
-      <c r="B64" s="48"/>
+      <c r="B64" s="48" t="s">
+        <v>11</v>
+      </c>
       <c r="C64" s="49" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="D64" s="42"/>
       <c r="E64" s="21" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="F64" s="19"/>
       <c r="G64" s="45"/>
-      <c r="H64" s="48"/>
+      <c r="H64" s="48" t="s">
+        <v>11</v>
+      </c>
       <c r="I64" s="51"/>
       <c r="J64" s="20"/>
     </row>
@@ -8770,15 +9074,15 @@
       <c r="A65" s="18"/>
       <c r="B65" s="46"/>
       <c r="C65" s="22" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="D65" s="42"/>
       <c r="E65" s="21" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="F65" s="19"/>
       <c r="G65" s="23" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="H65" s="46"/>
       <c r="I65" s="19"/>
@@ -8788,15 +9092,15 @@
       <c r="A66" s="18"/>
       <c r="B66" s="19"/>
       <c r="C66" s="22" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D66" s="43"/>
       <c r="E66" s="21" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="F66" s="19"/>
       <c r="G66" s="23" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="H66" s="19"/>
       <c r="I66" s="19"/>
@@ -8814,572 +9118,588 @@
       <c r="I67" s="19"/>
       <c r="J67" s="20"/>
     </row>
-    <row r="68" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="182" t="s">
-        <v>26</v>
-      </c>
-      <c r="B68" s="183"/>
-      <c r="C68" s="183"/>
-      <c r="D68" s="183"/>
-      <c r="E68" s="183"/>
-      <c r="F68" s="183"/>
-      <c r="G68" s="183"/>
-      <c r="H68" s="183"/>
-      <c r="I68" s="183"/>
-      <c r="J68" s="184"/>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="73" t="s">
+        <v>78</v>
+      </c>
+      <c r="B68" s="74"/>
+      <c r="C68" s="74"/>
+      <c r="D68" s="74"/>
+      <c r="E68" s="74"/>
+      <c r="F68" s="74"/>
+      <c r="G68" s="74"/>
+      <c r="H68" s="74"/>
+      <c r="I68" s="74"/>
+      <c r="J68" s="75"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="173"/>
-      <c r="B69" s="174"/>
-      <c r="C69" s="174"/>
-      <c r="D69" s="174"/>
-      <c r="E69" s="174"/>
-      <c r="F69" s="174"/>
-      <c r="G69" s="174"/>
-      <c r="H69" s="174"/>
-      <c r="I69" s="174"/>
-      <c r="J69" s="175"/>
+      <c r="A69" s="64"/>
+      <c r="B69" s="65"/>
+      <c r="C69" s="65"/>
+      <c r="D69" s="65"/>
+      <c r="E69" s="65"/>
+      <c r="F69" s="65"/>
+      <c r="G69" s="65"/>
+      <c r="H69" s="65"/>
+      <c r="I69" s="65"/>
+      <c r="J69" s="66"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="176"/>
-      <c r="B70" s="177"/>
-      <c r="C70" s="177"/>
-      <c r="D70" s="177"/>
-      <c r="E70" s="177"/>
-      <c r="F70" s="177"/>
-      <c r="G70" s="177"/>
-      <c r="H70" s="177"/>
-      <c r="I70" s="177"/>
-      <c r="J70" s="178"/>
+      <c r="A70" s="67"/>
+      <c r="B70" s="68"/>
+      <c r="C70" s="68"/>
+      <c r="D70" s="68"/>
+      <c r="E70" s="68"/>
+      <c r="F70" s="68"/>
+      <c r="G70" s="68"/>
+      <c r="H70" s="68"/>
+      <c r="I70" s="68"/>
+      <c r="J70" s="69"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="176"/>
-      <c r="B71" s="177"/>
-      <c r="C71" s="177"/>
-      <c r="D71" s="177"/>
-      <c r="E71" s="177"/>
-      <c r="F71" s="177"/>
-      <c r="G71" s="177"/>
-      <c r="H71" s="177"/>
-      <c r="I71" s="177"/>
-      <c r="J71" s="178"/>
+      <c r="A71" s="67"/>
+      <c r="B71" s="68"/>
+      <c r="C71" s="68"/>
+      <c r="D71" s="68"/>
+      <c r="E71" s="68"/>
+      <c r="F71" s="68"/>
+      <c r="G71" s="68"/>
+      <c r="H71" s="68"/>
+      <c r="I71" s="68"/>
+      <c r="J71" s="69"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="176"/>
-      <c r="B72" s="177"/>
-      <c r="C72" s="177"/>
-      <c r="D72" s="177"/>
-      <c r="E72" s="177"/>
-      <c r="F72" s="177"/>
-      <c r="G72" s="177"/>
-      <c r="H72" s="177"/>
-      <c r="I72" s="177"/>
-      <c r="J72" s="178"/>
+      <c r="A72" s="67"/>
+      <c r="B72" s="68"/>
+      <c r="C72" s="68"/>
+      <c r="D72" s="68"/>
+      <c r="E72" s="68"/>
+      <c r="F72" s="68"/>
+      <c r="G72" s="68"/>
+      <c r="H72" s="68"/>
+      <c r="I72" s="68"/>
+      <c r="J72" s="69"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="176"/>
-      <c r="B73" s="177"/>
-      <c r="C73" s="177"/>
-      <c r="D73" s="177"/>
-      <c r="E73" s="177"/>
-      <c r="F73" s="177"/>
-      <c r="G73" s="177"/>
-      <c r="H73" s="177"/>
-      <c r="I73" s="177"/>
-      <c r="J73" s="178"/>
+      <c r="A73" s="67"/>
+      <c r="B73" s="68"/>
+      <c r="C73" s="68"/>
+      <c r="D73" s="68"/>
+      <c r="E73" s="68"/>
+      <c r="F73" s="68"/>
+      <c r="G73" s="68"/>
+      <c r="H73" s="68"/>
+      <c r="I73" s="68"/>
+      <c r="J73" s="69"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="176"/>
-      <c r="B74" s="177"/>
-      <c r="C74" s="177"/>
-      <c r="D74" s="177"/>
-      <c r="E74" s="177"/>
-      <c r="F74" s="177"/>
-      <c r="G74" s="177"/>
-      <c r="H74" s="177"/>
-      <c r="I74" s="177"/>
-      <c r="J74" s="178"/>
+      <c r="A74" s="67"/>
+      <c r="B74" s="68"/>
+      <c r="C74" s="68"/>
+      <c r="D74" s="68"/>
+      <c r="E74" s="68"/>
+      <c r="F74" s="68"/>
+      <c r="G74" s="68"/>
+      <c r="H74" s="68"/>
+      <c r="I74" s="68"/>
+      <c r="J74" s="69"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="176"/>
-      <c r="B75" s="177"/>
-      <c r="C75" s="177"/>
-      <c r="D75" s="177"/>
-      <c r="E75" s="177"/>
-      <c r="F75" s="177"/>
-      <c r="G75" s="177"/>
-      <c r="H75" s="177"/>
-      <c r="I75" s="177"/>
-      <c r="J75" s="178"/>
+      <c r="A75" s="67"/>
+      <c r="B75" s="68"/>
+      <c r="C75" s="68"/>
+      <c r="D75" s="68"/>
+      <c r="E75" s="68"/>
+      <c r="F75" s="68"/>
+      <c r="G75" s="68"/>
+      <c r="H75" s="68"/>
+      <c r="I75" s="68"/>
+      <c r="J75" s="69"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="176"/>
-      <c r="B76" s="177"/>
-      <c r="C76" s="177"/>
-      <c r="D76" s="177"/>
-      <c r="E76" s="177"/>
-      <c r="F76" s="177"/>
-      <c r="G76" s="177"/>
-      <c r="H76" s="177"/>
-      <c r="I76" s="177"/>
-      <c r="J76" s="178"/>
+      <c r="A76" s="67"/>
+      <c r="B76" s="68"/>
+      <c r="C76" s="68"/>
+      <c r="D76" s="68"/>
+      <c r="E76" s="68"/>
+      <c r="F76" s="68"/>
+      <c r="G76" s="68"/>
+      <c r="H76" s="68"/>
+      <c r="I76" s="68"/>
+      <c r="J76" s="69"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="176"/>
-      <c r="B77" s="177"/>
-      <c r="C77" s="177"/>
-      <c r="D77" s="177"/>
-      <c r="E77" s="177"/>
-      <c r="F77" s="177"/>
-      <c r="G77" s="177"/>
-      <c r="H77" s="177"/>
-      <c r="I77" s="177"/>
-      <c r="J77" s="178"/>
+      <c r="A77" s="67"/>
+      <c r="B77" s="68"/>
+      <c r="C77" s="68"/>
+      <c r="D77" s="68"/>
+      <c r="E77" s="68"/>
+      <c r="F77" s="68"/>
+      <c r="G77" s="68"/>
+      <c r="H77" s="68"/>
+      <c r="I77" s="68"/>
+      <c r="J77" s="69"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="176"/>
-      <c r="B78" s="177"/>
-      <c r="C78" s="177"/>
-      <c r="D78" s="177"/>
-      <c r="E78" s="177"/>
-      <c r="F78" s="177"/>
-      <c r="G78" s="177"/>
-      <c r="H78" s="177"/>
-      <c r="I78" s="177"/>
-      <c r="J78" s="178"/>
+      <c r="A78" s="67"/>
+      <c r="B78" s="68"/>
+      <c r="C78" s="68"/>
+      <c r="D78" s="68"/>
+      <c r="E78" s="68"/>
+      <c r="F78" s="68"/>
+      <c r="G78" s="68"/>
+      <c r="H78" s="68"/>
+      <c r="I78" s="68"/>
+      <c r="J78" s="69"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="176"/>
-      <c r="B79" s="177"/>
-      <c r="C79" s="177"/>
-      <c r="D79" s="177"/>
-      <c r="E79" s="177"/>
-      <c r="F79" s="177"/>
-      <c r="G79" s="177"/>
-      <c r="H79" s="177"/>
-      <c r="I79" s="177"/>
-      <c r="J79" s="178"/>
+      <c r="A79" s="67"/>
+      <c r="B79" s="68"/>
+      <c r="C79" s="68"/>
+      <c r="D79" s="68"/>
+      <c r="E79" s="68"/>
+      <c r="F79" s="68"/>
+      <c r="G79" s="68"/>
+      <c r="H79" s="68"/>
+      <c r="I79" s="68"/>
+      <c r="J79" s="69"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="176"/>
-      <c r="B80" s="177"/>
-      <c r="C80" s="177"/>
-      <c r="D80" s="177"/>
-      <c r="E80" s="177"/>
-      <c r="F80" s="177"/>
-      <c r="G80" s="177"/>
-      <c r="H80" s="177"/>
-      <c r="I80" s="177"/>
-      <c r="J80" s="178"/>
+      <c r="A80" s="67"/>
+      <c r="B80" s="68"/>
+      <c r="C80" s="68"/>
+      <c r="D80" s="68"/>
+      <c r="E80" s="68"/>
+      <c r="F80" s="68"/>
+      <c r="G80" s="68"/>
+      <c r="H80" s="68"/>
+      <c r="I80" s="68"/>
+      <c r="J80" s="69"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="176"/>
-      <c r="B81" s="177"/>
-      <c r="C81" s="177"/>
-      <c r="D81" s="177"/>
-      <c r="E81" s="177"/>
-      <c r="F81" s="177"/>
-      <c r="G81" s="177"/>
-      <c r="H81" s="177"/>
-      <c r="I81" s="177"/>
-      <c r="J81" s="178"/>
+      <c r="A81" s="67"/>
+      <c r="B81" s="68"/>
+      <c r="C81" s="68"/>
+      <c r="D81" s="68"/>
+      <c r="E81" s="68"/>
+      <c r="F81" s="68"/>
+      <c r="G81" s="68"/>
+      <c r="H81" s="68"/>
+      <c r="I81" s="68"/>
+      <c r="J81" s="69"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="176"/>
-      <c r="B82" s="177"/>
-      <c r="C82" s="177"/>
-      <c r="D82" s="177"/>
-      <c r="E82" s="177"/>
-      <c r="F82" s="177"/>
-      <c r="G82" s="177"/>
-      <c r="H82" s="177"/>
-      <c r="I82" s="177"/>
-      <c r="J82" s="178"/>
+      <c r="A82" s="67"/>
+      <c r="B82" s="68"/>
+      <c r="C82" s="68"/>
+      <c r="D82" s="68"/>
+      <c r="E82" s="68"/>
+      <c r="F82" s="68"/>
+      <c r="G82" s="68"/>
+      <c r="H82" s="68"/>
+      <c r="I82" s="68"/>
+      <c r="J82" s="69"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="176"/>
-      <c r="B83" s="177"/>
-      <c r="C83" s="177"/>
-      <c r="D83" s="177"/>
-      <c r="E83" s="177"/>
-      <c r="F83" s="177"/>
-      <c r="G83" s="177"/>
-      <c r="H83" s="177"/>
-      <c r="I83" s="177"/>
-      <c r="J83" s="178"/>
+      <c r="A83" s="67"/>
+      <c r="B83" s="68"/>
+      <c r="C83" s="68"/>
+      <c r="D83" s="68"/>
+      <c r="E83" s="68"/>
+      <c r="F83" s="68"/>
+      <c r="G83" s="68"/>
+      <c r="H83" s="68"/>
+      <c r="I83" s="68"/>
+      <c r="J83" s="69"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="176"/>
-      <c r="B84" s="177"/>
-      <c r="C84" s="177"/>
-      <c r="D84" s="177"/>
-      <c r="E84" s="177"/>
-      <c r="F84" s="177"/>
-      <c r="G84" s="177"/>
-      <c r="H84" s="177"/>
-      <c r="I84" s="177"/>
-      <c r="J84" s="178"/>
+      <c r="A84" s="67"/>
+      <c r="B84" s="68"/>
+      <c r="C84" s="68"/>
+      <c r="D84" s="68"/>
+      <c r="E84" s="68"/>
+      <c r="F84" s="68"/>
+      <c r="G84" s="68"/>
+      <c r="H84" s="68"/>
+      <c r="I84" s="68"/>
+      <c r="J84" s="69"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="176"/>
-      <c r="B85" s="177"/>
-      <c r="C85" s="177"/>
-      <c r="D85" s="177"/>
-      <c r="E85" s="177"/>
-      <c r="F85" s="177"/>
-      <c r="G85" s="177"/>
-      <c r="H85" s="177"/>
-      <c r="I85" s="177"/>
-      <c r="J85" s="178"/>
-    </row>
-    <row r="86" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="179"/>
-      <c r="B86" s="180"/>
-      <c r="C86" s="180"/>
-      <c r="D86" s="180"/>
-      <c r="E86" s="180"/>
-      <c r="F86" s="180"/>
-      <c r="G86" s="180"/>
-      <c r="H86" s="180"/>
-      <c r="I86" s="180"/>
-      <c r="J86" s="181"/>
-    </row>
-    <row r="87" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="185" t="s">
-        <v>35</v>
-      </c>
-      <c r="B87" s="186"/>
-      <c r="C87" s="186"/>
-      <c r="D87" s="186"/>
-      <c r="E87" s="186"/>
-      <c r="F87" s="187"/>
+      <c r="A85" s="67"/>
+      <c r="B85" s="68"/>
+      <c r="C85" s="68"/>
+      <c r="D85" s="68"/>
+      <c r="E85" s="68"/>
+      <c r="F85" s="68"/>
+      <c r="G85" s="68"/>
+      <c r="H85" s="68"/>
+      <c r="I85" s="68"/>
+      <c r="J85" s="69"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="70"/>
+      <c r="B86" s="71"/>
+      <c r="C86" s="71"/>
+      <c r="D86" s="71"/>
+      <c r="E86" s="71"/>
+      <c r="F86" s="71"/>
+      <c r="G86" s="71"/>
+      <c r="H86" s="71"/>
+      <c r="I86" s="71"/>
+      <c r="J86" s="72"/>
+    </row>
+    <row r="87" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="76" t="s">
+        <v>79</v>
+      </c>
+      <c r="B87" s="77"/>
+      <c r="C87" s="77"/>
+      <c r="D87" s="77"/>
+      <c r="E87" s="77"/>
+      <c r="F87" s="78"/>
       <c r="G87" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="H87" s="76" t="s">
         <v>81</v>
       </c>
-      <c r="H87" s="185" t="s">
-        <v>33</v>
-      </c>
-      <c r="I87" s="187"/>
+      <c r="I87" s="78"/>
       <c r="J87" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A88" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B88" s="188"/>
-      <c r="C88" s="188"/>
-      <c r="D88" s="188"/>
-      <c r="E88" s="188"/>
-      <c r="F88" s="189"/>
-      <c r="G88" s="12"/>
-      <c r="H88" s="68"/>
-      <c r="I88" s="69"/>
-      <c r="J88" s="10"/>
-    </row>
-    <row r="89" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="B88" s="79" t="s">
+        <v>84</v>
+      </c>
+      <c r="C88" s="79"/>
+      <c r="D88" s="79"/>
+      <c r="E88" s="79"/>
+      <c r="F88" s="80"/>
+      <c r="G88" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="H88" s="85" t="s">
+        <v>86</v>
+      </c>
+      <c r="I88" s="86"/>
+      <c r="J88" s="10">
+        <v>43544</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A89" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B89" s="149"/>
-      <c r="C89" s="149"/>
-      <c r="D89" s="149"/>
-      <c r="E89" s="149"/>
-      <c r="F89" s="150"/>
+        <v>87</v>
+      </c>
+      <c r="B89" s="81"/>
+      <c r="C89" s="81"/>
+      <c r="D89" s="81"/>
+      <c r="E89" s="81"/>
+      <c r="F89" s="82"/>
       <c r="G89" s="12"/>
-      <c r="H89" s="68"/>
-      <c r="I89" s="69"/>
+      <c r="H89" s="85"/>
+      <c r="I89" s="86"/>
       <c r="J89" s="10"/>
     </row>
-    <row r="90" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A90" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B90" s="149"/>
-      <c r="C90" s="149"/>
-      <c r="D90" s="149"/>
-      <c r="E90" s="149"/>
-      <c r="F90" s="150"/>
+        <v>88</v>
+      </c>
+      <c r="B90" s="81"/>
+      <c r="C90" s="81"/>
+      <c r="D90" s="81"/>
+      <c r="E90" s="81"/>
+      <c r="F90" s="82"/>
       <c r="G90" s="12"/>
-      <c r="H90" s="68"/>
-      <c r="I90" s="69"/>
+      <c r="H90" s="85"/>
+      <c r="I90" s="86"/>
       <c r="J90" s="10"/>
     </row>
-    <row r="91" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A91" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B91" s="64"/>
-      <c r="C91" s="64"/>
-      <c r="D91" s="64"/>
-      <c r="E91" s="64"/>
-      <c r="F91" s="65"/>
+        <v>89</v>
+      </c>
+      <c r="B91" s="83"/>
+      <c r="C91" s="83"/>
+      <c r="D91" s="83"/>
+      <c r="E91" s="83"/>
+      <c r="F91" s="84"/>
       <c r="G91" s="12"/>
-      <c r="H91" s="66"/>
-      <c r="I91" s="67"/>
+      <c r="H91" s="87"/>
+      <c r="I91" s="88"/>
       <c r="J91" s="7"/>
     </row>
-    <row r="92" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A92" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B92" s="64"/>
-      <c r="C92" s="64"/>
-      <c r="D92" s="64"/>
-      <c r="E92" s="64"/>
-      <c r="F92" s="65"/>
+        <v>90</v>
+      </c>
+      <c r="B92" s="83"/>
+      <c r="C92" s="83"/>
+      <c r="D92" s="83"/>
+      <c r="E92" s="83"/>
+      <c r="F92" s="84"/>
       <c r="G92" s="12"/>
-      <c r="H92" s="66"/>
-      <c r="I92" s="67"/>
+      <c r="H92" s="87"/>
+      <c r="I92" s="88"/>
       <c r="J92" s="7"/>
     </row>
-    <row r="93" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A93" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B93" s="64"/>
-      <c r="C93" s="64"/>
-      <c r="D93" s="64"/>
-      <c r="E93" s="64"/>
-      <c r="F93" s="65"/>
+        <v>91</v>
+      </c>
+      <c r="B93" s="83"/>
+      <c r="C93" s="83"/>
+      <c r="D93" s="83"/>
+      <c r="E93" s="83"/>
+      <c r="F93" s="84"/>
       <c r="G93" s="12"/>
-      <c r="H93" s="66"/>
-      <c r="I93" s="67"/>
+      <c r="H93" s="87"/>
+      <c r="I93" s="88"/>
       <c r="J93" s="7"/>
     </row>
-    <row r="94" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A94" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B94" s="64"/>
-      <c r="C94" s="64"/>
-      <c r="D94" s="64"/>
-      <c r="E94" s="64"/>
-      <c r="F94" s="65"/>
+        <v>92</v>
+      </c>
+      <c r="B94" s="83"/>
+      <c r="C94" s="83"/>
+      <c r="D94" s="83"/>
+      <c r="E94" s="83"/>
+      <c r="F94" s="84"/>
       <c r="G94" s="12"/>
-      <c r="H94" s="66"/>
-      <c r="I94" s="67"/>
+      <c r="H94" s="87"/>
+      <c r="I94" s="88"/>
       <c r="J94" s="7"/>
     </row>
-    <row r="95" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A95" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B95" s="64"/>
-      <c r="C95" s="64"/>
-      <c r="D95" s="64"/>
-      <c r="E95" s="64"/>
-      <c r="F95" s="65"/>
+        <v>93</v>
+      </c>
+      <c r="B95" s="83"/>
+      <c r="C95" s="83"/>
+      <c r="D95" s="83"/>
+      <c r="E95" s="83"/>
+      <c r="F95" s="84"/>
       <c r="G95" s="12"/>
-      <c r="H95" s="66"/>
-      <c r="I95" s="67"/>
+      <c r="H95" s="87"/>
+      <c r="I95" s="88"/>
       <c r="J95" s="7"/>
     </row>
-    <row r="96" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A96" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B96" s="64"/>
-      <c r="C96" s="64"/>
-      <c r="D96" s="64"/>
-      <c r="E96" s="64"/>
-      <c r="F96" s="65"/>
+        <v>94</v>
+      </c>
+      <c r="B96" s="83"/>
+      <c r="C96" s="83"/>
+      <c r="D96" s="83"/>
+      <c r="E96" s="83"/>
+      <c r="F96" s="84"/>
       <c r="G96" s="12"/>
-      <c r="H96" s="66"/>
-      <c r="I96" s="67"/>
+      <c r="H96" s="87"/>
+      <c r="I96" s="88"/>
       <c r="J96" s="7"/>
     </row>
-    <row r="97" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A97" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="B97" s="64"/>
-      <c r="C97" s="64"/>
-      <c r="D97" s="64"/>
-      <c r="E97" s="64"/>
-      <c r="F97" s="65"/>
+        <v>95</v>
+      </c>
+      <c r="B97" s="83"/>
+      <c r="C97" s="83"/>
+      <c r="D97" s="83"/>
+      <c r="E97" s="83"/>
+      <c r="F97" s="84"/>
       <c r="G97" s="12"/>
-      <c r="H97" s="66"/>
-      <c r="I97" s="67"/>
+      <c r="H97" s="87"/>
+      <c r="I97" s="88"/>
       <c r="J97" s="7"/>
     </row>
-    <row r="98" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A98" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="B98" s="64"/>
-      <c r="C98" s="64"/>
-      <c r="D98" s="64"/>
-      <c r="E98" s="64"/>
-      <c r="F98" s="65"/>
+        <v>96</v>
+      </c>
+      <c r="B98" s="83"/>
+      <c r="C98" s="83"/>
+      <c r="D98" s="83"/>
+      <c r="E98" s="83"/>
+      <c r="F98" s="84"/>
       <c r="G98" s="12"/>
-      <c r="H98" s="66"/>
-      <c r="I98" s="67"/>
+      <c r="H98" s="87"/>
+      <c r="I98" s="88"/>
       <c r="J98" s="7"/>
     </row>
-    <row r="99" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A99" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="B99" s="64"/>
-      <c r="C99" s="64"/>
-      <c r="D99" s="64"/>
-      <c r="E99" s="64"/>
-      <c r="F99" s="65"/>
+        <v>97</v>
+      </c>
+      <c r="B99" s="83"/>
+      <c r="C99" s="83"/>
+      <c r="D99" s="83"/>
+      <c r="E99" s="83"/>
+      <c r="F99" s="84"/>
       <c r="G99" s="12"/>
-      <c r="H99" s="66"/>
-      <c r="I99" s="67"/>
+      <c r="H99" s="87"/>
+      <c r="I99" s="88"/>
       <c r="J99" s="7"/>
     </row>
-    <row r="100" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A100" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="B100" s="64"/>
-      <c r="C100" s="64"/>
-      <c r="D100" s="64"/>
-      <c r="E100" s="64"/>
-      <c r="F100" s="65"/>
+        <v>98</v>
+      </c>
+      <c r="B100" s="83"/>
+      <c r="C100" s="83"/>
+      <c r="D100" s="83"/>
+      <c r="E100" s="83"/>
+      <c r="F100" s="84"/>
       <c r="G100" s="12"/>
-      <c r="H100" s="66"/>
-      <c r="I100" s="67"/>
+      <c r="H100" s="87"/>
+      <c r="I100" s="88"/>
       <c r="J100" s="7"/>
     </row>
-    <row r="101" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="155" t="s">
-        <v>85</v>
-      </c>
-      <c r="B101" s="156"/>
-      <c r="C101" s="156"/>
-      <c r="D101" s="156"/>
-      <c r="E101" s="156"/>
-      <c r="F101" s="156"/>
-      <c r="G101" s="156"/>
-      <c r="H101" s="156"/>
-      <c r="I101" s="156"/>
-      <c r="J101" s="157"/>
-    </row>
-    <row r="102" spans="1:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="85" t="s">
-        <v>75</v>
-      </c>
-      <c r="B102" s="158"/>
-      <c r="C102" s="158"/>
-      <c r="D102" s="158"/>
-      <c r="E102" s="159"/>
-      <c r="F102" s="85" t="s">
-        <v>76</v>
-      </c>
-      <c r="G102" s="158"/>
-      <c r="H102" s="158"/>
-      <c r="I102" s="158"/>
-      <c r="J102" s="159"/>
-    </row>
-    <row r="103" spans="1:10" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="160"/>
-      <c r="B103" s="161"/>
-      <c r="C103" s="161"/>
-      <c r="D103" s="161"/>
-      <c r="E103" s="162"/>
-      <c r="F103" s="161"/>
-      <c r="G103" s="161"/>
-      <c r="H103" s="161"/>
-      <c r="I103" s="161"/>
-      <c r="J103" s="162"/>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="93" t="s">
+        <v>99</v>
+      </c>
+      <c r="B101" s="94"/>
+      <c r="C101" s="94"/>
+      <c r="D101" s="94"/>
+      <c r="E101" s="94"/>
+      <c r="F101" s="94"/>
+      <c r="G101" s="94"/>
+      <c r="H101" s="94"/>
+      <c r="I101" s="94"/>
+      <c r="J101" s="95"/>
+    </row>
+    <row r="102" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="96" t="s">
+        <v>100</v>
+      </c>
+      <c r="B102" s="97"/>
+      <c r="C102" s="97"/>
+      <c r="D102" s="97"/>
+      <c r="E102" s="98"/>
+      <c r="F102" s="96" t="s">
+        <v>101</v>
+      </c>
+      <c r="G102" s="97"/>
+      <c r="H102" s="97"/>
+      <c r="I102" s="97"/>
+      <c r="J102" s="98"/>
+    </row>
+    <row r="103" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="99" t="s">
+        <v>102</v>
+      </c>
+      <c r="B103" s="100"/>
+      <c r="C103" s="100"/>
+      <c r="D103" s="100"/>
+      <c r="E103" s="101"/>
+      <c r="F103" s="100" t="s">
+        <v>103</v>
+      </c>
+      <c r="G103" s="100"/>
+      <c r="H103" s="100"/>
+      <c r="I103" s="100"/>
+      <c r="J103" s="101"/>
     </row>
     <row r="104" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="151" t="s">
-        <v>79</v>
-      </c>
-      <c r="B104" s="152"/>
+      <c r="A104" s="89" t="s">
+        <v>104</v>
+      </c>
+      <c r="B104" s="90"/>
       <c r="C104" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="D104" s="153" t="s">
-        <v>80</v>
-      </c>
-      <c r="E104" s="152"/>
-      <c r="F104" s="152"/>
+        <v>82</v>
+      </c>
+      <c r="D104" s="91" t="s">
+        <v>105</v>
+      </c>
+      <c r="E104" s="90"/>
+      <c r="F104" s="90"/>
       <c r="G104" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="H104" s="151" t="s">
-        <v>78</v>
-      </c>
-      <c r="I104" s="154"/>
+        <v>82</v>
+      </c>
+      <c r="H104" s="89" t="s">
+        <v>106</v>
+      </c>
+      <c r="I104" s="92"/>
       <c r="J104" s="36" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="57"/>
-      <c r="B105" s="58"/>
-      <c r="C105" s="52"/>
-      <c r="D105" s="59"/>
-      <c r="E105" s="60"/>
-      <c r="F105" s="61"/>
-      <c r="G105" s="53"/>
-      <c r="H105" s="59"/>
-      <c r="I105" s="61"/>
-      <c r="J105" s="52"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="176" t="s">
+        <v>108</v>
+      </c>
+      <c r="B105" s="177"/>
+      <c r="C105" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="D105" s="178" t="s">
+        <v>109</v>
+      </c>
+      <c r="E105" s="179"/>
+      <c r="F105" s="180"/>
+      <c r="G105" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H105" s="178" t="s">
+        <v>110</v>
+      </c>
+      <c r="I105" s="180"/>
+      <c r="J105" s="52" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="123">
-    <mergeCell ref="A42:J54"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="F55:J55"/>
-    <mergeCell ref="A56:J56"/>
-    <mergeCell ref="A69:J86"/>
-    <mergeCell ref="A68:J68"/>
-    <mergeCell ref="A87:F87"/>
-    <mergeCell ref="H87:I87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="H91:I91"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D104:F104"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="A101:J101"/>
-    <mergeCell ref="A102:E102"/>
-    <mergeCell ref="F102:J102"/>
-    <mergeCell ref="A103:E103"/>
-    <mergeCell ref="F103:J103"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="H93:I93"/>
-    <mergeCell ref="H95:I95"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="D105:F105"/>
+    <mergeCell ref="H105:I105"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="B97:F97"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="H96:I96"/>
+    <mergeCell ref="H97:I97"/>
+    <mergeCell ref="B95:F95"/>
+    <mergeCell ref="H98:I98"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A16:B19"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="F8:J11"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="C29:J29"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="A8:E15"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C26:H26"/>
     <mergeCell ref="F12:J12"/>
     <mergeCell ref="F13:J13"/>
     <mergeCell ref="A27:J27"/>
@@ -9396,65 +9716,73 @@
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="C22:H22"/>
     <mergeCell ref="C16:E19"/>
-    <mergeCell ref="A8:E15"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C28:J28"/>
-    <mergeCell ref="C29:J29"/>
-    <mergeCell ref="C30:J30"/>
-    <mergeCell ref="C31:J31"/>
-    <mergeCell ref="C32:J32"/>
-    <mergeCell ref="C33:J33"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A16:B19"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="F8:J11"/>
-    <mergeCell ref="A20:J20"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="D105:F105"/>
-    <mergeCell ref="H105:I105"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="H96:I96"/>
-    <mergeCell ref="H97:I97"/>
-    <mergeCell ref="B95:F95"/>
-    <mergeCell ref="H98:I98"/>
-    <mergeCell ref="H94:I94"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="H88:I88"/>
     <mergeCell ref="A35:J35"/>
     <mergeCell ref="A36:J36"/>
-    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A34:J34"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="H93:I93"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="H94:I94"/>
+    <mergeCell ref="H88:I88"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="A101:J101"/>
+    <mergeCell ref="A102:E102"/>
+    <mergeCell ref="F102:J102"/>
+    <mergeCell ref="A103:E103"/>
+    <mergeCell ref="F103:J103"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="H87:I87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="A42:J54"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="F55:J55"/>
+    <mergeCell ref="A56:J56"/>
+    <mergeCell ref="A69:J86"/>
+    <mergeCell ref="A68:J68"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="63" fitToHeight="6" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="41" max="16383" man="1"/>
+    <brk id="41" max="1048575" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
@@ -9644,24 +9972,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <Please_x0020_note xmlns="f17bae92-5fa7-4270-afeb-ed962faafa52" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B342DF5A2DEFD64586E21F8B44CF3641" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="97e464cb99569ca8a9ef17fb08900847">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns3="f17bae92-5fa7-4270-afeb-ed962faafa52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6356073c4c24c81483cf02fe07ae928c" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -9800,10 +10110,39 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <Please_x0020_note xmlns="f17bae92-5fa7-4270-afeb-ed962faafa52" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A06E1120-8501-409E-8BA8-1494F83C4851}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544619E3-E001-4BD0-A0E9-1E9FD84B48E5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="f17bae92-5fa7-4270-afeb-ed962faafa52"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9826,20 +10165,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544619E3-E001-4BD0-A0E9-1E9FD84B48E5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A06E1120-8501-409E-8BA8-1494F83C4851}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="f17bae92-5fa7-4270-afeb-ed962faafa52"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
continuidad de edición de ewo
</commit_message>
<xml_diff>
--- a/DigiTools/Content/formats/FORMATO_EWO.XLSX
+++ b/DigiTools/Content/formats/FORMATO_EWO.XLSX
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unilever\Web\Mtto\DigiTools\DigiTools\Content\formats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UNILEVER_MTTO\Dropbox\HPC\MttoApp\DigiTools\DigiTools\Content\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC477D80-2EF2-482A-83D0-CCF8CF24495E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5910945-BA99-49A9-8870-41D5A0F937D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EWO" sheetId="7" r:id="rId1"/>
@@ -81,51 +81,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
   <si>
-    <t>EWO (Emergency Work Order)</t>
+    <t>NOK</t>
   </si>
   <si>
-    <t>EWO #</t>
+    <t>OK</t>
   </si>
   <si>
-    <t>Area/Linea</t>
+    <t>No PM</t>
   </si>
   <si>
-    <t>Equipo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha </t>
-  </si>
-  <si>
-    <t>Aviso #</t>
-  </si>
-  <si>
-    <t>Diligenciada por</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo de Avería                                                                                                                                                                                                                                        </t>
-  </si>
-  <si>
-    <t>Turno</t>
-  </si>
-  <si>
-    <t>MesPack</t>
-  </si>
-  <si>
-    <t>Mespack H-360 FED 363.008</t>
-  </si>
-  <si>
-    <t>20/03/2019</t>
-  </si>
-  <si>
-    <t>1231</t>
-  </si>
-  <si>
-    <t>Jeison Perlaza</t>
-  </si>
-  <si>
-    <t>Mecánica</t>
+    <t>No AM</t>
   </si>
   <si>
     <t>Notificación Avería (Hora)</t>
@@ -166,15 +133,6 @@
     <t>Descripción gráfica de la falla [dibujos y/o planos]</t>
   </si>
   <si>
-    <t>Descripción de la avería. Si la reparación no se ha terminado en su totalidad, indique que necesita que se realice para terminarla:</t>
-  </si>
-  <si>
-    <t>una avería</t>
-  </si>
-  <si>
-    <t>( X  ) Cambio de Componente                    (    ) Ajuste</t>
-  </si>
-  <si>
     <t>Repuestos Utilizados</t>
   </si>
   <si>
@@ -190,118 +148,107 @@
     <t>Costo [COP]</t>
   </si>
   <si>
-    <t>uno mas</t>
+    <t>1 - Por qué?</t>
   </si>
   <si>
-    <t>1 metro</t>
+    <t>2 - Por qué?</t>
   </si>
   <si>
-    <t>$12333,0000</t>
+    <t>3 - Por qué?</t>
   </si>
   <si>
-    <t>prueba 2 de mttr</t>
+    <t>4 - Por qué?</t>
+  </si>
+  <si>
+    <t>5 - Por qué?</t>
+  </si>
+  <si>
+    <t>Dibujo / Diagrama / Foto del 5 Por qué</t>
+  </si>
+  <si>
+    <t>Ciclo de la causa raíz</t>
+  </si>
+  <si>
+    <t>¿Qué tipo de falla es? Diligencie las fechas de los mantenimiento planeados y selecciones la causa raiz basada en el gráfico de la bañera</t>
+  </si>
+  <si>
+    <t>Error Humano (instalación)</t>
+  </si>
+  <si>
+    <t>Falla de Diseño</t>
+  </si>
+  <si>
+    <t>Error Humano 
+(en operación)</t>
+  </si>
+  <si>
+    <t>Condiciones Básicas</t>
+  </si>
+  <si>
+    <t>Condiciones de Operación</t>
+  </si>
+  <si>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Lista de Acciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Descripción de la avería. Si la reparación no se ha terminado en su totalidad, indique que necesita que se realice para terminarla:</t>
+  </si>
+  <si>
+    <t>(  ) Cambio de Componente                    (  ) Ajuste</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>8.</t>
+  </si>
+  <si>
+    <t>9.</t>
+  </si>
+  <si>
+    <t>10.</t>
+  </si>
+  <si>
+    <t>11.</t>
+  </si>
+  <si>
+    <t>12.</t>
+  </si>
+  <si>
+    <t>13.</t>
   </si>
   <si>
     <t>IDENTIFICACIÓN DE CAUSAS RAICES</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">IDENTIFICACION DE CAUSAS RAICES - 5G </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(llene esta seccion teniendo en cuenta el principio de los 5G)</t>
-    </r>
-  </si>
-  <si>
-    <t>NOK</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">GEMBA </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Ir al lugar donde se produce el problema)</t>
-    </r>
-  </si>
-  <si>
-    <t>df</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">GEMBUTSU </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Ver los objetos, piezas y materiales reales que participan en el problema)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">GENJITSU </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Confirmar una descripcion precisa y cuantificada del problema)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">GENRI </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Se refiere a la teoria. Principios mecanicos y fisicos que rigen la operación)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">GENSOKU </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Siguen el estandar de operación.Las condiciones requeridas para operar sin causar problemas)</t>
-    </r>
-  </si>
-  <si>
-    <t>5W + 1H</t>
+    <t>EWO (Emergency Work Order)</t>
   </si>
   <si>
     <r>
@@ -391,6 +338,90 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">COMO (HOW) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>¿Cómo difiere con respecto al optimo? ¿Cuál es el costo ($), que cantidad, en que tiempo?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GENSOKU </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Siguen el estandar de operación.Las condiciones requeridas para operar sin causar problemas)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GENRI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Se refiere a la teoria. Principios mecanicos y fisicos que rigen la operación)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GENJITSU </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Confirmar una descripcion precisa y cuantificada del problema)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GEMBUTSU </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Ver los objetos, piezas y materiales reales que participan en el problema)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GEMBA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Ir al lugar donde se produce el problema)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Cual (WHICH)? </t>
     </r>
     <r>
@@ -404,86 +435,55 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">COMO (HOW) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>¿Cómo difiere con respecto al optimo? ¿Cuál es el costo ($), que cantidad, en que tiempo?</t>
-    </r>
-  </si>
-  <si>
     <t>HOW + WHAT + WHERE + WHEN + WHICH + WHO = FENOMENO</t>
   </si>
   <si>
-    <t>df df df df df df</t>
+    <t xml:space="preserve">Tipo de Avería                                                                                                                                                                                                                                        </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">5 ANÁLISIS POR QUÉ - POR QUÉ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Unilever DIN Offc Pro"/>
-        <family val="2"/>
-      </rPr>
-      <t>(diligencie este campo si todas las causas reaices se encuentran OK)</t>
-    </r>
+    <t>Diligenciada por</t>
   </si>
   <si>
-    <t>1 - Por qué?</t>
+    <t xml:space="preserve">Fecha </t>
   </si>
   <si>
-    <t>2 - Por qué?</t>
+    <t>Aviso #</t>
   </si>
   <si>
-    <t>3 - Por qué?</t>
+    <t>Equipo</t>
   </si>
   <si>
-    <t>4 - Por qué?</t>
+    <t>Area/Linea</t>
   </si>
   <si>
-    <t>5 - Por qué?</t>
+    <t>Turno</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>EWO #</t>
   </si>
   <si>
-    <t>Dibujo / Diagrama / Foto del 5 Por qué</t>
+    <t>5W + 1H</t>
   </si>
   <si>
-    <t>otra prueba</t>
+    <t xml:space="preserve">Técnico(s) de Mantenimiento Involucrado(s)                                                                                                                                                                                                                    </t>
   </si>
   <si>
-    <t>¿Qué tipo de falla es? Diligencie las fechas de los mantenimiento planeados y selecciones la causa raiz basada en el gráfico de la bañera</t>
+    <t>Operario(s) Involucrado(s)</t>
   </si>
   <si>
-    <t>Fecha Ultimo Mtto</t>
+    <t xml:space="preserve">Fecha                                                                                                                                                                                                                                                                                                </t>
   </si>
   <si>
-    <t>Fecha Proximo Mtto</t>
+    <t>Ejecución Validada Por</t>
   </si>
   <si>
-    <t>Error Humano (instalación)</t>
+    <t>Análisis Elaborado Por</t>
   </si>
   <si>
-    <t>Condiciones de Operación</t>
+    <t>Contramedidas Definidas Por</t>
   </si>
   <si>
-    <t>Falla de Diseño</t>
-  </si>
-  <si>
-    <t>Condiciones Básicas</t>
-  </si>
-  <si>
-    <t>No PM</t>
+    <t>Tipo de Accion</t>
   </si>
   <si>
     <r>
@@ -501,74 +501,10 @@
     </r>
   </si>
   <si>
-    <t>Error Humano 
-(en operación)</t>
+    <t>Fecha Ultimo Mtto</t>
   </si>
   <si>
-    <t>No AM</t>
-  </si>
-  <si>
-    <t>Ciclo de la causa raíz</t>
-  </si>
-  <si>
-    <t>Lista de Acciones</t>
-  </si>
-  <si>
-    <t>Tipo de Accion</t>
-  </si>
-  <si>
-    <t>Responsable</t>
-  </si>
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>prueba</t>
-  </si>
-  <si>
-    <t>CM</t>
-  </si>
-  <si>
-    <t>Angel Morales</t>
-  </si>
-  <si>
-    <t>2.</t>
-  </si>
-  <si>
-    <t>3.</t>
-  </si>
-  <si>
-    <t>4.</t>
-  </si>
-  <si>
-    <t>5.</t>
-  </si>
-  <si>
-    <t>6.</t>
-  </si>
-  <si>
-    <t>7.</t>
-  </si>
-  <si>
-    <t>8.</t>
-  </si>
-  <si>
-    <t>9.</t>
-  </si>
-  <si>
-    <t>10.</t>
-  </si>
-  <si>
-    <t>11.</t>
-  </si>
-  <si>
-    <t>12.</t>
-  </si>
-  <si>
-    <t>13.</t>
+    <t>Fecha Proximo Mtto</t>
   </si>
   <si>
     <r>
@@ -633,37 +569,32 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Técnico(s) de Mantenimiento Involucrado(s)                                                                                                                                                                                                                    </t>
+    <r>
+      <t xml:space="preserve">5 ANÁLISIS POR QUÉ - POR QUÉ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(diligencie este campo si todas las causas reaices se encuentran OK)</t>
+    </r>
   </si>
   <si>
-    <t>Operario(s) Involucrado(s)</t>
-  </si>
-  <si>
-    <t>Édinson Rodríguez Urrea</t>
-  </si>
-  <si>
-    <t>Deisy Ipus</t>
-  </si>
-  <si>
-    <t>Análisis Elaborado Por</t>
-  </si>
-  <si>
-    <t>Contramedidas Definidas Por</t>
-  </si>
-  <si>
-    <t>Ejecución Validada Por</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha                                                                                                                                                                                                                                                                                                </t>
-  </si>
-  <si>
-    <t>Fabian Morante Olmos</t>
-  </si>
-  <si>
-    <t>Diego Fernando Murillo Arboleda</t>
-  </si>
-  <si>
-    <t>Carlos Andres Varela</t>
+    <r>
+      <t xml:space="preserve">IDENTIFICACION DE CAUSAS RAICES - 5G </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Unilever DIN Offc Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>(llene esta seccion teniendo en cuenta el principio de los 5G)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -791,8 +722,21 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF0000FF"/>
+      <name val="Unilever DIN Offc Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
       <i/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Unilever DIN Offc Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
       <color theme="1"/>
       <name val="Unilever DIN Offc Pro"/>
       <family val="2"/>
@@ -805,23 +749,9 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
-      <color theme="1"/>
-      <name val="Unilever DIN Offc Pro"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Unilever DIN Offc Pro"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="7"/>
-      <color rgb="FF0000FF"/>
-      <name val="Unilever DIN Offc Pro"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -832,9 +762,10 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <color theme="1"/>
+      <name val="Unilever DIN Offc Pro"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1354,569 +1285,569 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="190">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1950,7 +1881,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1966,7 +1897,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2036,9 +1967,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
+      <xdr:colOff>631050</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>447676</xdr:rowOff>
+      <xdr:rowOff>447675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7463,159 +7394,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>571500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="image1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>285750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="image3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Elipse 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{386A29A4-D55C-4AED-926C-AC5703E538A5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1069975" y="21590000"/>
-          <a:ext cx="1016000" cy="2540000"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:alpha val="11000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-CO" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7959,46 +7737,46 @@
     <col min="9" max="10" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="39.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="144" t="s">
-        <v>0</v>
+    <row r="1" spans="1:16" ht="39.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="81" t="s">
+        <v>53</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="145"/>
-      <c r="I1" s="145"/>
-      <c r="J1" s="147"/>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="84"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
-      <c r="C2" s="96" t="s">
-        <v>3</v>
+      <c r="C2" s="85" t="s">
+        <v>70</v>
       </c>
-      <c r="D2" s="148"/>
+      <c r="D2" s="86"/>
       <c r="E2" s="31" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
-      <c r="H2" s="149" t="s">
-        <v>7</v>
+      <c r="H2" s="87" t="s">
+        <v>66</v>
       </c>
-      <c r="I2" s="150"/>
+      <c r="I2" s="88"/>
       <c r="J2" s="2" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -8007,33 +7785,17 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25">
-        <v>2</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="162" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="163"/>
-      <c r="E3" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="162" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="163"/>
-      <c r="J3" s="30">
-        <v>3</v>
-      </c>
+    <row r="3" spans="1:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="30"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -8041,27 +7803,27 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="151" t="s">
-        <v>15</v>
+    <row r="4" spans="1:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="89" t="s">
+        <v>4</v>
       </c>
-      <c r="B4" s="151" t="s">
-        <v>16</v>
+      <c r="B4" s="89" t="s">
+        <v>5</v>
       </c>
-      <c r="C4" s="153" t="s">
-        <v>17</v>
+      <c r="C4" s="91" t="s">
+        <v>6</v>
       </c>
-      <c r="D4" s="153"/>
-      <c r="E4" s="153"/>
-      <c r="F4" s="154"/>
-      <c r="G4" s="154"/>
-      <c r="H4" s="151" t="s">
-        <v>18</v>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="89" t="s">
+        <v>7</v>
       </c>
-      <c r="I4" s="155" t="s">
-        <v>19</v>
+      <c r="I4" s="93" t="s">
+        <v>8</v>
       </c>
-      <c r="J4" s="156"/>
+      <c r="J4" s="94"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -8069,27 +7831,27 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="152"/>
-      <c r="B5" s="152"/>
+    <row r="5" spans="1:16" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="90"/>
+      <c r="B5" s="90"/>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
-      <c r="H5" s="152"/>
-      <c r="I5" s="157"/>
-      <c r="J5" s="158"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="96"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -8097,35 +7859,17 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
-        <v>43544.515972222202</v>
-      </c>
-      <c r="B6" s="15">
-        <v>43544.524305555598</v>
-      </c>
-      <c r="C6" s="16">
-        <v>12</v>
-      </c>
-      <c r="D6" s="16">
-        <v>9</v>
-      </c>
-      <c r="E6" s="16">
-        <v>2</v>
-      </c>
-      <c r="F6" s="16">
-        <v>1</v>
-      </c>
-      <c r="G6" s="16">
-        <v>3</v>
-      </c>
-      <c r="H6" s="15">
-        <v>43544.534722222197</v>
-      </c>
-      <c r="I6" s="168">
-        <v>27</v>
-      </c>
-      <c r="J6" s="169"/>
+    <row r="6" spans="1:16" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="110"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -8133,21 +7877,21 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="164" t="s">
-        <v>25</v>
+    <row r="7" spans="1:16" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="105" t="s">
+        <v>14</v>
       </c>
-      <c r="B7" s="165"/>
-      <c r="C7" s="165"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="119" t="s">
-        <v>26</v>
+      <c r="B7" s="106"/>
+      <c r="C7" s="106"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="97" t="s">
+        <v>37</v>
       </c>
-      <c r="G7" s="167"/>
-      <c r="H7" s="167"/>
-      <c r="I7" s="167"/>
-      <c r="J7" s="120"/>
+      <c r="G7" s="108"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="98"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -8156,216 +7900,204 @@
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="140"/>
-      <c r="B8" s="141"/>
-      <c r="C8" s="141"/>
-      <c r="D8" s="141"/>
-      <c r="E8" s="142"/>
-      <c r="F8" s="170" t="s">
-        <v>27</v>
+      <c r="A8" s="131"/>
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="132"/>
+      <c r="E8" s="133"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="112"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="113"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="99"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="115"/>
+      <c r="H9" s="115"/>
+      <c r="I9" s="115"/>
+      <c r="J9" s="116"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="99"/>
+      <c r="B10" s="100"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="129"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="115"/>
+      <c r="H10" s="115"/>
+      <c r="I10" s="115"/>
+      <c r="J10" s="116"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="99"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="100"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="129"/>
+      <c r="F11" s="114"/>
+      <c r="G11" s="115"/>
+      <c r="H11" s="115"/>
+      <c r="I11" s="115"/>
+      <c r="J11" s="116"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="99"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="117" t="s">
+        <v>38</v>
       </c>
-      <c r="G8" s="171"/>
-      <c r="H8" s="171"/>
-      <c r="I8" s="171"/>
-      <c r="J8" s="172"/>
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="143"/>
-      <c r="B9" s="136"/>
-      <c r="C9" s="136"/>
-      <c r="D9" s="136"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="174"/>
-      <c r="H9" s="174"/>
-      <c r="I9" s="174"/>
-      <c r="J9" s="175"/>
-      <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="143"/>
-      <c r="B10" s="136"/>
-      <c r="C10" s="136"/>
-      <c r="D10" s="136"/>
-      <c r="E10" s="137"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="174"/>
-      <c r="H10" s="174"/>
-      <c r="I10" s="174"/>
-      <c r="J10" s="175"/>
-      <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="143"/>
-      <c r="B11" s="136"/>
-      <c r="C11" s="136"/>
-      <c r="D11" s="136"/>
-      <c r="E11" s="137"/>
-      <c r="F11" s="173"/>
-      <c r="G11" s="174"/>
-      <c r="H11" s="174"/>
-      <c r="I11" s="174"/>
-      <c r="J11" s="175"/>
-      <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="143"/>
-      <c r="B12" s="136"/>
-      <c r="C12" s="136"/>
-      <c r="D12" s="136"/>
-      <c r="E12" s="137"/>
-      <c r="F12" s="121" t="s">
-        <v>28</v>
+      <c r="G12" s="118"/>
+      <c r="H12" s="118"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="119"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="99"/>
+      <c r="B13" s="100"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="120" t="s">
+        <v>15</v>
       </c>
-      <c r="G12" s="122"/>
-      <c r="H12" s="122"/>
-      <c r="I12" s="122"/>
-      <c r="J12" s="123"/>
-      <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="143"/>
-      <c r="B13" s="136"/>
-      <c r="C13" s="136"/>
-      <c r="D13" s="136"/>
-      <c r="E13" s="137"/>
-      <c r="F13" s="124" t="s">
-        <v>29</v>
+      <c r="G13" s="121"/>
+      <c r="H13" s="121"/>
+      <c r="I13" s="121"/>
+      <c r="J13" s="122"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="99"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="100"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="129"/>
+      <c r="F14" s="33" t="s">
+        <v>16</v>
       </c>
-      <c r="G13" s="125"/>
-      <c r="H13" s="125"/>
-      <c r="I13" s="125"/>
-      <c r="J13" s="126"/>
-      <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="143"/>
-      <c r="B14" s="136"/>
-      <c r="C14" s="136"/>
-      <c r="D14" s="136"/>
-      <c r="E14" s="137"/>
-      <c r="F14" s="33" t="s">
-        <v>30</v>
+      <c r="G14" s="123" t="s">
+        <v>17</v>
       </c>
-      <c r="G14" s="130" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="130"/>
+      <c r="H14" s="123"/>
       <c r="I14" s="34" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="J14" s="35" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="143"/>
-      <c r="B15" s="136"/>
-      <c r="C15" s="136"/>
-      <c r="D15" s="136"/>
-      <c r="E15" s="137"/>
-      <c r="F15" s="17">
-        <v>233</v>
-      </c>
-      <c r="G15" s="131" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="131"/>
-      <c r="I15" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>36</v>
-      </c>
+      <c r="A15" s="99"/>
+      <c r="B15" s="100"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="129"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="143" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="136"/>
-      <c r="C16" s="136"/>
-      <c r="D16" s="136"/>
-      <c r="E16" s="137"/>
+      <c r="A16" s="99"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="100"/>
+      <c r="E16" s="129"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="131"/>
-      <c r="H16" s="131"/>
+      <c r="G16" s="124"/>
+      <c r="H16" s="124"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="143"/>
-      <c r="B17" s="136"/>
-      <c r="C17" s="136"/>
-      <c r="D17" s="136"/>
-      <c r="E17" s="137"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="129"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="131"/>
-      <c r="H17" s="131"/>
+      <c r="G17" s="124"/>
+      <c r="H17" s="124"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="143"/>
-      <c r="B18" s="136"/>
-      <c r="C18" s="136"/>
-      <c r="D18" s="136"/>
-      <c r="E18" s="137"/>
+      <c r="A18" s="99"/>
+      <c r="B18" s="100"/>
+      <c r="C18" s="100"/>
+      <c r="D18" s="100"/>
+      <c r="E18" s="129"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="131"/>
-      <c r="H18" s="131"/>
+      <c r="G18" s="124"/>
+      <c r="H18" s="124"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="161"/>
-      <c r="B19" s="138"/>
-      <c r="C19" s="138"/>
-      <c r="D19" s="138"/>
-      <c r="E19" s="139"/>
+    <row r="19" spans="1:16" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="101"/>
+      <c r="B19" s="102"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="102"/>
+      <c r="E19" s="130"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="132"/>
-      <c r="H19" s="132"/>
+      <c r="G19" s="125"/>
+      <c r="H19" s="125"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="127" t="s">
-        <v>38</v>
+    <row r="20" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="54" t="s">
+        <v>52</v>
       </c>
-      <c r="B20" s="128"/>
-      <c r="C20" s="128"/>
-      <c r="D20" s="128"/>
-      <c r="E20" s="128"/>
-      <c r="F20" s="128"/>
-      <c r="G20" s="128"/>
-      <c r="H20" s="128"/>
-      <c r="I20" s="128"/>
-      <c r="J20" s="129"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="56"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="185" t="s">
-        <v>39</v>
+    <row r="21" spans="1:16" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="76" t="s">
+        <v>87</v>
       </c>
-      <c r="B21" s="186"/>
-      <c r="C21" s="186"/>
-      <c r="D21" s="186"/>
-      <c r="E21" s="186"/>
-      <c r="F21" s="186"/>
-      <c r="G21" s="186"/>
-      <c r="H21" s="186"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
       <c r="I21" s="5" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -8374,22 +8106,18 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="119" t="s">
-        <v>42</v>
+    <row r="22" spans="1:16" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="97" t="s">
+        <v>63</v>
       </c>
-      <c r="B22" s="120"/>
-      <c r="C22" s="133" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="134"/>
-      <c r="E22" s="134"/>
-      <c r="F22" s="134"/>
-      <c r="G22" s="134"/>
-      <c r="H22" s="135"/>
-      <c r="I22" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="B22" s="98"/>
+      <c r="C22" s="126"/>
+      <c r="D22" s="127"/>
+      <c r="E22" s="127"/>
+      <c r="F22" s="127"/>
+      <c r="G22" s="127"/>
+      <c r="H22" s="128"/>
+      <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -8398,22 +8126,18 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="119" t="s">
-        <v>45</v>
+    <row r="23" spans="1:16" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="97" t="s">
+        <v>62</v>
       </c>
-      <c r="B23" s="120"/>
-      <c r="C23" s="133" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="134"/>
-      <c r="E23" s="134"/>
-      <c r="F23" s="134"/>
-      <c r="G23" s="134"/>
-      <c r="H23" s="135"/>
-      <c r="I23" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="B23" s="98"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="127"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="128"/>
+      <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -8422,22 +8146,18 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="119" t="s">
-        <v>46</v>
+    <row r="24" spans="1:16" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="97" t="s">
+        <v>61</v>
       </c>
-      <c r="B24" s="120"/>
-      <c r="C24" s="133" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="134"/>
-      <c r="E24" s="134"/>
-      <c r="F24" s="134"/>
-      <c r="G24" s="134"/>
-      <c r="H24" s="135"/>
-      <c r="I24" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="B24" s="98"/>
+      <c r="C24" s="126"/>
+      <c r="D24" s="127"/>
+      <c r="E24" s="127"/>
+      <c r="F24" s="127"/>
+      <c r="G24" s="127"/>
+      <c r="H24" s="128"/>
+      <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -8446,20 +8166,18 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="119" t="s">
-        <v>47</v>
+    <row r="25" spans="1:16" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="97" t="s">
+        <v>60</v>
       </c>
-      <c r="B25" s="120"/>
-      <c r="C25" s="133"/>
-      <c r="D25" s="134"/>
-      <c r="E25" s="134"/>
-      <c r="F25" s="134"/>
-      <c r="G25" s="134"/>
-      <c r="H25" s="135"/>
-      <c r="I25" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="B25" s="98"/>
+      <c r="C25" s="126"/>
+      <c r="D25" s="127"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="127"/>
+      <c r="G25" s="127"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -8468,20 +8186,18 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="119" t="s">
-        <v>48</v>
+    <row r="26" spans="1:16" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="97" t="s">
+        <v>59</v>
       </c>
-      <c r="B26" s="120"/>
-      <c r="C26" s="133"/>
-      <c r="D26" s="134"/>
-      <c r="E26" s="134"/>
-      <c r="F26" s="134"/>
-      <c r="G26" s="134"/>
-      <c r="H26" s="135"/>
-      <c r="I26" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="B26" s="98"/>
+      <c r="C26" s="126"/>
+      <c r="D26" s="127"/>
+      <c r="E26" s="127"/>
+      <c r="F26" s="127"/>
+      <c r="G26" s="127"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="9"/>
       <c r="J26" s="9"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -8490,19 +8206,19 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="127" t="s">
-        <v>49</v>
+    <row r="27" spans="1:16" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="54" t="s">
+        <v>74</v>
       </c>
-      <c r="B27" s="128"/>
-      <c r="C27" s="128"/>
-      <c r="D27" s="128"/>
-      <c r="E27" s="128"/>
-      <c r="F27" s="128"/>
-      <c r="G27" s="128"/>
-      <c r="H27" s="128"/>
-      <c r="I27" s="128"/>
-      <c r="J27" s="129"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="56"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -8510,21 +8226,19 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="119" t="s">
-        <v>50</v>
+    <row r="28" spans="1:16" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="97" t="s">
+        <v>54</v>
       </c>
-      <c r="B28" s="120"/>
-      <c r="C28" s="159" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="159"/>
-      <c r="E28" s="159"/>
-      <c r="F28" s="159"/>
-      <c r="G28" s="159"/>
-      <c r="H28" s="159"/>
-      <c r="I28" s="159"/>
-      <c r="J28" s="160"/>
+      <c r="B28" s="98"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="72"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -8532,21 +8246,19 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="119" t="s">
-        <v>51</v>
+    <row r="29" spans="1:16" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="97" t="s">
+        <v>55</v>
       </c>
-      <c r="B29" s="120"/>
-      <c r="C29" s="159" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="159"/>
-      <c r="E29" s="159"/>
-      <c r="F29" s="159"/>
-      <c r="G29" s="159"/>
-      <c r="H29" s="159"/>
-      <c r="I29" s="159"/>
-      <c r="J29" s="160"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="72"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -8554,21 +8266,19 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="119" t="s">
-        <v>52</v>
+    <row r="30" spans="1:16" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="97" t="s">
+        <v>56</v>
       </c>
-      <c r="B30" s="120"/>
-      <c r="C30" s="159" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="159"/>
-      <c r="E30" s="159"/>
-      <c r="F30" s="159"/>
-      <c r="G30" s="159"/>
-      <c r="H30" s="159"/>
-      <c r="I30" s="159"/>
-      <c r="J30" s="160"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="72"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -8576,21 +8286,19 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="119" t="s">
-        <v>53</v>
+    <row r="31" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="97" t="s">
+        <v>57</v>
       </c>
-      <c r="B31" s="120"/>
-      <c r="C31" s="159" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="159"/>
-      <c r="E31" s="159"/>
-      <c r="F31" s="159"/>
-      <c r="G31" s="159"/>
-      <c r="H31" s="159"/>
-      <c r="I31" s="159"/>
-      <c r="J31" s="160"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="72"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -8598,21 +8306,19 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="119" t="s">
-        <v>54</v>
+    <row r="32" spans="1:16" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="97" t="s">
+        <v>64</v>
       </c>
-      <c r="B32" s="120"/>
-      <c r="C32" s="159" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="159"/>
-      <c r="E32" s="159"/>
-      <c r="F32" s="159"/>
-      <c r="G32" s="159"/>
-      <c r="H32" s="159"/>
-      <c r="I32" s="159"/>
-      <c r="J32" s="160"/>
+      <c r="B32" s="98"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="72"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -8620,21 +8326,19 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="119" t="s">
-        <v>55</v>
+    <row r="33" spans="1:16" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="97" t="s">
+        <v>58</v>
       </c>
-      <c r="B33" s="120"/>
-      <c r="C33" s="159" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" s="159"/>
-      <c r="E33" s="159"/>
-      <c r="F33" s="159"/>
-      <c r="G33" s="159"/>
-      <c r="H33" s="159"/>
-      <c r="I33" s="159"/>
-      <c r="J33" s="160"/>
+      <c r="B33" s="98"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="72"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -8642,19 +8346,19 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="187" t="s">
-        <v>56</v>
+    <row r="34" spans="1:16" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="78" t="s">
+        <v>65</v>
       </c>
-      <c r="B34" s="188"/>
-      <c r="C34" s="188"/>
-      <c r="D34" s="188"/>
-      <c r="E34" s="188"/>
-      <c r="F34" s="188"/>
-      <c r="G34" s="188"/>
-      <c r="H34" s="188"/>
-      <c r="I34" s="188"/>
-      <c r="J34" s="189"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="79"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="79"/>
+      <c r="G34" s="79"/>
+      <c r="H34" s="79"/>
+      <c r="I34" s="79"/>
+      <c r="J34" s="80"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -8662,19 +8366,17 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="181" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="159"/>
-      <c r="C35" s="159"/>
-      <c r="D35" s="159"/>
-      <c r="E35" s="159"/>
-      <c r="F35" s="159"/>
-      <c r="G35" s="159"/>
-      <c r="H35" s="159"/>
-      <c r="I35" s="159"/>
-      <c r="J35" s="160"/>
+    <row r="35" spans="1:16" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="70"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="72"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -8682,285 +8384,283 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="182" t="s">
-        <v>58</v>
+    <row r="36" spans="1:16" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="73" t="s">
+        <v>86</v>
       </c>
-      <c r="B36" s="183"/>
-      <c r="C36" s="183"/>
-      <c r="D36" s="183"/>
-      <c r="E36" s="183"/>
-      <c r="F36" s="183"/>
-      <c r="G36" s="183"/>
-      <c r="H36" s="183"/>
-      <c r="I36" s="183"/>
-      <c r="J36" s="184"/>
+      <c r="B36" s="74"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="74"/>
+      <c r="I36" s="74"/>
+      <c r="J36" s="75"/>
     </row>
     <row r="37" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="114" t="s">
-        <v>59</v>
+      <c r="A37" s="134" t="s">
+        <v>20</v>
       </c>
-      <c r="B37" s="115"/>
-      <c r="C37" s="116" t="s">
-        <v>60</v>
+      <c r="B37" s="135"/>
+      <c r="C37" s="136" t="s">
+        <v>21</v>
       </c>
-      <c r="D37" s="115"/>
-      <c r="E37" s="116" t="s">
-        <v>61</v>
+      <c r="D37" s="135"/>
+      <c r="E37" s="136" t="s">
+        <v>22</v>
       </c>
-      <c r="F37" s="115"/>
-      <c r="G37" s="116" t="s">
-        <v>62</v>
+      <c r="F37" s="135"/>
+      <c r="G37" s="136" t="s">
+        <v>23</v>
       </c>
-      <c r="H37" s="115"/>
-      <c r="I37" s="116" t="s">
-        <v>63</v>
+      <c r="H37" s="135"/>
+      <c r="I37" s="136" t="s">
+        <v>24</v>
       </c>
-      <c r="J37" s="117"/>
+      <c r="J37" s="137"/>
     </row>
     <row r="38" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="118"/>
-      <c r="B38" s="106"/>
-      <c r="C38" s="106"/>
-      <c r="D38" s="106"/>
-      <c r="E38" s="106"/>
-      <c r="F38" s="106"/>
-      <c r="G38" s="106"/>
-      <c r="H38" s="106"/>
-      <c r="I38" s="106"/>
-      <c r="J38" s="108"/>
+      <c r="A38" s="138"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="144"/>
     </row>
     <row r="39" spans="1:16" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="118" t="s">
-        <v>64</v>
+      <c r="A39" s="138" t="s">
+        <v>36</v>
       </c>
-      <c r="B39" s="106"/>
-      <c r="C39" s="106"/>
-      <c r="D39" s="106"/>
-      <c r="E39" s="106"/>
-      <c r="F39" s="106"/>
-      <c r="G39" s="106"/>
-      <c r="H39" s="106"/>
-      <c r="I39" s="106"/>
-      <c r="J39" s="109"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="62"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="62"/>
+      <c r="I39" s="62"/>
+      <c r="J39" s="145"/>
     </row>
     <row r="40" spans="1:16" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="102" t="s">
-        <v>64</v>
+      <c r="A40" s="139" t="s">
+        <v>36</v>
       </c>
-      <c r="B40" s="103"/>
-      <c r="C40" s="106"/>
-      <c r="D40" s="107"/>
-      <c r="E40" s="106" t="s">
-        <v>64</v>
+      <c r="B40" s="140"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="143"/>
+      <c r="E40" s="62" t="s">
+        <v>36</v>
       </c>
-      <c r="F40" s="106"/>
-      <c r="G40" s="106" t="s">
-        <v>64</v>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62" t="s">
+        <v>36</v>
       </c>
-      <c r="H40" s="106"/>
-      <c r="I40" s="110" t="s">
-        <v>64</v>
+      <c r="H40" s="62"/>
+      <c r="I40" s="146" t="s">
+        <v>36</v>
       </c>
-      <c r="J40" s="109"/>
-    </row>
-    <row r="41" spans="1:16" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="104"/>
-      <c r="B41" s="105"/>
-      <c r="C41" s="105"/>
-      <c r="D41" s="105"/>
-      <c r="E41" s="113"/>
-      <c r="F41" s="113"/>
-      <c r="G41" s="113"/>
-      <c r="H41" s="113"/>
-      <c r="I41" s="111"/>
-      <c r="J41" s="112"/>
+      <c r="J40" s="145"/>
+    </row>
+    <row r="41" spans="1:16" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="141"/>
+      <c r="B41" s="142"/>
+      <c r="C41" s="142"/>
+      <c r="D41" s="142"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="63"/>
+      <c r="I41" s="147"/>
+      <c r="J41" s="148"/>
     </row>
     <row r="42" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="54" t="s">
-        <v>65</v>
+      <c r="A42" s="163" t="s">
+        <v>25</v>
       </c>
-      <c r="B42" s="55"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="55"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="56"/>
+      <c r="B42" s="164"/>
+      <c r="C42" s="164"/>
+      <c r="D42" s="164"/>
+      <c r="E42" s="164"/>
+      <c r="F42" s="164"/>
+      <c r="G42" s="164"/>
+      <c r="H42" s="164"/>
+      <c r="I42" s="164"/>
+      <c r="J42" s="165"/>
     </row>
     <row r="43" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="57"/>
-      <c r="B43" s="58"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="59"/>
+      <c r="A43" s="166"/>
+      <c r="B43" s="167"/>
+      <c r="C43" s="167"/>
+      <c r="D43" s="167"/>
+      <c r="E43" s="167"/>
+      <c r="F43" s="167"/>
+      <c r="G43" s="167"/>
+      <c r="H43" s="167"/>
+      <c r="I43" s="167"/>
+      <c r="J43" s="168"/>
     </row>
     <row r="44" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="57"/>
-      <c r="B44" s="58"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="59"/>
+      <c r="A44" s="166"/>
+      <c r="B44" s="167"/>
+      <c r="C44" s="167"/>
+      <c r="D44" s="167"/>
+      <c r="E44" s="167"/>
+      <c r="F44" s="167"/>
+      <c r="G44" s="167"/>
+      <c r="H44" s="167"/>
+      <c r="I44" s="167"/>
+      <c r="J44" s="168"/>
     </row>
     <row r="45" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="57"/>
-      <c r="B45" s="58"/>
-      <c r="C45" s="58"/>
-      <c r="D45" s="58"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="58"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="58"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="59"/>
+      <c r="A45" s="166"/>
+      <c r="B45" s="167"/>
+      <c r="C45" s="167"/>
+      <c r="D45" s="167"/>
+      <c r="E45" s="167"/>
+      <c r="F45" s="167"/>
+      <c r="G45" s="167"/>
+      <c r="H45" s="167"/>
+      <c r="I45" s="167"/>
+      <c r="J45" s="168"/>
     </row>
     <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="57"/>
-      <c r="B46" s="58"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="58"/>
-      <c r="J46" s="59"/>
+      <c r="A46" s="166"/>
+      <c r="B46" s="167"/>
+      <c r="C46" s="167"/>
+      <c r="D46" s="167"/>
+      <c r="E46" s="167"/>
+      <c r="F46" s="167"/>
+      <c r="G46" s="167"/>
+      <c r="H46" s="167"/>
+      <c r="I46" s="167"/>
+      <c r="J46" s="168"/>
     </row>
     <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="57"/>
-      <c r="B47" s="58"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="58"/>
-      <c r="J47" s="59"/>
+      <c r="A47" s="166"/>
+      <c r="B47" s="167"/>
+      <c r="C47" s="167"/>
+      <c r="D47" s="167"/>
+      <c r="E47" s="167"/>
+      <c r="F47" s="167"/>
+      <c r="G47" s="167"/>
+      <c r="H47" s="167"/>
+      <c r="I47" s="167"/>
+      <c r="J47" s="168"/>
     </row>
     <row r="48" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="57"/>
-      <c r="B48" s="58"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="58"/>
-      <c r="J48" s="59"/>
+      <c r="A48" s="166"/>
+      <c r="B48" s="167"/>
+      <c r="C48" s="167"/>
+      <c r="D48" s="167"/>
+      <c r="E48" s="167"/>
+      <c r="F48" s="167"/>
+      <c r="G48" s="167"/>
+      <c r="H48" s="167"/>
+      <c r="I48" s="167"/>
+      <c r="J48" s="168"/>
     </row>
     <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="57"/>
-      <c r="B49" s="58"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
-      <c r="J49" s="59"/>
+      <c r="A49" s="166"/>
+      <c r="B49" s="167"/>
+      <c r="C49" s="167"/>
+      <c r="D49" s="167"/>
+      <c r="E49" s="167"/>
+      <c r="F49" s="167"/>
+      <c r="G49" s="167"/>
+      <c r="H49" s="167"/>
+      <c r="I49" s="167"/>
+      <c r="J49" s="168"/>
     </row>
     <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="57"/>
-      <c r="B50" s="58"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
-      <c r="J50" s="59"/>
+      <c r="A50" s="166"/>
+      <c r="B50" s="167"/>
+      <c r="C50" s="167"/>
+      <c r="D50" s="167"/>
+      <c r="E50" s="167"/>
+      <c r="F50" s="167"/>
+      <c r="G50" s="167"/>
+      <c r="H50" s="167"/>
+      <c r="I50" s="167"/>
+      <c r="J50" s="168"/>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="57"/>
-      <c r="B51" s="58"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="58"/>
-      <c r="I51" s="58"/>
-      <c r="J51" s="59"/>
+      <c r="A51" s="166"/>
+      <c r="B51" s="167"/>
+      <c r="C51" s="167"/>
+      <c r="D51" s="167"/>
+      <c r="E51" s="167"/>
+      <c r="F51" s="167"/>
+      <c r="G51" s="167"/>
+      <c r="H51" s="167"/>
+      <c r="I51" s="167"/>
+      <c r="J51" s="168"/>
     </row>
     <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="57"/>
-      <c r="B52" s="58"/>
-      <c r="C52" s="58"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="58"/>
-      <c r="G52" s="58"/>
-      <c r="H52" s="58"/>
-      <c r="I52" s="58"/>
-      <c r="J52" s="59"/>
+      <c r="A52" s="166"/>
+      <c r="B52" s="167"/>
+      <c r="C52" s="167"/>
+      <c r="D52" s="167"/>
+      <c r="E52" s="167"/>
+      <c r="F52" s="167"/>
+      <c r="G52" s="167"/>
+      <c r="H52" s="167"/>
+      <c r="I52" s="167"/>
+      <c r="J52" s="168"/>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="57"/>
-      <c r="B53" s="58"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="58"/>
-      <c r="J53" s="59"/>
+      <c r="A53" s="166"/>
+      <c r="B53" s="167"/>
+      <c r="C53" s="167"/>
+      <c r="D53" s="167"/>
+      <c r="E53" s="167"/>
+      <c r="F53" s="167"/>
+      <c r="G53" s="167"/>
+      <c r="H53" s="167"/>
+      <c r="I53" s="167"/>
+      <c r="J53" s="168"/>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="57"/>
-      <c r="B54" s="58"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
-      <c r="J54" s="59"/>
+      <c r="A54" s="166"/>
+      <c r="B54" s="167"/>
+      <c r="C54" s="167"/>
+      <c r="D54" s="167"/>
+      <c r="E54" s="167"/>
+      <c r="F54" s="167"/>
+      <c r="G54" s="167"/>
+      <c r="H54" s="167"/>
+      <c r="I54" s="167"/>
+      <c r="J54" s="168"/>
     </row>
     <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="60" t="s">
-        <v>66</v>
+      <c r="A55" s="169"/>
+      <c r="B55" s="169"/>
+      <c r="C55" s="169"/>
+      <c r="D55" s="169"/>
+      <c r="E55" s="169"/>
+      <c r="F55" s="169"/>
+      <c r="G55" s="169"/>
+      <c r="H55" s="169"/>
+      <c r="I55" s="169"/>
+      <c r="J55" s="169"/>
+    </row>
+    <row r="56" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="170" t="s">
+        <v>27</v>
       </c>
-      <c r="B55" s="60"/>
-      <c r="C55" s="60"/>
-      <c r="D55" s="60"/>
-      <c r="E55" s="60"/>
-      <c r="F55" s="60"/>
-      <c r="G55" s="60"/>
-      <c r="H55" s="60"/>
-      <c r="I55" s="60"/>
-      <c r="J55" s="60"/>
-    </row>
-    <row r="56" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="B56" s="62"/>
-      <c r="C56" s="62"/>
-      <c r="D56" s="62"/>
-      <c r="E56" s="62"/>
-      <c r="F56" s="62"/>
-      <c r="G56" s="62"/>
-      <c r="H56" s="62"/>
-      <c r="I56" s="62"/>
-      <c r="J56" s="63"/>
+      <c r="B56" s="171"/>
+      <c r="C56" s="171"/>
+      <c r="D56" s="171"/>
+      <c r="E56" s="171"/>
+      <c r="F56" s="171"/>
+      <c r="G56" s="171"/>
+      <c r="H56" s="171"/>
+      <c r="I56" s="171"/>
+      <c r="J56" s="172"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="18"/>
@@ -9037,7 +8737,7 @@
     <row r="63" spans="1:10" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A63" s="18"/>
       <c r="B63" s="43" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
@@ -9045,28 +8745,24 @@
       <c r="F63" s="19"/>
       <c r="G63" s="44"/>
       <c r="H63" s="50" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="I63" s="19"/>
       <c r="J63" s="20"/>
     </row>
     <row r="64" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="47"/>
-      <c r="B64" s="48" t="s">
-        <v>11</v>
-      </c>
+      <c r="B64" s="48"/>
       <c r="C64" s="49" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="D64" s="42"/>
       <c r="E64" s="21" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="F64" s="19"/>
       <c r="G64" s="45"/>
-      <c r="H64" s="48" t="s">
-        <v>11</v>
-      </c>
+      <c r="H64" s="48"/>
       <c r="I64" s="51"/>
       <c r="J64" s="20"/>
     </row>
@@ -9074,15 +8770,15 @@
       <c r="A65" s="18"/>
       <c r="B65" s="46"/>
       <c r="C65" s="22" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="D65" s="42"/>
       <c r="E65" s="21" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="F65" s="19"/>
       <c r="G65" s="23" t="s">
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="H65" s="46"/>
       <c r="I65" s="19"/>
@@ -9092,15 +8788,15 @@
       <c r="A66" s="18"/>
       <c r="B66" s="19"/>
       <c r="C66" s="22" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D66" s="43"/>
       <c r="E66" s="21" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="F66" s="19"/>
       <c r="G66" s="23" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="H66" s="19"/>
       <c r="I66" s="19"/>
@@ -9118,542 +8814,618 @@
       <c r="I67" s="19"/>
       <c r="J67" s="20"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="73" t="s">
+    <row r="68" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="182" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="183"/>
+      <c r="C68" s="183"/>
+      <c r="D68" s="183"/>
+      <c r="E68" s="183"/>
+      <c r="F68" s="183"/>
+      <c r="G68" s="183"/>
+      <c r="H68" s="183"/>
+      <c r="I68" s="183"/>
+      <c r="J68" s="184"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="173"/>
+      <c r="B69" s="174"/>
+      <c r="C69" s="174"/>
+      <c r="D69" s="174"/>
+      <c r="E69" s="174"/>
+      <c r="F69" s="174"/>
+      <c r="G69" s="174"/>
+      <c r="H69" s="174"/>
+      <c r="I69" s="174"/>
+      <c r="J69" s="175"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="176"/>
+      <c r="B70" s="177"/>
+      <c r="C70" s="177"/>
+      <c r="D70" s="177"/>
+      <c r="E70" s="177"/>
+      <c r="F70" s="177"/>
+      <c r="G70" s="177"/>
+      <c r="H70" s="177"/>
+      <c r="I70" s="177"/>
+      <c r="J70" s="178"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="176"/>
+      <c r="B71" s="177"/>
+      <c r="C71" s="177"/>
+      <c r="D71" s="177"/>
+      <c r="E71" s="177"/>
+      <c r="F71" s="177"/>
+      <c r="G71" s="177"/>
+      <c r="H71" s="177"/>
+      <c r="I71" s="177"/>
+      <c r="J71" s="178"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="176"/>
+      <c r="B72" s="177"/>
+      <c r="C72" s="177"/>
+      <c r="D72" s="177"/>
+      <c r="E72" s="177"/>
+      <c r="F72" s="177"/>
+      <c r="G72" s="177"/>
+      <c r="H72" s="177"/>
+      <c r="I72" s="177"/>
+      <c r="J72" s="178"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="176"/>
+      <c r="B73" s="177"/>
+      <c r="C73" s="177"/>
+      <c r="D73" s="177"/>
+      <c r="E73" s="177"/>
+      <c r="F73" s="177"/>
+      <c r="G73" s="177"/>
+      <c r="H73" s="177"/>
+      <c r="I73" s="177"/>
+      <c r="J73" s="178"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="176"/>
+      <c r="B74" s="177"/>
+      <c r="C74" s="177"/>
+      <c r="D74" s="177"/>
+      <c r="E74" s="177"/>
+      <c r="F74" s="177"/>
+      <c r="G74" s="177"/>
+      <c r="H74" s="177"/>
+      <c r="I74" s="177"/>
+      <c r="J74" s="178"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="176"/>
+      <c r="B75" s="177"/>
+      <c r="C75" s="177"/>
+      <c r="D75" s="177"/>
+      <c r="E75" s="177"/>
+      <c r="F75" s="177"/>
+      <c r="G75" s="177"/>
+      <c r="H75" s="177"/>
+      <c r="I75" s="177"/>
+      <c r="J75" s="178"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="176"/>
+      <c r="B76" s="177"/>
+      <c r="C76" s="177"/>
+      <c r="D76" s="177"/>
+      <c r="E76" s="177"/>
+      <c r="F76" s="177"/>
+      <c r="G76" s="177"/>
+      <c r="H76" s="177"/>
+      <c r="I76" s="177"/>
+      <c r="J76" s="178"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="176"/>
+      <c r="B77" s="177"/>
+      <c r="C77" s="177"/>
+      <c r="D77" s="177"/>
+      <c r="E77" s="177"/>
+      <c r="F77" s="177"/>
+      <c r="G77" s="177"/>
+      <c r="H77" s="177"/>
+      <c r="I77" s="177"/>
+      <c r="J77" s="178"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="176"/>
+      <c r="B78" s="177"/>
+      <c r="C78" s="177"/>
+      <c r="D78" s="177"/>
+      <c r="E78" s="177"/>
+      <c r="F78" s="177"/>
+      <c r="G78" s="177"/>
+      <c r="H78" s="177"/>
+      <c r="I78" s="177"/>
+      <c r="J78" s="178"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="176"/>
+      <c r="B79" s="177"/>
+      <c r="C79" s="177"/>
+      <c r="D79" s="177"/>
+      <c r="E79" s="177"/>
+      <c r="F79" s="177"/>
+      <c r="G79" s="177"/>
+      <c r="H79" s="177"/>
+      <c r="I79" s="177"/>
+      <c r="J79" s="178"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="176"/>
+      <c r="B80" s="177"/>
+      <c r="C80" s="177"/>
+      <c r="D80" s="177"/>
+      <c r="E80" s="177"/>
+      <c r="F80" s="177"/>
+      <c r="G80" s="177"/>
+      <c r="H80" s="177"/>
+      <c r="I80" s="177"/>
+      <c r="J80" s="178"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="176"/>
+      <c r="B81" s="177"/>
+      <c r="C81" s="177"/>
+      <c r="D81" s="177"/>
+      <c r="E81" s="177"/>
+      <c r="F81" s="177"/>
+      <c r="G81" s="177"/>
+      <c r="H81" s="177"/>
+      <c r="I81" s="177"/>
+      <c r="J81" s="178"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="176"/>
+      <c r="B82" s="177"/>
+      <c r="C82" s="177"/>
+      <c r="D82" s="177"/>
+      <c r="E82" s="177"/>
+      <c r="F82" s="177"/>
+      <c r="G82" s="177"/>
+      <c r="H82" s="177"/>
+      <c r="I82" s="177"/>
+      <c r="J82" s="178"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="176"/>
+      <c r="B83" s="177"/>
+      <c r="C83" s="177"/>
+      <c r="D83" s="177"/>
+      <c r="E83" s="177"/>
+      <c r="F83" s="177"/>
+      <c r="G83" s="177"/>
+      <c r="H83" s="177"/>
+      <c r="I83" s="177"/>
+      <c r="J83" s="178"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="176"/>
+      <c r="B84" s="177"/>
+      <c r="C84" s="177"/>
+      <c r="D84" s="177"/>
+      <c r="E84" s="177"/>
+      <c r="F84" s="177"/>
+      <c r="G84" s="177"/>
+      <c r="H84" s="177"/>
+      <c r="I84" s="177"/>
+      <c r="J84" s="178"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="176"/>
+      <c r="B85" s="177"/>
+      <c r="C85" s="177"/>
+      <c r="D85" s="177"/>
+      <c r="E85" s="177"/>
+      <c r="F85" s="177"/>
+      <c r="G85" s="177"/>
+      <c r="H85" s="177"/>
+      <c r="I85" s="177"/>
+      <c r="J85" s="178"/>
+    </row>
+    <row r="86" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="179"/>
+      <c r="B86" s="180"/>
+      <c r="C86" s="180"/>
+      <c r="D86" s="180"/>
+      <c r="E86" s="180"/>
+      <c r="F86" s="180"/>
+      <c r="G86" s="180"/>
+      <c r="H86" s="180"/>
+      <c r="I86" s="180"/>
+      <c r="J86" s="181"/>
+    </row>
+    <row r="87" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="185" t="s">
+        <v>35</v>
+      </c>
+      <c r="B87" s="186"/>
+      <c r="C87" s="186"/>
+      <c r="D87" s="186"/>
+      <c r="E87" s="186"/>
+      <c r="F87" s="187"/>
+      <c r="G87" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="H87" s="185" t="s">
+        <v>33</v>
+      </c>
+      <c r="I87" s="187"/>
+      <c r="J87" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B88" s="188"/>
+      <c r="C88" s="188"/>
+      <c r="D88" s="188"/>
+      <c r="E88" s="188"/>
+      <c r="F88" s="189"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="68"/>
+      <c r="I88" s="69"/>
+      <c r="J88" s="10"/>
+    </row>
+    <row r="89" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B89" s="149"/>
+      <c r="C89" s="149"/>
+      <c r="D89" s="149"/>
+      <c r="E89" s="149"/>
+      <c r="F89" s="150"/>
+      <c r="G89" s="12"/>
+      <c r="H89" s="68"/>
+      <c r="I89" s="69"/>
+      <c r="J89" s="10"/>
+    </row>
+    <row r="90" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B90" s="149"/>
+      <c r="C90" s="149"/>
+      <c r="D90" s="149"/>
+      <c r="E90" s="149"/>
+      <c r="F90" s="150"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="68"/>
+      <c r="I90" s="69"/>
+      <c r="J90" s="10"/>
+    </row>
+    <row r="91" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B91" s="64"/>
+      <c r="C91" s="64"/>
+      <c r="D91" s="64"/>
+      <c r="E91" s="64"/>
+      <c r="F91" s="65"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="66"/>
+      <c r="I91" s="67"/>
+      <c r="J91" s="7"/>
+    </row>
+    <row r="92" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B92" s="64"/>
+      <c r="C92" s="64"/>
+      <c r="D92" s="64"/>
+      <c r="E92" s="64"/>
+      <c r="F92" s="65"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="66"/>
+      <c r="I92" s="67"/>
+      <c r="J92" s="7"/>
+    </row>
+    <row r="93" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B93" s="64"/>
+      <c r="C93" s="64"/>
+      <c r="D93" s="64"/>
+      <c r="E93" s="64"/>
+      <c r="F93" s="65"/>
+      <c r="G93" s="12"/>
+      <c r="H93" s="66"/>
+      <c r="I93" s="67"/>
+      <c r="J93" s="7"/>
+    </row>
+    <row r="94" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B94" s="64"/>
+      <c r="C94" s="64"/>
+      <c r="D94" s="64"/>
+      <c r="E94" s="64"/>
+      <c r="F94" s="65"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="66"/>
+      <c r="I94" s="67"/>
+      <c r="J94" s="7"/>
+    </row>
+    <row r="95" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B95" s="64"/>
+      <c r="C95" s="64"/>
+      <c r="D95" s="64"/>
+      <c r="E95" s="64"/>
+      <c r="F95" s="65"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="66"/>
+      <c r="I95" s="67"/>
+      <c r="J95" s="7"/>
+    </row>
+    <row r="96" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B96" s="64"/>
+      <c r="C96" s="64"/>
+      <c r="D96" s="64"/>
+      <c r="E96" s="64"/>
+      <c r="F96" s="65"/>
+      <c r="G96" s="12"/>
+      <c r="H96" s="66"/>
+      <c r="I96" s="67"/>
+      <c r="J96" s="7"/>
+    </row>
+    <row r="97" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B97" s="64"/>
+      <c r="C97" s="64"/>
+      <c r="D97" s="64"/>
+      <c r="E97" s="64"/>
+      <c r="F97" s="65"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="66"/>
+      <c r="I97" s="67"/>
+      <c r="J97" s="7"/>
+    </row>
+    <row r="98" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B98" s="64"/>
+      <c r="C98" s="64"/>
+      <c r="D98" s="64"/>
+      <c r="E98" s="64"/>
+      <c r="F98" s="65"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="66"/>
+      <c r="I98" s="67"/>
+      <c r="J98" s="7"/>
+    </row>
+    <row r="99" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B99" s="64"/>
+      <c r="C99" s="64"/>
+      <c r="D99" s="64"/>
+      <c r="E99" s="64"/>
+      <c r="F99" s="65"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="66"/>
+      <c r="I99" s="67"/>
+      <c r="J99" s="7"/>
+    </row>
+    <row r="100" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B100" s="64"/>
+      <c r="C100" s="64"/>
+      <c r="D100" s="64"/>
+      <c r="E100" s="64"/>
+      <c r="F100" s="65"/>
+      <c r="G100" s="12"/>
+      <c r="H100" s="66"/>
+      <c r="I100" s="67"/>
+      <c r="J100" s="7"/>
+    </row>
+    <row r="101" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="155" t="s">
+        <v>85</v>
+      </c>
+      <c r="B101" s="156"/>
+      <c r="C101" s="156"/>
+      <c r="D101" s="156"/>
+      <c r="E101" s="156"/>
+      <c r="F101" s="156"/>
+      <c r="G101" s="156"/>
+      <c r="H101" s="156"/>
+      <c r="I101" s="156"/>
+      <c r="J101" s="157"/>
+    </row>
+    <row r="102" spans="1:10" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="85" t="s">
+        <v>75</v>
+      </c>
+      <c r="B102" s="158"/>
+      <c r="C102" s="158"/>
+      <c r="D102" s="158"/>
+      <c r="E102" s="159"/>
+      <c r="F102" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="G102" s="158"/>
+      <c r="H102" s="158"/>
+      <c r="I102" s="158"/>
+      <c r="J102" s="159"/>
+    </row>
+    <row r="103" spans="1:10" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="160"/>
+      <c r="B103" s="161"/>
+      <c r="C103" s="161"/>
+      <c r="D103" s="161"/>
+      <c r="E103" s="162"/>
+      <c r="F103" s="161"/>
+      <c r="G103" s="161"/>
+      <c r="H103" s="161"/>
+      <c r="I103" s="161"/>
+      <c r="J103" s="162"/>
+    </row>
+    <row r="104" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="151" t="s">
+        <v>79</v>
+      </c>
+      <c r="B104" s="152"/>
+      <c r="C104" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="D104" s="153" t="s">
+        <v>80</v>
+      </c>
+      <c r="E104" s="152"/>
+      <c r="F104" s="152"/>
+      <c r="G104" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="H104" s="151" t="s">
         <v>78</v>
       </c>
-      <c r="B68" s="74"/>
-      <c r="C68" s="74"/>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
-      <c r="F68" s="74"/>
-      <c r="G68" s="74"/>
-      <c r="H68" s="74"/>
-      <c r="I68" s="74"/>
-      <c r="J68" s="75"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="64"/>
-      <c r="B69" s="65"/>
-      <c r="C69" s="65"/>
-      <c r="D69" s="65"/>
-      <c r="E69" s="65"/>
-      <c r="F69" s="65"/>
-      <c r="G69" s="65"/>
-      <c r="H69" s="65"/>
-      <c r="I69" s="65"/>
-      <c r="J69" s="66"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="67"/>
-      <c r="B70" s="68"/>
-      <c r="C70" s="68"/>
-      <c r="D70" s="68"/>
-      <c r="E70" s="68"/>
-      <c r="F70" s="68"/>
-      <c r="G70" s="68"/>
-      <c r="H70" s="68"/>
-      <c r="I70" s="68"/>
-      <c r="J70" s="69"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="67"/>
-      <c r="B71" s="68"/>
-      <c r="C71" s="68"/>
-      <c r="D71" s="68"/>
-      <c r="E71" s="68"/>
-      <c r="F71" s="68"/>
-      <c r="G71" s="68"/>
-      <c r="H71" s="68"/>
-      <c r="I71" s="68"/>
-      <c r="J71" s="69"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="67"/>
-      <c r="B72" s="68"/>
-      <c r="C72" s="68"/>
-      <c r="D72" s="68"/>
-      <c r="E72" s="68"/>
-      <c r="F72" s="68"/>
-      <c r="G72" s="68"/>
-      <c r="H72" s="68"/>
-      <c r="I72" s="68"/>
-      <c r="J72" s="69"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="67"/>
-      <c r="B73" s="68"/>
-      <c r="C73" s="68"/>
-      <c r="D73" s="68"/>
-      <c r="E73" s="68"/>
-      <c r="F73" s="68"/>
-      <c r="G73" s="68"/>
-      <c r="H73" s="68"/>
-      <c r="I73" s="68"/>
-      <c r="J73" s="69"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="67"/>
-      <c r="B74" s="68"/>
-      <c r="C74" s="68"/>
-      <c r="D74" s="68"/>
-      <c r="E74" s="68"/>
-      <c r="F74" s="68"/>
-      <c r="G74" s="68"/>
-      <c r="H74" s="68"/>
-      <c r="I74" s="68"/>
-      <c r="J74" s="69"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="67"/>
-      <c r="B75" s="68"/>
-      <c r="C75" s="68"/>
-      <c r="D75" s="68"/>
-      <c r="E75" s="68"/>
-      <c r="F75" s="68"/>
-      <c r="G75" s="68"/>
-      <c r="H75" s="68"/>
-      <c r="I75" s="68"/>
-      <c r="J75" s="69"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="67"/>
-      <c r="B76" s="68"/>
-      <c r="C76" s="68"/>
-      <c r="D76" s="68"/>
-      <c r="E76" s="68"/>
-      <c r="F76" s="68"/>
-      <c r="G76" s="68"/>
-      <c r="H76" s="68"/>
-      <c r="I76" s="68"/>
-      <c r="J76" s="69"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="67"/>
-      <c r="B77" s="68"/>
-      <c r="C77" s="68"/>
-      <c r="D77" s="68"/>
-      <c r="E77" s="68"/>
-      <c r="F77" s="68"/>
-      <c r="G77" s="68"/>
-      <c r="H77" s="68"/>
-      <c r="I77" s="68"/>
-      <c r="J77" s="69"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="67"/>
-      <c r="B78" s="68"/>
-      <c r="C78" s="68"/>
-      <c r="D78" s="68"/>
-      <c r="E78" s="68"/>
-      <c r="F78" s="68"/>
-      <c r="G78" s="68"/>
-      <c r="H78" s="68"/>
-      <c r="I78" s="68"/>
-      <c r="J78" s="69"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="67"/>
-      <c r="B79" s="68"/>
-      <c r="C79" s="68"/>
-      <c r="D79" s="68"/>
-      <c r="E79" s="68"/>
-      <c r="F79" s="68"/>
-      <c r="G79" s="68"/>
-      <c r="H79" s="68"/>
-      <c r="I79" s="68"/>
-      <c r="J79" s="69"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="67"/>
-      <c r="B80" s="68"/>
-      <c r="C80" s="68"/>
-      <c r="D80" s="68"/>
-      <c r="E80" s="68"/>
-      <c r="F80" s="68"/>
-      <c r="G80" s="68"/>
-      <c r="H80" s="68"/>
-      <c r="I80" s="68"/>
-      <c r="J80" s="69"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="67"/>
-      <c r="B81" s="68"/>
-      <c r="C81" s="68"/>
-      <c r="D81" s="68"/>
-      <c r="E81" s="68"/>
-      <c r="F81" s="68"/>
-      <c r="G81" s="68"/>
-      <c r="H81" s="68"/>
-      <c r="I81" s="68"/>
-      <c r="J81" s="69"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="67"/>
-      <c r="B82" s="68"/>
-      <c r="C82" s="68"/>
-      <c r="D82" s="68"/>
-      <c r="E82" s="68"/>
-      <c r="F82" s="68"/>
-      <c r="G82" s="68"/>
-      <c r="H82" s="68"/>
-      <c r="I82" s="68"/>
-      <c r="J82" s="69"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="67"/>
-      <c r="B83" s="68"/>
-      <c r="C83" s="68"/>
-      <c r="D83" s="68"/>
-      <c r="E83" s="68"/>
-      <c r="F83" s="68"/>
-      <c r="G83" s="68"/>
-      <c r="H83" s="68"/>
-      <c r="I83" s="68"/>
-      <c r="J83" s="69"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="67"/>
-      <c r="B84" s="68"/>
-      <c r="C84" s="68"/>
-      <c r="D84" s="68"/>
-      <c r="E84" s="68"/>
-      <c r="F84" s="68"/>
-      <c r="G84" s="68"/>
-      <c r="H84" s="68"/>
-      <c r="I84" s="68"/>
-      <c r="J84" s="69"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="67"/>
-      <c r="B85" s="68"/>
-      <c r="C85" s="68"/>
-      <c r="D85" s="68"/>
-      <c r="E85" s="68"/>
-      <c r="F85" s="68"/>
-      <c r="G85" s="68"/>
-      <c r="H85" s="68"/>
-      <c r="I85" s="68"/>
-      <c r="J85" s="69"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="70"/>
-      <c r="B86" s="71"/>
-      <c r="C86" s="71"/>
-      <c r="D86" s="71"/>
-      <c r="E86" s="71"/>
-      <c r="F86" s="71"/>
-      <c r="G86" s="71"/>
-      <c r="H86" s="71"/>
-      <c r="I86" s="71"/>
-      <c r="J86" s="72"/>
-    </row>
-    <row r="87" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="76" t="s">
-        <v>79</v>
+      <c r="I104" s="154"/>
+      <c r="J104" s="36" t="s">
+        <v>77</v>
       </c>
-      <c r="B87" s="77"/>
-      <c r="C87" s="77"/>
-      <c r="D87" s="77"/>
-      <c r="E87" s="77"/>
-      <c r="F87" s="78"/>
-      <c r="G87" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="H87" s="76" t="s">
-        <v>81</v>
-      </c>
-      <c r="I87" s="78"/>
-      <c r="J87" s="24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="B88" s="79" t="s">
-        <v>84</v>
-      </c>
-      <c r="C88" s="79"/>
-      <c r="D88" s="79"/>
-      <c r="E88" s="79"/>
-      <c r="F88" s="80"/>
-      <c r="G88" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="H88" s="85" t="s">
-        <v>86</v>
-      </c>
-      <c r="I88" s="86"/>
-      <c r="J88" s="10">
-        <v>43544</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A89" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="B89" s="81"/>
-      <c r="C89" s="81"/>
-      <c r="D89" s="81"/>
-      <c r="E89" s="81"/>
-      <c r="F89" s="82"/>
-      <c r="G89" s="12"/>
-      <c r="H89" s="85"/>
-      <c r="I89" s="86"/>
-      <c r="J89" s="10"/>
-    </row>
-    <row r="90" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="B90" s="81"/>
-      <c r="C90" s="81"/>
-      <c r="D90" s="81"/>
-      <c r="E90" s="81"/>
-      <c r="F90" s="82"/>
-      <c r="G90" s="12"/>
-      <c r="H90" s="85"/>
-      <c r="I90" s="86"/>
-      <c r="J90" s="10"/>
-    </row>
-    <row r="91" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B91" s="83"/>
-      <c r="C91" s="83"/>
-      <c r="D91" s="83"/>
-      <c r="E91" s="83"/>
-      <c r="F91" s="84"/>
-      <c r="G91" s="12"/>
-      <c r="H91" s="87"/>
-      <c r="I91" s="88"/>
-      <c r="J91" s="7"/>
-    </row>
-    <row r="92" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="B92" s="83"/>
-      <c r="C92" s="83"/>
-      <c r="D92" s="83"/>
-      <c r="E92" s="83"/>
-      <c r="F92" s="84"/>
-      <c r="G92" s="12"/>
-      <c r="H92" s="87"/>
-      <c r="I92" s="88"/>
-      <c r="J92" s="7"/>
-    </row>
-    <row r="93" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="B93" s="83"/>
-      <c r="C93" s="83"/>
-      <c r="D93" s="83"/>
-      <c r="E93" s="83"/>
-      <c r="F93" s="84"/>
-      <c r="G93" s="12"/>
-      <c r="H93" s="87"/>
-      <c r="I93" s="88"/>
-      <c r="J93" s="7"/>
-    </row>
-    <row r="94" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A94" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="B94" s="83"/>
-      <c r="C94" s="83"/>
-      <c r="D94" s="83"/>
-      <c r="E94" s="83"/>
-      <c r="F94" s="84"/>
-      <c r="G94" s="12"/>
-      <c r="H94" s="87"/>
-      <c r="I94" s="88"/>
-      <c r="J94" s="7"/>
-    </row>
-    <row r="95" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A95" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="B95" s="83"/>
-      <c r="C95" s="83"/>
-      <c r="D95" s="83"/>
-      <c r="E95" s="83"/>
-      <c r="F95" s="84"/>
-      <c r="G95" s="12"/>
-      <c r="H95" s="87"/>
-      <c r="I95" s="88"/>
-      <c r="J95" s="7"/>
-    </row>
-    <row r="96" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A96" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="B96" s="83"/>
-      <c r="C96" s="83"/>
-      <c r="D96" s="83"/>
-      <c r="E96" s="83"/>
-      <c r="F96" s="84"/>
-      <c r="G96" s="12"/>
-      <c r="H96" s="87"/>
-      <c r="I96" s="88"/>
-      <c r="J96" s="7"/>
-    </row>
-    <row r="97" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A97" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="B97" s="83"/>
-      <c r="C97" s="83"/>
-      <c r="D97" s="83"/>
-      <c r="E97" s="83"/>
-      <c r="F97" s="84"/>
-      <c r="G97" s="12"/>
-      <c r="H97" s="87"/>
-      <c r="I97" s="88"/>
-      <c r="J97" s="7"/>
-    </row>
-    <row r="98" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A98" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="B98" s="83"/>
-      <c r="C98" s="83"/>
-      <c r="D98" s="83"/>
-      <c r="E98" s="83"/>
-      <c r="F98" s="84"/>
-      <c r="G98" s="12"/>
-      <c r="H98" s="87"/>
-      <c r="I98" s="88"/>
-      <c r="J98" s="7"/>
-    </row>
-    <row r="99" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A99" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="B99" s="83"/>
-      <c r="C99" s="83"/>
-      <c r="D99" s="83"/>
-      <c r="E99" s="83"/>
-      <c r="F99" s="84"/>
-      <c r="G99" s="12"/>
-      <c r="H99" s="87"/>
-      <c r="I99" s="88"/>
-      <c r="J99" s="7"/>
-    </row>
-    <row r="100" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A100" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="B100" s="83"/>
-      <c r="C100" s="83"/>
-      <c r="D100" s="83"/>
-      <c r="E100" s="83"/>
-      <c r="F100" s="84"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="87"/>
-      <c r="I100" s="88"/>
-      <c r="J100" s="7"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="93" t="s">
-        <v>99</v>
-      </c>
-      <c r="B101" s="94"/>
-      <c r="C101" s="94"/>
-      <c r="D101" s="94"/>
-      <c r="E101" s="94"/>
-      <c r="F101" s="94"/>
-      <c r="G101" s="94"/>
-      <c r="H101" s="94"/>
-      <c r="I101" s="94"/>
-      <c r="J101" s="95"/>
-    </row>
-    <row r="102" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="96" t="s">
-        <v>100</v>
-      </c>
-      <c r="B102" s="97"/>
-      <c r="C102" s="97"/>
-      <c r="D102" s="97"/>
-      <c r="E102" s="98"/>
-      <c r="F102" s="96" t="s">
-        <v>101</v>
-      </c>
-      <c r="G102" s="97"/>
-      <c r="H102" s="97"/>
-      <c r="I102" s="97"/>
-      <c r="J102" s="98"/>
-    </row>
-    <row r="103" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="99" t="s">
-        <v>102</v>
-      </c>
-      <c r="B103" s="100"/>
-      <c r="C103" s="100"/>
-      <c r="D103" s="100"/>
-      <c r="E103" s="101"/>
-      <c r="F103" s="100" t="s">
-        <v>103</v>
-      </c>
-      <c r="G103" s="100"/>
-      <c r="H103" s="100"/>
-      <c r="I103" s="100"/>
-      <c r="J103" s="101"/>
-    </row>
-    <row r="104" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="89" t="s">
-        <v>104</v>
-      </c>
-      <c r="B104" s="90"/>
-      <c r="C104" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="D104" s="91" t="s">
-        <v>105</v>
-      </c>
-      <c r="E104" s="90"/>
-      <c r="F104" s="90"/>
-      <c r="G104" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="H104" s="89" t="s">
-        <v>106</v>
-      </c>
-      <c r="I104" s="92"/>
-      <c r="J104" s="36" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="176" t="s">
-        <v>108</v>
-      </c>
-      <c r="B105" s="177"/>
-      <c r="C105" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="D105" s="178" t="s">
-        <v>109</v>
-      </c>
-      <c r="E105" s="179"/>
-      <c r="F105" s="180"/>
-      <c r="G105" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="H105" s="178" t="s">
-        <v>110</v>
-      </c>
-      <c r="I105" s="180"/>
-      <c r="J105" s="52" t="s">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="105" spans="1:10" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="57"/>
+      <c r="B105" s="58"/>
+      <c r="C105" s="52"/>
+      <c r="D105" s="59"/>
+      <c r="E105" s="60"/>
+      <c r="F105" s="61"/>
+      <c r="G105" s="53"/>
+      <c r="H105" s="59"/>
+      <c r="I105" s="61"/>
+      <c r="J105" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="123">
+    <mergeCell ref="A42:J54"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="F55:J55"/>
+    <mergeCell ref="A56:J56"/>
+    <mergeCell ref="A69:J86"/>
+    <mergeCell ref="A68:J68"/>
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="H87:I87"/>
+    <mergeCell ref="B88:F88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B91:F91"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="B94:F94"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="A101:J101"/>
+    <mergeCell ref="A102:E102"/>
+    <mergeCell ref="F102:J102"/>
+    <mergeCell ref="A103:E103"/>
+    <mergeCell ref="F103:J103"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B92:F92"/>
+    <mergeCell ref="H93:I93"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="F13:J13"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C16:E19"/>
+    <mergeCell ref="A8:E15"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:J5"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C28:J28"/>
+    <mergeCell ref="C29:J29"/>
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A16:B19"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="F8:J11"/>
+    <mergeCell ref="A20:J20"/>
     <mergeCell ref="A105:B105"/>
     <mergeCell ref="D105:F105"/>
     <mergeCell ref="H105:I105"/>
@@ -9670,119 +9442,19 @@
     <mergeCell ref="H97:I97"/>
     <mergeCell ref="B95:F95"/>
     <mergeCell ref="H98:I98"/>
-    <mergeCell ref="C33:J33"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A16:B19"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="F8:J11"/>
-    <mergeCell ref="A20:J20"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="C28:J28"/>
-    <mergeCell ref="C29:J29"/>
-    <mergeCell ref="C30:J30"/>
-    <mergeCell ref="C31:J31"/>
-    <mergeCell ref="C32:J32"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:J5"/>
-    <mergeCell ref="A8:E15"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C16:E19"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="H94:I94"/>
+    <mergeCell ref="B96:F96"/>
+    <mergeCell ref="H88:I88"/>
     <mergeCell ref="A35:J35"/>
     <mergeCell ref="A36:J36"/>
+    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A34:J34"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B92:F92"/>
-    <mergeCell ref="H93:I93"/>
-    <mergeCell ref="H95:I95"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="H94:I94"/>
-    <mergeCell ref="H88:I88"/>
-    <mergeCell ref="B94:F94"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="D104:F104"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="H100:I100"/>
-    <mergeCell ref="A101:J101"/>
-    <mergeCell ref="A102:E102"/>
-    <mergeCell ref="F102:J102"/>
-    <mergeCell ref="A103:E103"/>
-    <mergeCell ref="F103:J103"/>
-    <mergeCell ref="B96:F96"/>
-    <mergeCell ref="B91:F91"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="H91:I91"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="A87:F87"/>
-    <mergeCell ref="H87:I87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="A42:J54"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="F55:J55"/>
-    <mergeCell ref="A56:J56"/>
-    <mergeCell ref="A69:J86"/>
-    <mergeCell ref="A68:J68"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="63" fitToHeight="6" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="41" max="1048575" man="1"/>
+    <brk id="41" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
@@ -9972,6 +9644,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <Please_x0020_note xmlns="f17bae92-5fa7-4270-afeb-ed962faafa52" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B342DF5A2DEFD64586E21F8B44CF3641" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="97e464cb99569ca8a9ef17fb08900847">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns3="f17bae92-5fa7-4270-afeb-ed962faafa52" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6356073c4c24c81483cf02fe07ae928c" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -10110,39 +9800,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <Please_x0020_note xmlns="f17bae92-5fa7-4270-afeb-ed962faafa52" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544619E3-E001-4BD0-A0E9-1E9FD84B48E5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A06E1120-8501-409E-8BA8-1494F83C4851}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="f17bae92-5fa7-4270-afeb-ed962faafa52"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10165,9 +9826,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A06E1120-8501-409E-8BA8-1494F83C4851}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544619E3-E001-4BD0-A0E9-1E9FD84B48E5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="f17bae92-5fa7-4270-afeb-ed962faafa52"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Agregado de circulo que encierra el factor de la falla en el excel
</commit_message>
<xml_diff>
--- a/DigiTools/Content/formats/FORMATO_EWO.XLSX
+++ b/DigiTools/Content/formats/FORMATO_EWO.XLSX
@@ -6798,6 +6798,64 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>209876</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219168</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>94990</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="ff"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1"/>
+          <a:ext cx="2076450" cy="1557338"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="4F81BD">
+            <a:alpha val="30000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>

</xml_diff>